<commit_message>
Generated the latest version of summary tables:
  Extraction summary - Supp Table S4
  CPU time - Supp Table S5
</commit_message>
<xml_diff>
--- a/documents/CPU_timing/mSigHdp-paper-tracking.xlsx
+++ b/documents/CPU_timing/mSigHdp-paper-tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\documents\CPU_timing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D548CD6-CFB6-4C5C-AC3F-61D7F70E4F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87EF474A-4D44-42EF-8F3E-123B5060B6BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="1245" windowWidth="18015" windowHeight="12855" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -51,7 +51,7 @@
     <author>tc={951A56E7-234C-4F7A-A36A-03F37A929761}</author>
   </authors>
   <commentList>
-    <comment ref="H15" authorId="0" shapeId="0" xr:uid="{E68ABE94-AAC2-428A-BBD6-EBC4EF1F710E}">
+    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{E68ABE94-AAC2-428A-BBD6-EBC4EF1F710E}">
       <text>
         <t>[线程批注]
 你的Excel版本可读取此线程批注; 但如果在更新版本的Excel中打开文件，则对批注所作的任何改动都将被删除。了解详细信息: https://go.microsoft.com/fwlink/?linkid=870924
@@ -61,7 +61,7 @@
 Now re-running on hpc-super queue.</t>
       </text>
     </comment>
-    <comment ref="H16" authorId="1" shapeId="0" xr:uid="{05356E87-CF50-43B3-B006-266C95804CB2}">
+    <comment ref="H18" authorId="1" shapeId="0" xr:uid="{05356E87-CF50-43B3-B006-266C95804CB2}">
       <text>
         <t>[线程批注]
 你的Excel版本可读取此线程批注; 但如果在更新版本的Excel中打开文件，则对批注所作的任何改动都将被删除。了解详细信息: https://go.microsoft.com/fwlink/?linkid=870924
@@ -71,7 +71,7 @@
 Now re-running on hpc-super queue.</t>
       </text>
     </comment>
-    <comment ref="H17" authorId="2" shapeId="0" xr:uid="{951A56E7-234C-4F7A-A36A-03F37A929761}">
+    <comment ref="H19" authorId="2" shapeId="0" xr:uid="{951A56E7-234C-4F7A-A36A-03F37A929761}">
       <text>
         <t>[线程批注]
 你的Excel版本可读取此线程批注; 但如果在更新版本的Excel中打开文件，则对批注所作的任何改动都将被删除。了解详细信息: https://go.microsoft.com/fwlink/?linkid=870924
@@ -177,7 +177,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="200">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -1235,12 +1235,35 @@
 &lt;135856&gt;
 (wuyang)</t>
   </si>
+  <si>
+    <t>SP_default</t>
+  </si>
+  <si>
+    <t>m2
+&lt;1686242&gt;
+(e0240162)</t>
+  </si>
+  <si>
+    <t>m2
+&lt;&gt;
+(e0240162)</t>
+  </si>
+  <si>
+    <t>m2
+&lt;1811473&gt;
+(e0240162)</t>
+  </si>
+  <si>
+    <t>m2
+&lt;1811857&gt;
+(e0240162)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1321,12 +1344,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1392,7 +1409,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1505,6 +1522,12 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1557,9 +1580,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1855,17 +1875,17 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="H15" dT="2022-08-28T11:28:19.37" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{E68ABE94-AAC2-428A-BBD6-EBC4EF1F710E}">
+  <threadedComment ref="H17" dT="2022-08-28T11:28:19.37" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{E68ABE94-AAC2-428A-BBD6-EBC4EF1F710E}">
     <text>Failed when using queue hpc-long
 I assume that hpc-long can only allocate 100GB to each job, and this causes the error.
 Now re-running on hpc-super queue.</text>
   </threadedComment>
-  <threadedComment ref="H16" dT="2022-08-28T11:28:19.37" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{05356E87-CF50-43B3-B006-266C95804CB2}">
+  <threadedComment ref="H18" dT="2022-08-28T11:28:19.37" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{05356E87-CF50-43B3-B006-266C95804CB2}">
     <text>Failed when using queue hpc-long
 I assume that hpc-long can only allocate 100GB to each job, and this causes the error.
 Now re-running on hpc-super queue.</text>
   </threadedComment>
-  <threadedComment ref="H17" dT="2022-08-28T11:28:19.37" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{951A56E7-234C-4F7A-A36A-03F37A929761}">
+  <threadedComment ref="H19" dT="2022-08-28T11:28:19.37" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{951A56E7-234C-4F7A-A36A-03F37A929761}">
     <text>Failed when using queue hpc-long
 I assume that hpc-long can only allocate 100GB to each job, and this causes the error.
 Now re-running on hpc-super queue.</text>
@@ -2053,10 +2073,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
@@ -2098,40 +2118,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="50.1" customHeight="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="M1" s="45" t="s">
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="M1" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="F2" s="9">
         <v>5</v>
       </c>
@@ -2170,13 +2190,13 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="68.25" customHeight="1">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="40" t="s">
         <v>71</v>
       </c>
       <c r="D3" s="10">
@@ -2198,121 +2218,121 @@
       <c r="J3" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="K3" s="42" t="s">
+      <c r="K3" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="M3" s="42" t="s">
+      <c r="M3" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="N3" s="42" t="s">
+      <c r="N3" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="O3" s="42" t="s">
+      <c r="O3" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="P3" s="42" t="s">
+      <c r="P3" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="Q3" s="42" t="s">
+      <c r="Q3" s="44" t="s">
         <v>127</v>
       </c>
-      <c r="R3" s="42" t="s">
+      <c r="R3" s="44" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="75" customHeight="1">
-      <c r="A4" s="41"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="38"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="10">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="H4" s="42" t="s">
+      <c r="H4" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="I4" s="42" t="s">
+      <c r="I4" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="J4" s="42" t="s">
+      <c r="J4" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="K4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="42"/>
+      <c r="K4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
     </row>
     <row r="5" spans="1:18" ht="36" customHeight="1">
-      <c r="A5" s="41"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="38"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="10">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="42"/>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="42"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="44"/>
     </row>
     <row r="6" spans="1:18" ht="36" customHeight="1">
-      <c r="A6" s="41"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="38"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="10">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="44"/>
     </row>
     <row r="7" spans="1:18" ht="36" customHeight="1">
-      <c r="A7" s="41"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="38"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="10">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="42"/>
-      <c r="O7" s="42"/>
-      <c r="P7" s="42"/>
-      <c r="Q7" s="42"/>
-      <c r="R7" s="42"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="44"/>
+      <c r="R7" s="44"/>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="2"/>
@@ -2323,139 +2343,139 @@
       <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:18" ht="54" customHeight="1">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="51" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="10">
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="G9" s="42" t="s">
+      <c r="G9" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="H9" s="42" t="s">
+      <c r="H9" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="I9" s="42" t="s">
+      <c r="I9" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="J9" s="42" t="s">
+      <c r="J9" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="42" t="s">
+      <c r="K9" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="M9" s="42" t="s">
+      <c r="M9" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="N9" s="42" t="s">
+      <c r="N9" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="O9" s="42" t="s">
+      <c r="O9" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="P9" s="42" t="s">
+      <c r="P9" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="Q9" s="42" t="s">
+      <c r="Q9" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="R9" s="42" t="s">
+      <c r="R9" s="44" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="54" customHeight="1">
-      <c r="A10" s="41"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="49"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
       <c r="D10" s="10">
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="42"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="44"/>
     </row>
     <row r="11" spans="1:18" ht="54" customHeight="1">
-      <c r="A11" s="41"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="49"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
       <c r="D11" s="10">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="42"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="44"/>
     </row>
     <row r="12" spans="1:18" ht="54" customHeight="1">
-      <c r="A12" s="41"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="49"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="10">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="42"/>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="42"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+      <c r="M12" s="44"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="44"/>
+      <c r="Q12" s="44"/>
+      <c r="R12" s="44"/>
     </row>
     <row r="13" spans="1:18" ht="54" customHeight="1">
-      <c r="A13" s="41"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="49"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="10">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="42"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="44"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="44"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="5"/>
@@ -2468,14 +2488,14 @@
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:18" ht="94.5" customHeight="1">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
@@ -2538,10 +2558,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:H5"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2554,32 +2574,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:15" ht="45">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="F2" s="9" t="s">
         <v>38</v>
       </c>
@@ -2596,92 +2616,92 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="45" customHeight="1">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="40" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:15" ht="45" customHeight="1">
-      <c r="A4" s="41"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="38"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="45" customHeight="1">
-      <c r="A5" s="41"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="38"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="42" t="s">
+      <c r="F5" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="45" customHeight="1">
-      <c r="A6" s="41"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="38"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="42" t="s">
+      <c r="F6" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:15" ht="45" customHeight="1">
-      <c r="A7" s="41"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="38"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="42" t="s">
+      <c r="F7" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
       <c r="K7" s="2"/>
@@ -2713,54 +2733,43 @@
         <v>34</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
       <c r="J9" s="4"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="4"/>
       <c r="G10" s="5"/>
-      <c r="I10" s="2"/>
       <c r="J10" s="4"/>
       <c r="K10" s="5"/>
-      <c r="O10" s="34"/>
-    </row>
-    <row r="11" spans="1:15" ht="45">
-      <c r="A11" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>59</v>
-      </c>
+    </row>
+    <row r="11" spans="1:15" ht="90" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11" s="15"/>
       <c r="D11" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="I11" s="4"/>
+      <c r="F11" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="G11" s="5"/>
       <c r="J11" s="4"/>
       <c r="K11" s="5"/>
-      <c r="O11" s="34"/>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="10"/>
@@ -2768,264 +2777,305 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
       <c r="I12" s="2"/>
       <c r="J12" s="4"/>
       <c r="K12" s="5"/>
       <c r="O12" s="34"/>
     </row>
-    <row r="13" spans="1:15" ht="60" customHeight="1">
-      <c r="A13" s="41" t="s">
+    <row r="13" spans="1:15" ht="45">
+      <c r="A13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="5"/>
+      <c r="O13" s="34"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="5"/>
+      <c r="O14" s="34"/>
+    </row>
+    <row r="15" spans="1:15" ht="60" customHeight="1">
+      <c r="A15" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B15" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C15" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D15" s="2">
         <v>145879</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="42" t="s">
+      <c r="E15" s="5"/>
+      <c r="F15" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="O13" s="34"/>
-    </row>
-    <row r="14" spans="1:15" ht="60" customHeight="1">
-      <c r="A14" s="41"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="2">
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="O15" s="34"/>
+    </row>
+    <row r="16" spans="1:15" ht="60" customHeight="1">
+      <c r="A16" s="43"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="2">
         <v>200437</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="42" t="s">
+      <c r="E16" s="5"/>
+      <c r="F16" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="O14" s="34"/>
-    </row>
-    <row r="15" spans="1:15" ht="60" customHeight="1">
-      <c r="A15" s="41"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="2">
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="O16" s="34"/>
+    </row>
+    <row r="17" spans="1:15" ht="60" customHeight="1">
+      <c r="A17" s="43"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="2">
         <v>310111</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="42" t="s">
+      <c r="E17" s="5"/>
+      <c r="F17" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="O15" s="34"/>
-    </row>
-    <row r="16" spans="1:15" ht="60" customHeight="1">
-      <c r="A16" s="41"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="2">
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="O17" s="34"/>
+    </row>
+    <row r="18" spans="1:15" ht="60" customHeight="1">
+      <c r="A18" s="43"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="2">
         <v>528401</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="42" t="s">
+      <c r="E18" s="5"/>
+      <c r="F18" s="44" t="s">
         <v>163</v>
       </c>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="O16" s="34"/>
-    </row>
-    <row r="17" spans="1:15" ht="60" customHeight="1">
-      <c r="A17" s="41"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="2">
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="O18" s="34"/>
+    </row>
+    <row r="19" spans="1:15" ht="60" customHeight="1">
+      <c r="A19" s="43"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="2">
         <v>1076753</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="42" t="s">
+      <c r="E19" s="5"/>
+      <c r="F19" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="O17" s="34"/>
-    </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="1:15" ht="270" customHeight="1">
-      <c r="A19" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-    </row>
-    <row r="20" spans="1:15" ht="30" customHeight="1">
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="O19" s="34"/>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="10"/>
-      <c r="B20" s="40"/>
+      <c r="B20" s="10"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:15" ht="60" customHeight="1">
-      <c r="A21" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="2">
-        <v>145879</v>
+    <row r="21" spans="1:15" ht="270" customHeight="1">
+      <c r="A21" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
       <c r="H21" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="I21" s="42" t="s">
         <v>181</v>
       </c>
+      <c r="I21" s="2"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" spans="1:15" ht="60" customHeight="1">
-      <c r="A22" s="41"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="2">
-        <v>200437</v>
-      </c>
+    <row r="22" spans="1:15" ht="30" customHeight="1">
+      <c r="A22" s="10"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="H22" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="I22" s="42"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:15" ht="60" customHeight="1">
-      <c r="A23" s="41"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="39"/>
+      <c r="A23" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="42"/>
+      <c r="C23" s="41" t="s">
+        <v>64</v>
+      </c>
       <c r="D23" s="2">
-        <v>310111</v>
+        <v>145879</v>
       </c>
       <c r="E23" s="5"/>
       <c r="H23" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="I23" s="42"/>
+        <v>184</v>
+      </c>
+      <c r="I23" s="44" t="s">
+        <v>181</v>
+      </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:15" ht="60" customHeight="1">
-      <c r="A24" s="41"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="39"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="41"/>
       <c r="D24" s="2">
-        <v>528401</v>
+        <v>200437</v>
       </c>
       <c r="E24" s="5"/>
       <c r="H24" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="I24" s="42"/>
+        <v>185</v>
+      </c>
+      <c r="I24" s="44"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:15" ht="60" customHeight="1">
-      <c r="A25" s="41"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="39"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="41"/>
       <c r="D25" s="2">
-        <v>1076753</v>
+        <v>310111</v>
       </c>
       <c r="E25" s="5"/>
       <c r="H25" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="I25" s="42"/>
+        <v>186</v>
+      </c>
+      <c r="I25" s="44"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="5"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+    <row r="26" spans="1:15" ht="60" customHeight="1">
+      <c r="A26" s="43"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="2">
+        <v>528401</v>
+      </c>
       <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
+      <c r="H26" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="I26" s="44"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:15" ht="75" customHeight="1">
-      <c r="A27" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
+    <row r="27" spans="1:15" ht="60" customHeight="1">
+      <c r="A27" s="43"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="2">
+        <v>1076753</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="H27" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="I27" s="44"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" t="s">
+      <c r="A28" s="5"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+    </row>
+    <row r="29" spans="1:15" ht="75" customHeight="1">
+      <c r="A29" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
-      <c r="A29" s="5" t="s">
+    <row r="31" spans="1:15">
+      <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A29:F29"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -3037,21 +3087,21 @@
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="B15:B19"/>
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="B19:B25"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="I21:I25"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="B21:B27"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="I23:I27"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="C15:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3063,10 +3113,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3082,24 +3132,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="46.5" customHeight="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="47" t="s">
         <v>20</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -3108,10 +3158,10 @@
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14" ht="30.75" customHeight="1">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="1"/>
       <c r="F2" s="9" t="s">
         <v>39</v>
@@ -3195,219 +3245,212 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
+      <c r="I6" s="5"/>
       <c r="N6" s="5"/>
     </row>
-    <row r="7" spans="1:14" ht="45">
+    <row r="7" spans="1:14" ht="75">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>195</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>58</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="C7" s="15"/>
       <c r="D7" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>173</v>
-      </c>
+      <c r="F7" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="I7" s="5"/>
       <c r="N7" s="5"/>
     </row>
-    <row r="8" spans="1:14" ht="45">
+    <row r="8" spans="1:14">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>180</v>
-      </c>
       <c r="N8" s="5"/>
     </row>
-    <row r="9" spans="1:14" ht="90">
-      <c r="A9" s="5" t="s">
-        <v>25</v>
+    <row r="9" spans="1:14" ht="45">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>55</v>
+        <v>62</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>58</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="27" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="H9" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="G9" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="H9" s="31" t="s">
-        <v>173</v>
-      </c>
-      <c r="I9" s="33" t="s">
-        <v>22</v>
-      </c>
       <c r="N9" s="5"/>
     </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="5"/>
+    <row r="10" spans="1:14" ht="45">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:14" ht="270" customHeight="1">
-      <c r="A11" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>66</v>
+    <row r="11" spans="1:14" ht="90">
+      <c r="A11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="H11" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="I11" s="10"/>
+        <v>173</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>22</v>
+      </c>
       <c r="N11" s="5"/>
     </row>
-    <row r="12" spans="1:14" ht="45">
+    <row r="12" spans="1:14">
       <c r="A12" s="5"/>
-      <c r="B12" s="40"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="5"/>
+      <c r="N12" s="5"/>
+    </row>
+    <row r="13" spans="1:14" ht="270" customHeight="1">
+      <c r="A13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="10"/>
+      <c r="N13" s="5"/>
+    </row>
+    <row r="14" spans="1:14" ht="45">
+      <c r="A14" s="5"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I14" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="N12" s="5"/>
-    </row>
-    <row r="13" spans="1:14" ht="54" customHeight="1">
-      <c r="A13" s="41" t="s">
+      <c r="N14" s="5"/>
+    </row>
+    <row r="15" spans="1:14" ht="54" customHeight="1">
+      <c r="A15" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="39" t="s">
+      <c r="B15" s="42"/>
+      <c r="C15" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D15" s="5">
         <v>145879</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="42" t="s">
+      <c r="E15" s="5"/>
+      <c r="F15" s="44" t="s">
         <v>170</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H15" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I15" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="N13" s="5"/>
-    </row>
-    <row r="14" spans="1:14" ht="54" customHeight="1">
-      <c r="A14" s="41"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="5">
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="1:14" ht="54" customHeight="1">
+      <c r="A16" s="43"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="5">
         <v>200437</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="42"/>
-      <c r="H14" s="24" t="s">
+      <c r="E16" s="5"/>
+      <c r="F16" s="44"/>
+      <c r="H16" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="I16" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="N14" s="5"/>
-    </row>
-    <row r="15" spans="1:14" ht="54" customHeight="1">
-      <c r="A15" s="41"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="5">
+      <c r="N16" s="5"/>
+    </row>
+    <row r="17" spans="1:14" ht="54" customHeight="1">
+      <c r="A17" s="43"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="5">
         <v>310111</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="42"/>
-      <c r="H15" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="N15" s="5"/>
-    </row>
-    <row r="16" spans="1:14" ht="54" customHeight="1">
-      <c r="A16" s="41"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="5">
-        <v>528401</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="42"/>
-      <c r="H16" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="I16" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="N16" s="5"/>
-    </row>
-    <row r="17" spans="1:14" ht="54" customHeight="1">
-      <c r="A17" s="41"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="5">
-        <v>1076753</v>
-      </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="42"/>
+      <c r="F17" s="44"/>
       <c r="H17" s="25" t="s">
         <v>82</v>
       </c>
@@ -3416,67 +3459,101 @@
       </c>
       <c r="N17" s="5"/>
     </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+    <row r="18" spans="1:14" ht="54" customHeight="1">
+      <c r="A18" s="43"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="5">
+        <v>528401</v>
+      </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
+      <c r="F18" s="44"/>
+      <c r="H18" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="I18" s="21" t="s">
+        <v>22</v>
+      </c>
       <c r="N18" s="5"/>
     </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+    <row r="19" spans="1:14" ht="54" customHeight="1">
+      <c r="A19" s="43"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="5">
+        <v>1076753</v>
+      </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
+      <c r="F19" s="44"/>
+      <c r="H19" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>22</v>
+      </c>
       <c r="N19" s="5"/>
     </row>
-    <row r="20" spans="1:14" ht="105" customHeight="1">
-      <c r="A20" s="38" t="s">
+    <row r="20" spans="1:14">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="1:14" ht="105" customHeight="1">
+      <c r="A22" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" t="s">
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
-      <c r="A22" t="s">
+    <row r="24" spans="1:14">
+      <c r="A24" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="F13:F17"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="F15:F19"/>
+    <mergeCell ref="B13:B19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="A15:A19"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="D1:D2"/>
@@ -3494,10 +3571,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3509,29 +3586,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="F2" s="9" t="s">
         <v>38</v>
       </c>
@@ -3543,88 +3620,88 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="45">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="51" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="G3" s="50"/>
-      <c r="H3" s="56" t="s">
+      <c r="G3" s="52"/>
+      <c r="H3" s="39" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45">
-      <c r="A4" s="41"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="49"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="52" t="s">
         <v>155</v>
       </c>
-      <c r="G4" s="50"/>
-      <c r="H4" s="56" t="s">
+      <c r="G4" s="52"/>
+      <c r="H4" s="39" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45">
-      <c r="A5" s="41"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="49"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="51"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="50" t="s">
+      <c r="F5" s="52" t="s">
         <v>156</v>
       </c>
-      <c r="G5" s="50"/>
-      <c r="H5" s="56" t="s">
+      <c r="G5" s="52"/>
+      <c r="H5" s="39" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45">
-      <c r="A6" s="41"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="49"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="50" t="s">
+      <c r="F6" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="G6" s="50"/>
-      <c r="H6" s="56" t="s">
+      <c r="G6" s="52"/>
+      <c r="H6" s="39" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45">
-      <c r="A7" s="41"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="49"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="52" t="s">
         <v>158</v>
       </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="56" t="s">
+      <c r="G7" s="52"/>
+      <c r="H7" s="39" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3636,23 +3713,23 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="45">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="40" t="s">
         <v>71</v>
       </c>
       <c r="D9" s="2">
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="42" t="s">
+      <c r="G9" s="44" t="s">
         <v>86</v>
       </c>
       <c r="H9" s="27" t="s">
@@ -3660,57 +3737,57 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="36" customHeight="1">
-      <c r="A10" s="41"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="38"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="40"/>
       <c r="D10" s="2">
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
       <c r="H10" s="27" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="36" customHeight="1">
-      <c r="A11" s="41"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="38"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="2">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
       <c r="H11" s="27" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="36" customHeight="1">
-      <c r="A12" s="41"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="38"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="2">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
       <c r="H12" s="27" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="36" customHeight="1">
-      <c r="A13" s="41"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="38"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
       <c r="H13" s="27" t="s">
         <v>79</v>
       </c>
@@ -3726,82 +3803,82 @@
       <c r="H14" s="29"/>
     </row>
     <row r="15" spans="1:8" ht="54" customHeight="1">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="51" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="2">
         <v>145879</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42" t="s">
+      <c r="G15" s="44"/>
+      <c r="H15" s="44" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="54" customHeight="1">
-      <c r="A16" s="41"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="49"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="51"/>
       <c r="D16" s="2">
         <v>200437</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
     </row>
     <row r="17" spans="1:8" ht="54" customHeight="1">
-      <c r="A17" s="41"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="49"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="51"/>
       <c r="D17" s="2">
         <v>310111</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="42" t="s">
+      <c r="F17" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
     </row>
     <row r="18" spans="1:8" ht="54" customHeight="1">
-      <c r="A18" s="41"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="49"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="51"/>
       <c r="D18" s="2">
         <v>528401</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="42" t="s">
+      <c r="F18" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
     </row>
     <row r="19" spans="1:8" ht="54" customHeight="1">
-      <c r="A19" s="41"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="49"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="51"/>
       <c r="D19" s="2">
         <v>1076753</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="42" t="s">
+      <c r="F19" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="2"/>
@@ -3812,201 +3889,189 @@
       <c r="F20" s="20"/>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:8" ht="30">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:8" ht="60" customHeight="1">
+      <c r="A21" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" s="51"/>
+      <c r="D21" s="2">
+        <v>145879</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="31" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="45">
+      <c r="A22" s="45"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="2">
+        <v>200437</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="38" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="45"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="2">
+        <v>310111</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="45"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="2">
+        <v>528401</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="45"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="2">
+        <v>1076753</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="2"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:8" ht="30">
+      <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B27" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C27" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="27" t="s">
+      <c r="E27" s="2"/>
+      <c r="F27" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="G21" s="27" t="s">
+      <c r="G27" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="H21" s="27" t="s">
+      <c r="H27" s="27" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="2"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-    </row>
-    <row r="23" spans="1:8" ht="45">
-      <c r="A23" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="40" t="s">
-        <v>165</v>
-      </c>
-      <c r="C23" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="5">
-        <v>145879</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23" s="27" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="45">
-      <c r="A24" s="43"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="5">
-        <v>200437</v>
-      </c>
-      <c r="E24" s="5"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24" s="27" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="45" customHeight="1">
-      <c r="A25" s="43"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="5">
-        <v>310111</v>
-      </c>
-      <c r="E25" s="5"/>
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25" s="42" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="45" customHeight="1">
-      <c r="A26" s="43"/>
-      <c r="B26" s="40"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="5">
-        <v>528401</v>
-      </c>
-      <c r="E26" s="5"/>
-      <c r="F26"/>
-      <c r="G26"/>
-      <c r="H26" s="42"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="43"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="5">
-        <v>1076753</v>
-      </c>
-      <c r="E27" s="5"/>
-      <c r="F27"/>
-      <c r="G27"/>
-      <c r="H27" s="42"/>
-    </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="5"/>
+      <c r="A28" s="2"/>
       <c r="B28" s="10"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
     </row>
-    <row r="29" spans="1:8" ht="54" customHeight="1">
-      <c r="A29" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="C29" s="46" t="s">
-        <v>63</v>
+    <row r="29" spans="1:8" ht="45">
+      <c r="A29" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="C29" s="43" t="s">
+        <v>54</v>
       </c>
       <c r="D29" s="5">
         <v>145879</v>
       </c>
       <c r="E29" s="5"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
+      <c r="F29"/>
+      <c r="G29"/>
       <c r="H29" s="27" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="54" customHeight="1">
-      <c r="A30" s="43"/>
-      <c r="B30" s="40"/>
-      <c r="C30" s="47"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="45">
+      <c r="A30" s="45"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="43"/>
       <c r="D30" s="5">
         <v>200437</v>
       </c>
       <c r="E30" s="5"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
+      <c r="F30"/>
+      <c r="G30"/>
       <c r="H30" s="27" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="54" customHeight="1">
-      <c r="A31" s="43"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="47"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="45" customHeight="1">
+      <c r="A31" s="45"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="43"/>
       <c r="D31" s="5">
         <v>310111</v>
       </c>
       <c r="E31" s="5"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="27" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="54" customHeight="1">
-      <c r="A32" s="43"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="47"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31" s="44" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="45" customHeight="1">
+      <c r="A32" s="45"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="43"/>
       <c r="D32" s="5">
         <v>528401</v>
       </c>
       <c r="E32" s="5"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="27" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="54" customHeight="1">
-      <c r="A33" s="43"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="47"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32" s="44"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="45"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="43"/>
       <c r="D33" s="5">
         <v>1076753</v>
       </c>
       <c r="E33" s="5"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="27" t="s">
-        <v>114</v>
-      </c>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33" s="44"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="5"/>
-      <c r="B34" s="40"/>
+      <c r="B34" s="10"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
@@ -4014,77 +4079,163 @@
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
     </row>
-    <row r="35" spans="1:8" ht="270" customHeight="1">
-      <c r="A35" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="40"/>
-      <c r="C35" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>34</v>
+    <row r="35" spans="1:8" ht="54" customHeight="1">
+      <c r="A35" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="C35" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="5">
+        <v>145879</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
       <c r="H35" s="27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="54" customHeight="1">
+      <c r="A36" s="45"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="5">
+        <v>200437</v>
+      </c>
       <c r="E36" s="5"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="H36" s="27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="54" customHeight="1">
+      <c r="A37" s="45"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="5">
+        <v>310111</v>
+      </c>
       <c r="E37" s="5"/>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-    </row>
-    <row r="38" spans="1:8" ht="94.5" customHeight="1">
-      <c r="A38" s="38" t="s">
+      <c r="H37" s="27" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="54" customHeight="1">
+      <c r="A38" s="45"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="5">
+        <v>528401</v>
+      </c>
+      <c r="E38" s="5"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="54" customHeight="1">
+      <c r="A39" s="45"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="5">
+        <v>1076753</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="27" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="5"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+    </row>
+    <row r="41" spans="1:8" ht="270" customHeight="1">
+      <c r="A41" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="42"/>
+      <c r="C41" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+    </row>
+    <row r="44" spans="1:8" ht="94.5" customHeight="1">
+      <c r="A44" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="B38" s="38"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" t="s">
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="5" t="s">
+    <row r="46" spans="1:8">
+      <c r="A46" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
-      <c r="A41" t="s">
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
         <v>137</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="38">
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H25:H27"/>
+    <mergeCell ref="H31:H33"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F17:G17"/>
@@ -4092,21 +4243,24 @@
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H15:H19"/>
     <mergeCell ref="G9:G13"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="C29:C33"/>
     <mergeCell ref="B15:B19"/>
     <mergeCell ref="C15:C19"/>
     <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="A44:F44"/>
     <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B29:B35"/>
+    <mergeCell ref="B35:B41"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="C35:C39"/>
+    <mergeCell ref="A35:A39"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="C9:C13"/>
@@ -4126,10 +4280,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4142,29 +4296,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="49.5" customHeight="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="47" t="s">
         <v>20</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="45"/>
+      <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="44"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="1"/>
       <c r="F2" s="9" t="s">
         <v>39</v>
@@ -4174,13 +4328,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="36" customHeight="1">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="40" t="s">
         <v>51</v>
       </c>
       <c r="D3" s="2">
@@ -4192,9 +4346,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="36" customHeight="1">
-      <c r="A4" s="41"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="38"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
@@ -4204,9 +4358,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="36" customHeight="1">
-      <c r="A5" s="41"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="38"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
@@ -4216,9 +4370,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="36" customHeight="1">
-      <c r="A6" s="41"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="38"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
@@ -4228,9 +4382,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1">
-      <c r="A7" s="41"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="38"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
@@ -4246,71 +4400,71 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="45" customHeight="1">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="51" t="s">
         <v>46</v>
       </c>
       <c r="D9" s="2">
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="51" t="s">
+      <c r="F9" s="53" t="s">
         <v>178</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="45" customHeight="1">
-      <c r="A10" s="41"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="49"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="51"/>
       <c r="D10" s="2">
         <v>200437</v>
       </c>
-      <c r="F10" s="51"/>
+      <c r="F10" s="53"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="45" customHeight="1">
-      <c r="A11" s="41"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="49"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="51"/>
       <c r="D11" s="2">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="51"/>
+      <c r="F11" s="53"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="45" customHeight="1">
-      <c r="A12" s="41"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="49"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="2">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="52" t="s">
-        <v>189</v>
-      </c>
+      <c r="F12" s="53"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="45" customHeight="1">
-      <c r="A13" s="41"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="49"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="52"/>
+      <c r="F13" s="31" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2"/>
@@ -4319,259 +4473,328 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="30">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:8" ht="75" customHeight="1">
+      <c r="A15" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15" s="51"/>
+      <c r="D15" s="2">
+        <v>145879</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="G15" s="10"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="43"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="2">
+        <v>200437</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="54" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="43"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="2">
+        <v>310111</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="54"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="43"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="2">
+        <v>528401</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="54"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="43"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="2">
+        <v>1076753</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="54"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:14" ht="30">
+      <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B21" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C21" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="26" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="G15" s="28" t="s">
+      <c r="G21" s="28" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:14" ht="75" customHeight="1">
-      <c r="A17" s="10" t="s">
+    <row r="22" spans="1:14">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" ht="75" customHeight="1">
+      <c r="A23" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B23" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="26" t="s">
+      <c r="E23" s="5"/>
+      <c r="F23" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="G23" s="28" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="N18" s="12"/>
-    </row>
-    <row r="19" spans="1:14" ht="54" customHeight="1">
-      <c r="A19" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="C19" s="46" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" s="5">
-        <v>145879</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="N19" s="12"/>
-    </row>
-    <row r="20" spans="1:14" ht="54" customHeight="1">
-      <c r="A20" s="41"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="5">
-        <v>200437</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="N20" s="12"/>
-    </row>
-    <row r="21" spans="1:14" ht="54" customHeight="1">
-      <c r="A21" s="41"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="5">
-        <v>310111</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="N21" s="12"/>
-    </row>
-    <row r="22" spans="1:14" ht="54" customHeight="1">
-      <c r="A22" s="41"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="5">
-        <v>528401</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="N22" s="12"/>
-    </row>
-    <row r="23" spans="1:14" ht="54" customHeight="1">
-      <c r="A23" s="41"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="5">
-        <v>1076753</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="N23" s="12"/>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="5"/>
-      <c r="B24" s="40"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="N24" s="12"/>
     </row>
     <row r="25" spans="1:14" ht="54" customHeight="1">
-      <c r="A25" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="46" t="s">
-        <v>69</v>
+      <c r="A25" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="C25" s="48" t="s">
+        <v>95</v>
       </c>
       <c r="D25" s="5">
         <v>145879</v>
       </c>
       <c r="E25" s="5"/>
-      <c r="F25" s="27" t="s">
-        <v>97</v>
+      <c r="F25" s="31" t="s">
+        <v>105</v>
       </c>
       <c r="N25" s="12"/>
     </row>
     <row r="26" spans="1:14" ht="54" customHeight="1">
-      <c r="A26" s="41"/>
-      <c r="B26" s="40"/>
-      <c r="C26" s="47"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="5">
         <v>200437</v>
       </c>
       <c r="E26" s="5"/>
-      <c r="F26" s="27" t="s">
-        <v>98</v>
+      <c r="F26" s="31" t="s">
+        <v>101</v>
       </c>
       <c r="N26" s="12"/>
     </row>
     <row r="27" spans="1:14" ht="54" customHeight="1">
-      <c r="A27" s="41"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="47"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="49"/>
       <c r="D27" s="5">
         <v>310111</v>
       </c>
       <c r="E27" s="5"/>
-      <c r="F27" s="27" t="s">
-        <v>99</v>
-      </c>
+      <c r="F27" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="N27" s="12"/>
     </row>
     <row r="28" spans="1:14" ht="54" customHeight="1">
-      <c r="A28" s="41"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="47"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="49"/>
       <c r="D28" s="5">
         <v>528401</v>
       </c>
       <c r="E28" s="5"/>
-      <c r="F28" s="27" t="s">
-        <v>100</v>
-      </c>
+      <c r="F28" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="N28" s="12"/>
     </row>
     <row r="29" spans="1:14" ht="54" customHeight="1">
-      <c r="A29" s="41"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="47"/>
+      <c r="A29" s="43"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="49"/>
       <c r="D29" s="5">
         <v>1076753</v>
       </c>
       <c r="E29" s="5"/>
-      <c r="F29" s="27" t="s">
-        <v>96</v>
-      </c>
+      <c r="F29" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="N29" s="12"/>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="B30" s="42"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:14" ht="99.95" customHeight="1">
-      <c r="A31" s="38" t="s">
+      <c r="N30" s="12"/>
+    </row>
+    <row r="31" spans="1:14" ht="54" customHeight="1">
+      <c r="A31" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="42"/>
+      <c r="C31" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="5">
+        <v>145879</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="N31" s="12"/>
+    </row>
+    <row r="32" spans="1:14" ht="54" customHeight="1">
+      <c r="A32" s="43"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="5">
+        <v>200437</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="N32" s="12"/>
+    </row>
+    <row r="33" spans="1:7" ht="54" customHeight="1">
+      <c r="A33" s="43"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="5">
+        <v>310111</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="54" customHeight="1">
+      <c r="A34" s="43"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="5">
+        <v>528401</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="54" customHeight="1">
+      <c r="A35" s="43"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="5">
+        <v>1076753</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:7" ht="99.95" customHeight="1">
+      <c r="A37" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32" t="s">
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A31:G31"/>
+  <mergeCells count="22">
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="C31:C35"/>
     <mergeCell ref="A25:A29"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="B25:B35"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="C15:C19"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="C25:C29"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="B19:B29"/>
     <mergeCell ref="C9:C13"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="F16:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4586,7 +4809,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4607,12 +4830,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -4702,27 +4925,27 @@
       <c r="K4" s="2"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
     </row>
     <row r="7" spans="1:12" ht="90" customHeight="1">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -4782,12 +5005,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -4829,99 +5052,99 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="40" t="s">
         <v>49</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="44" t="s">
         <v>183</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="44" t="s">
         <v>183</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="44" t="s">
         <v>183</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="44" t="s">
         <v>183</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="53" t="s">
+      <c r="J3" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="41" t="s">
+      <c r="K3" s="43" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A4" s="41"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="38"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="41"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="43"/>
     </row>
     <row r="5" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A5" s="41"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="38"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="41"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="43"/>
     </row>
     <row r="6" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A6" s="41"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="38"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="41"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="43"/>
     </row>
     <row r="7" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A7" s="41"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="38"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="41"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="43"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="10"/>
@@ -4950,29 +5173,29 @@
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
     </row>
     <row r="11" spans="1:12" ht="99.95" customHeight="1">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -5041,12 +5264,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -5088,13 +5311,13 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="45">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="49" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="10">
@@ -5123,11 +5346,11 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1">
-      <c r="A4" s="41"/>
-      <c r="B4" s="40" t="s">
+      <c r="A4" s="43"/>
+      <c r="B4" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="54"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="10">
         <v>200437</v>
       </c>
@@ -5148,9 +5371,9 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1">
-      <c r="A5" s="41"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="54"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="56"/>
       <c r="D5" s="10">
         <v>310111</v>
       </c>
@@ -5171,9 +5394,9 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
-      <c r="A6" s="41"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="54"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="10">
         <v>528401</v>
       </c>
@@ -5194,9 +5417,9 @@
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
-      <c r="A7" s="41"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="54"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="56"/>
       <c r="D7" s="10">
         <v>1076753</v>
       </c>
@@ -5221,14 +5444,14 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:12" ht="90" customHeight="1">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -5291,13 +5514,13 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
       <c r="J1" s="10"/>
       <c r="K1" s="11"/>
       <c r="L1" s="10"/>
@@ -5341,13 +5564,13 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="45" customHeight="1">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="40" t="s">
         <v>51</v>
       </c>
       <c r="D3" s="2">
@@ -5365,23 +5588,23 @@
       <c r="H3" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="I3" s="55" t="s">
+      <c r="I3" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="J3" s="41" t="s">
+      <c r="J3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="53" t="s">
+      <c r="K3" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="41" t="s">
+      <c r="L3" s="43" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="45" customHeight="1">
-      <c r="A4" s="41"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="38"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
@@ -5397,15 +5620,15 @@
       <c r="H4" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="I4" s="55"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="41"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="43"/>
     </row>
     <row r="5" spans="1:12" ht="45" customHeight="1">
-      <c r="A5" s="41"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="38"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
@@ -5421,15 +5644,15 @@
       <c r="H5" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="I5" s="55"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="41"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="43"/>
     </row>
     <row r="6" spans="1:12" ht="45" customHeight="1">
-      <c r="A6" s="41"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="38"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
@@ -5445,15 +5668,15 @@
       <c r="H6" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="I6" s="55"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="41"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="43"/>
     </row>
     <row r="7" spans="1:12" ht="45" customHeight="1">
-      <c r="A7" s="41"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="38"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
@@ -5469,10 +5692,10 @@
       <c r="H7" s="31" t="s">
         <v>194</v>
       </c>
-      <c r="I7" s="55"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="41"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="43"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="10"/>
@@ -5489,30 +5712,30 @@
       <c r="L8" s="2"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
     </row>
     <row r="11" spans="1:12" ht="75" customHeight="1">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -5555,12 +5778,12 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="38"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="5"/>

</xml_diff>

<commit_message>
Finished re-running SigProfilerExtractor for SBS_set2/Realistic on HPC-cluster.
The newly-generated results are also included in the summary tables and plots
</commit_message>
<xml_diff>
--- a/documents/CPU_timing/mSigHdp-paper-tracking.xlsx
+++ b/documents/CPU_timing/mSigHdp-paper-tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\documents\CPU_timing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87EF474A-4D44-42EF-8F3E-123B5060B6BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A2AB4A-D369-4022-B780-8352B2E8FE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11550" yWindow="1485" windowWidth="15615" windowHeight="13980" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -1531,7 +1531,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1540,16 +1546,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1561,16 +1567,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -1580,6 +1577,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2118,40 +2118,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="50.1" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="M1" s="47" t="s">
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="M1" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
       <c r="F2" s="9">
         <v>5</v>
       </c>
@@ -2190,10 +2190,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="68.25" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>136</v>
       </c>
       <c r="C3" s="40" t="s">
@@ -2218,121 +2218,121 @@
       <c r="J3" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="K3" s="44" t="s">
+      <c r="K3" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="M3" s="44" t="s">
+      <c r="M3" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="N3" s="44" t="s">
+      <c r="N3" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="O3" s="44" t="s">
+      <c r="O3" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="P3" s="44" t="s">
+      <c r="P3" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="Q3" s="44" t="s">
+      <c r="Q3" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="R3" s="44" t="s">
+      <c r="R3" s="43" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="75" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="50"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="52"/>
       <c r="C4" s="40"/>
       <c r="D4" s="10">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="44" t="s">
+      <c r="G4" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="H4" s="44" t="s">
+      <c r="H4" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="I4" s="44" t="s">
+      <c r="I4" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="J4" s="44" t="s">
+      <c r="J4" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="K4" s="44"/>
-      <c r="M4" s="44"/>
-      <c r="N4" s="44"/>
-      <c r="O4" s="44"/>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="44"/>
-      <c r="R4" s="44"/>
+      <c r="K4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
     </row>
     <row r="5" spans="1:18" ht="36" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="50"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="52"/>
       <c r="C5" s="40"/>
       <c r="D5" s="10">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
     </row>
     <row r="6" spans="1:18" ht="36" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="50"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="40"/>
       <c r="D6" s="10">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="44"/>
-      <c r="P6" s="44"/>
-      <c r="Q6" s="44"/>
-      <c r="R6" s="44"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
     </row>
     <row r="7" spans="1:18" ht="36" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="50"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="40"/>
       <c r="D7" s="10">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="M7" s="44"/>
-      <c r="N7" s="44"/>
-      <c r="O7" s="44"/>
-      <c r="P7" s="44"/>
-      <c r="Q7" s="44"/>
-      <c r="R7" s="44"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="43"/>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="2"/>
@@ -2343,139 +2343,139 @@
       <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:18" ht="54" customHeight="1">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="49" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="10">
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="G9" s="44" t="s">
+      <c r="G9" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="H9" s="44" t="s">
+      <c r="H9" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="I9" s="44" t="s">
+      <c r="I9" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="J9" s="44" t="s">
+      <c r="J9" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="44" t="s">
+      <c r="K9" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="M9" s="44" t="s">
+      <c r="M9" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="N9" s="44" t="s">
+      <c r="N9" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="O9" s="44" t="s">
+      <c r="O9" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="P9" s="44" t="s">
+      <c r="P9" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="Q9" s="44" t="s">
+      <c r="Q9" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="R9" s="44" t="s">
+      <c r="R9" s="43" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="54" customHeight="1">
-      <c r="A10" s="43"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="51"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="10">
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="44"/>
-      <c r="Q10" s="44"/>
-      <c r="R10" s="44"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
     </row>
     <row r="11" spans="1:18" ht="54" customHeight="1">
-      <c r="A11" s="43"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="51"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="10">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="44"/>
-      <c r="O11" s="44"/>
-      <c r="P11" s="44"/>
-      <c r="Q11" s="44"/>
-      <c r="R11" s="44"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
     </row>
     <row r="12" spans="1:18" ht="54" customHeight="1">
-      <c r="A12" s="43"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="51"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="10">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="44"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="44"/>
-      <c r="R12" s="44"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
     </row>
     <row r="13" spans="1:18" ht="54" customHeight="1">
-      <c r="A13" s="43"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="10">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="44"/>
-      <c r="O13" s="44"/>
-      <c r="P13" s="44"/>
-      <c r="Q13" s="44"/>
-      <c r="R13" s="44"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="43"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="5"/>
@@ -2509,28 +2509,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="M3:M7"/>
-    <mergeCell ref="N3:N7"/>
-    <mergeCell ref="O3:O7"/>
-    <mergeCell ref="P3:P7"/>
-    <mergeCell ref="M9:M13"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="N9:N13"/>
-    <mergeCell ref="O9:O13"/>
-    <mergeCell ref="P9:P13"/>
-    <mergeCell ref="Q9:Q13"/>
-    <mergeCell ref="R9:R13"/>
-    <mergeCell ref="Q3:Q7"/>
-    <mergeCell ref="R3:R7"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="K9:K13"/>
     <mergeCell ref="J9:J13"/>
@@ -2546,6 +2524,28 @@
     <mergeCell ref="K3:K7"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="H4:H7"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="P3:P7"/>
+    <mergeCell ref="M9:M13"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="N9:N13"/>
+    <mergeCell ref="O9:O13"/>
+    <mergeCell ref="P9:P13"/>
+    <mergeCell ref="Q9:Q13"/>
+    <mergeCell ref="R9:R13"/>
+    <mergeCell ref="Q3:Q7"/>
+    <mergeCell ref="R3:R7"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="M3:M7"/>
+    <mergeCell ref="N3:N7"/>
+    <mergeCell ref="O3:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2574,32 +2574,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:15" ht="45">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
       <c r="F2" s="9" t="s">
         <v>38</v>
       </c>
@@ -2616,10 +2616,10 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="45" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>144</v>
       </c>
       <c r="C3" s="40" t="s">
@@ -2629,79 +2629,79 @@
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:15" ht="45" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="45" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="45" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="44" t="s">
+      <c r="F6" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:15" ht="45" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="43" t="s">
         <v>151</v>
       </c>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
       <c r="K7" s="2"/>
@@ -2733,11 +2733,11 @@
         <v>34</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
       <c r="J9" s="4"/>
       <c r="K9" s="5"/>
     </row>
@@ -2827,84 +2827,84 @@
       <c r="O14" s="34"/>
     </row>
     <row r="15" spans="1:15" ht="60" customHeight="1">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="44" t="s">
         <v>165</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="47" t="s">
         <v>56</v>
       </c>
       <c r="D15" s="2">
         <v>145879</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="44" t="s">
+      <c r="F15" s="43" t="s">
         <v>160</v>
       </c>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
       <c r="O15" s="34"/>
     </row>
     <row r="16" spans="1:15" ht="60" customHeight="1">
-      <c r="A16" s="43"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="45"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="2">
         <v>200437</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="44" t="s">
+      <c r="F16" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
       <c r="O16" s="34"/>
     </row>
     <row r="17" spans="1:15" ht="60" customHeight="1">
-      <c r="A17" s="43"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="45"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="47"/>
       <c r="D17" s="2">
         <v>310111</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="44" t="s">
+      <c r="F17" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
       <c r="O17" s="34"/>
     </row>
     <row r="18" spans="1:15" ht="60" customHeight="1">
-      <c r="A18" s="43"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="45"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="47"/>
       <c r="D18" s="2">
         <v>528401</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="44" t="s">
+      <c r="F18" s="43" t="s">
         <v>163</v>
       </c>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
       <c r="O18" s="34"/>
     </row>
     <row r="19" spans="1:15" ht="60" customHeight="1">
-      <c r="A19" s="43"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="45"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="47"/>
       <c r="D19" s="2">
         <v>1076753</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="44" t="s">
+      <c r="F19" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
       <c r="O19" s="34"/>
     </row>
     <row r="20" spans="1:15">
@@ -2924,7 +2924,7 @@
       <c r="A21" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="44" t="s">
         <v>176</v>
       </c>
       <c r="C21" s="18" t="s">
@@ -2945,7 +2945,7 @@
     </row>
     <row r="22" spans="1:15" ht="30" customHeight="1">
       <c r="A22" s="10"/>
-      <c r="B22" s="42"/>
+      <c r="B22" s="44"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -2955,11 +2955,11 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:15" ht="60" customHeight="1">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="42"/>
-      <c r="C23" s="41" t="s">
+      <c r="B23" s="44"/>
+      <c r="C23" s="46" t="s">
         <v>64</v>
       </c>
       <c r="D23" s="2">
@@ -2969,16 +2969,16 @@
       <c r="H23" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="I23" s="44" t="s">
+      <c r="I23" s="43" t="s">
         <v>181</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:15" ht="60" customHeight="1">
-      <c r="A24" s="43"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="41"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="46"/>
       <c r="D24" s="2">
         <v>200437</v>
       </c>
@@ -2986,14 +2986,14 @@
       <c r="H24" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="I24" s="44"/>
+      <c r="I24" s="43"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:15" ht="60" customHeight="1">
-      <c r="A25" s="43"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="41"/>
+      <c r="A25" s="45"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="46"/>
       <c r="D25" s="2">
         <v>310111</v>
       </c>
@@ -3001,14 +3001,14 @@
       <c r="H25" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="I25" s="44"/>
+      <c r="I25" s="43"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:15" ht="60" customHeight="1">
-      <c r="A26" s="43"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="41"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="46"/>
       <c r="D26" s="2">
         <v>528401</v>
       </c>
@@ -3016,14 +3016,14 @@
       <c r="H26" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="I26" s="44"/>
+      <c r="I26" s="43"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
     </row>
     <row r="27" spans="1:15" ht="60" customHeight="1">
-      <c r="A27" s="43"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="41"/>
+      <c r="A27" s="45"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="46"/>
       <c r="D27" s="2">
         <v>1076753</v>
       </c>
@@ -3031,7 +3031,7 @@
       <c r="H27" s="27" t="s">
         <v>188</v>
       </c>
-      <c r="I27" s="44"/>
+      <c r="I27" s="43"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
@@ -3075,6 +3075,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="B21:B27"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="I23:I27"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
     <mergeCell ref="A29:F29"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="A1:A2"/>
@@ -3091,17 +3102,6 @@
     <mergeCell ref="F18:H18"/>
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="B15:B19"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="B21:B27"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="I23:I27"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="C15:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3132,24 +3132,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="46.5" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="42" t="s">
         <v>20</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -3158,10 +3158,10 @@
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14" ht="30.75" customHeight="1">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="1"/>
       <c r="F2" s="9" t="s">
         <v>39</v>
@@ -3363,7 +3363,7 @@
       <c r="A13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="44" t="s">
         <v>176</v>
       </c>
       <c r="C13" s="18" t="s">
@@ -3384,7 +3384,7 @@
     </row>
     <row r="14" spans="1:14" ht="45">
       <c r="A14" s="5"/>
-      <c r="B14" s="42"/>
+      <c r="B14" s="44"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -3403,18 +3403,18 @@
       <c r="N14" s="5"/>
     </row>
     <row r="15" spans="1:14" ht="54" customHeight="1">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="41" t="s">
+      <c r="B15" s="44"/>
+      <c r="C15" s="46" t="s">
         <v>65</v>
       </c>
       <c r="D15" s="5">
         <v>145879</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="44" t="s">
+      <c r="F15" s="43" t="s">
         <v>170</v>
       </c>
       <c r="H15" s="24" t="s">
@@ -3426,14 +3426,14 @@
       <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:14" ht="54" customHeight="1">
-      <c r="A16" s="43"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="41"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="5">
         <v>200437</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="44"/>
+      <c r="F16" s="43"/>
       <c r="H16" s="24" t="s">
         <v>77</v>
       </c>
@@ -3443,14 +3443,14 @@
       <c r="N16" s="5"/>
     </row>
     <row r="17" spans="1:14" ht="54" customHeight="1">
-      <c r="A17" s="43"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="41"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="46"/>
       <c r="D17" s="5">
         <v>310111</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="44"/>
+      <c r="F17" s="43"/>
       <c r="H17" s="25" t="s">
         <v>82</v>
       </c>
@@ -3460,14 +3460,14 @@
       <c r="N17" s="5"/>
     </row>
     <row r="18" spans="1:14" ht="54" customHeight="1">
-      <c r="A18" s="43"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="41"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="46"/>
       <c r="D18" s="5">
         <v>528401</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="44"/>
+      <c r="F18" s="43"/>
       <c r="H18" s="25" t="s">
         <v>82</v>
       </c>
@@ -3477,14 +3477,14 @@
       <c r="N18" s="5"/>
     </row>
     <row r="19" spans="1:14" ht="54" customHeight="1">
-      <c r="A19" s="43"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="41"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="46"/>
       <c r="D19" s="5">
         <v>1076753</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="44"/>
+      <c r="F19" s="43"/>
       <c r="H19" s="25" t="s">
         <v>82</v>
       </c>
@@ -3549,16 +3549,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="F15:F19"/>
     <mergeCell ref="B13:B19"/>
     <mergeCell ref="C15:C19"/>
     <mergeCell ref="A15:A19"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3573,8 +3573,8 @@
   </sheetPr>
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3586,29 +3586,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
       <c r="F2" s="9" t="s">
         <v>38</v>
       </c>
@@ -3620,87 +3620,87 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="45">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="49" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="48"/>
       <c r="H3" s="39" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="51"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="48"/>
       <c r="H4" s="39" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="51"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="52" t="s">
+      <c r="F5" s="48" t="s">
         <v>156</v>
       </c>
-      <c r="G5" s="52"/>
+      <c r="G5" s="48"/>
       <c r="H5" s="39" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="51"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="52" t="s">
+      <c r="F6" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="G6" s="52"/>
+      <c r="G6" s="48"/>
       <c r="H6" s="39" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="51"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="49"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="G7" s="52"/>
+      <c r="G7" s="48"/>
       <c r="H7" s="39" t="s">
         <v>158</v>
       </c>
@@ -3713,10 +3713,10 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="45">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="44" t="s">
         <v>136</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -3726,10 +3726,10 @@
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="44" t="s">
+      <c r="G9" s="43" t="s">
         <v>86</v>
       </c>
       <c r="H9" s="27" t="s">
@@ -3737,57 +3737,57 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="36" customHeight="1">
-      <c r="A10" s="43"/>
-      <c r="B10" s="50"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="40"/>
       <c r="D10" s="2">
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="27" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="36" customHeight="1">
-      <c r="A11" s="43"/>
-      <c r="B11" s="50"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="40"/>
       <c r="D11" s="2">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
       <c r="H11" s="27" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="36" customHeight="1">
-      <c r="A12" s="43"/>
-      <c r="B12" s="50"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="52"/>
       <c r="C12" s="40"/>
       <c r="D12" s="2">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
       <c r="H12" s="27" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="36" customHeight="1">
-      <c r="A13" s="43"/>
-      <c r="B13" s="50"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="40"/>
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
       <c r="H13" s="27" t="s">
         <v>79</v>
       </c>
@@ -3803,82 +3803,82 @@
       <c r="H14" s="29"/>
     </row>
     <row r="15" spans="1:8" ht="54" customHeight="1">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="49" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="2">
         <v>145879</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="44" t="s">
+      <c r="F15" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44" t="s">
+      <c r="G15" s="43"/>
+      <c r="H15" s="43" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="54" customHeight="1">
-      <c r="A16" s="43"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="51"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="49"/>
       <c r="D16" s="2">
         <v>200437</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="44" t="s">
+      <c r="F16" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
     </row>
     <row r="17" spans="1:8" ht="54" customHeight="1">
-      <c r="A17" s="43"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="51"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="49"/>
       <c r="D17" s="2">
         <v>310111</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="44" t="s">
+      <c r="F17" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
     </row>
     <row r="18" spans="1:8" ht="54" customHeight="1">
-      <c r="A18" s="43"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="51"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="49"/>
       <c r="D18" s="2">
         <v>528401</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="44" t="s">
+      <c r="F18" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
     </row>
     <row r="19" spans="1:8" ht="54" customHeight="1">
-      <c r="A19" s="43"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="51"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="2">
         <v>1076753</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="44" t="s">
+      <c r="F19" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="2"/>
@@ -3890,27 +3890,27 @@
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:8" ht="60" customHeight="1">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="47" t="s">
         <v>195</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="C21" s="51"/>
+      <c r="C21" s="49"/>
       <c r="D21" s="2">
         <v>145879</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="20"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="31" t="s">
+      <c r="H21" s="35" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="45">
-      <c r="A22" s="45"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="51"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="49"/>
       <c r="D22" s="2">
         <v>200437</v>
       </c>
@@ -3922,9 +3922,9 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="45"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="51"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="2">
         <v>310111</v>
       </c>
@@ -3933,9 +3933,9 @@
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="45"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="51"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="49"/>
       <c r="D24" s="2">
         <v>528401</v>
       </c>
@@ -3944,9 +3944,9 @@
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="45"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="51"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="2">
         <v>1076753</v>
       </c>
@@ -3998,13 +3998,13 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" ht="45">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="44" t="s">
         <v>165</v>
       </c>
-      <c r="C29" s="43" t="s">
+      <c r="C29" s="45" t="s">
         <v>54</v>
       </c>
       <c r="D29" s="5">
@@ -4018,9 +4018,9 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="45">
-      <c r="A30" s="45"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="43"/>
+      <c r="A30" s="47"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="45"/>
       <c r="D30" s="5">
         <v>200437</v>
       </c>
@@ -4032,42 +4032,42 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="45" customHeight="1">
-      <c r="A31" s="45"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="43"/>
+      <c r="A31" s="47"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="45"/>
       <c r="D31" s="5">
         <v>310111</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31"/>
       <c r="G31"/>
-      <c r="H31" s="44" t="s">
+      <c r="H31" s="43" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="45" customHeight="1">
-      <c r="A32" s="45"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="43"/>
+      <c r="A32" s="47"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="45"/>
       <c r="D32" s="5">
         <v>528401</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32"/>
       <c r="G32"/>
-      <c r="H32" s="44"/>
+      <c r="H32" s="43"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="45"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="43"/>
+      <c r="A33" s="47"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="45"/>
       <c r="D33" s="5">
         <v>1076753</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33"/>
       <c r="G33"/>
-      <c r="H33" s="44"/>
+      <c r="H33" s="43"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="5"/>
@@ -4080,13 +4080,13 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" ht="54" customHeight="1">
-      <c r="A35" s="45" t="s">
+      <c r="A35" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="C35" s="48" t="s">
+      <c r="C35" s="50" t="s">
         <v>63</v>
       </c>
       <c r="D35" s="5">
@@ -4100,9 +4100,9 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="54" customHeight="1">
-      <c r="A36" s="45"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="49"/>
+      <c r="A36" s="47"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="51"/>
       <c r="D36" s="5">
         <v>200437</v>
       </c>
@@ -4114,9 +4114,9 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="54" customHeight="1">
-      <c r="A37" s="45"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="49"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="51"/>
       <c r="D37" s="5">
         <v>310111</v>
       </c>
@@ -4128,9 +4128,9 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="54" customHeight="1">
-      <c r="A38" s="45"/>
-      <c r="B38" s="42"/>
-      <c r="C38" s="49"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="44"/>
+      <c r="C38" s="51"/>
       <c r="D38" s="5">
         <v>528401</v>
       </c>
@@ -4142,9 +4142,9 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="54" customHeight="1">
-      <c r="A39" s="45"/>
-      <c r="B39" s="42"/>
-      <c r="C39" s="49"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="51"/>
       <c r="D39" s="5">
         <v>1076753</v>
       </c>
@@ -4157,7 +4157,7 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="5"/>
-      <c r="B40" s="42"/>
+      <c r="B40" s="44"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -4169,7 +4169,7 @@
       <c r="A41" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="42"/>
+      <c r="B41" s="44"/>
       <c r="C41" s="19" t="s">
         <v>70</v>
       </c>
@@ -4230,28 +4230,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H31:H33"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H15:H19"/>
-    <mergeCell ref="G9:G13"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="C21:C25"/>
     <mergeCell ref="A44:F44"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="B35:B41"/>
@@ -4268,6 +4246,28 @@
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="F9:F13"/>
+    <mergeCell ref="G9:G13"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="H31:H33"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H15:H19"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4282,8 +4282,8 @@
   </sheetPr>
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:F19"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4296,29 +4296,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="49.5" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="42" t="s">
         <v>20</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="47"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="1"/>
       <c r="F2" s="9" t="s">
         <v>39</v>
@@ -4328,10 +4328,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="36" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>136</v>
       </c>
       <c r="C3" s="40" t="s">
@@ -4346,8 +4346,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="36" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
@@ -4358,8 +4358,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="36" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
@@ -4370,8 +4370,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="36" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
@@ -4382,8 +4382,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
@@ -4400,13 +4400,13 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="45" customHeight="1">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="49" t="s">
         <v>46</v>
       </c>
       <c r="D9" s="2">
@@ -4420,9 +4420,9 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="45" customHeight="1">
-      <c r="A10" s="43"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="51"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="2">
         <v>200437</v>
       </c>
@@ -4431,9 +4431,9 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="45" customHeight="1">
-      <c r="A11" s="43"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="51"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="2">
         <v>310111</v>
       </c>
@@ -4443,28 +4443,29 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="45" customHeight="1">
-      <c r="A12" s="43"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="51"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="2">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="53"/>
+      <c r="F12" s="57" t="s">
+        <v>189</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="45" customHeight="1">
-      <c r="A13" s="43"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="51"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="31" t="s">
-        <v>189</v>
-      </c>
+      <c r="F13" s="57"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2"/>
@@ -4472,65 +4473,66 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" ht="75" customHeight="1">
-      <c r="A15" s="43" t="s">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="45" t="s">
         <v>195</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="C15" s="51"/>
+      <c r="C15" s="49"/>
       <c r="D15" s="2">
         <v>145879</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="35" t="s">
+      <c r="F15" s="57" t="s">
         <v>199</v>
       </c>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="43"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="51"/>
+    <row r="16" spans="1:8" ht="15" customHeight="1">
+      <c r="A16" s="45"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="49"/>
       <c r="D16" s="2">
         <v>200437</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="54" t="s">
-        <v>199</v>
-      </c>
+      <c r="F16" s="57"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="43"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="51"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="49"/>
       <c r="D17" s="2">
         <v>310111</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="54"/>
+      <c r="F17" s="57"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="43"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="51"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="49"/>
       <c r="D18" s="2">
         <v>528401</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="54"/>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="43"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="51"/>
+      <c r="F18" s="57"/>
+    </row>
+    <row r="19" spans="1:14" ht="45">
+      <c r="A19" s="45"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="2">
         <v>1076753</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="54"/>
+      <c r="F19" s="31" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2"/>
@@ -4597,13 +4599,13 @@
       <c r="N24" s="12"/>
     </row>
     <row r="25" spans="1:14" ht="54" customHeight="1">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="C25" s="48" t="s">
+      <c r="C25" s="50" t="s">
         <v>95</v>
       </c>
       <c r="D25" s="5">
@@ -4616,9 +4618,9 @@
       <c r="N25" s="12"/>
     </row>
     <row r="26" spans="1:14" ht="54" customHeight="1">
-      <c r="A26" s="43"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="49"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="51"/>
       <c r="D26" s="5">
         <v>200437</v>
       </c>
@@ -4629,9 +4631,9 @@
       <c r="N26" s="12"/>
     </row>
     <row r="27" spans="1:14" ht="54" customHeight="1">
-      <c r="A27" s="43"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="49"/>
+      <c r="A27" s="45"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="51"/>
       <c r="D27" s="5">
         <v>310111</v>
       </c>
@@ -4642,9 +4644,9 @@
       <c r="N27" s="12"/>
     </row>
     <row r="28" spans="1:14" ht="54" customHeight="1">
-      <c r="A28" s="43"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="49"/>
+      <c r="A28" s="45"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="51"/>
       <c r="D28" s="5">
         <v>528401</v>
       </c>
@@ -4655,9 +4657,9 @@
       <c r="N28" s="12"/>
     </row>
     <row r="29" spans="1:14" ht="54" customHeight="1">
-      <c r="A29" s="43"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="49"/>
+      <c r="A29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="51"/>
       <c r="D29" s="5">
         <v>1076753</v>
       </c>
@@ -4669,18 +4671,18 @@
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="5"/>
-      <c r="B30" s="42"/>
+      <c r="B30" s="44"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="N30" s="12"/>
     </row>
     <row r="31" spans="1:14" ht="54" customHeight="1">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="42"/>
-      <c r="C31" s="48" t="s">
+      <c r="B31" s="44"/>
+      <c r="C31" s="50" t="s">
         <v>69</v>
       </c>
       <c r="D31" s="5">
@@ -4693,9 +4695,9 @@
       <c r="N31" s="12"/>
     </row>
     <row r="32" spans="1:14" ht="54" customHeight="1">
-      <c r="A32" s="43"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="49"/>
+      <c r="A32" s="45"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="51"/>
       <c r="D32" s="5">
         <v>200437</v>
       </c>
@@ -4706,9 +4708,9 @@
       <c r="N32" s="12"/>
     </row>
     <row r="33" spans="1:7" ht="54" customHeight="1">
-      <c r="A33" s="43"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="49"/>
+      <c r="A33" s="45"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="51"/>
       <c r="D33" s="5">
         <v>310111</v>
       </c>
@@ -4718,9 +4720,9 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="54" customHeight="1">
-      <c r="A34" s="43"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="49"/>
+      <c r="A34" s="45"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="51"/>
       <c r="D34" s="5">
         <v>528401</v>
       </c>
@@ -4730,9 +4732,9 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="54" customHeight="1">
-      <c r="A35" s="43"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="49"/>
+      <c r="A35" s="45"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="51"/>
       <c r="D35" s="5">
         <v>1076753</v>
       </c>
@@ -4772,7 +4774,17 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="23">
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="A3:A7"/>
@@ -4783,18 +4795,9 @@
     <mergeCell ref="B15:B19"/>
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="C15:C19"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
     <mergeCell ref="C9:C13"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="A9:A13"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="F16:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4830,12 +4833,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -5005,12 +5008,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -5052,10 +5055,10 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>136</v>
       </c>
       <c r="C3" s="40" t="s">
@@ -5064,87 +5067,87 @@
       <c r="D3" s="2">
         <v>145879</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="H3" s="44" t="s">
+      <c r="H3" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="I3" s="43" t="s">
+      <c r="I3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="55" t="s">
+      <c r="J3" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="45" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="45"/>
     </row>
     <row r="5" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="45"/>
     </row>
     <row r="6" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="45"/>
     </row>
     <row r="7" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="45"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="10"/>
@@ -5264,12 +5267,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -5311,13 +5314,13 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="45">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="51" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="10">
@@ -5346,11 +5349,11 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="56"/>
+      <c r="C4" s="55"/>
       <c r="D4" s="10">
         <v>200437</v>
       </c>
@@ -5371,9 +5374,9 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="56"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="55"/>
       <c r="D5" s="10">
         <v>310111</v>
       </c>
@@ -5394,9 +5397,9 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="56"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="55"/>
       <c r="D6" s="10">
         <v>528401</v>
       </c>
@@ -5417,9 +5420,9 @@
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="56"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="55"/>
       <c r="D7" s="10">
         <v>1076753</v>
       </c>
@@ -5514,13 +5517,13 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
       <c r="J1" s="10"/>
       <c r="K1" s="11"/>
       <c r="L1" s="10"/>
@@ -5564,10 +5567,10 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="45" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>136</v>
       </c>
       <c r="C3" s="40" t="s">
@@ -5588,22 +5591,22 @@
       <c r="H3" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="I3" s="57" t="s">
+      <c r="I3" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="J3" s="43" t="s">
+      <c r="J3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="55" t="s">
+      <c r="K3" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="43" t="s">
+      <c r="L3" s="45" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="45" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
@@ -5620,14 +5623,14 @@
       <c r="H4" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="I4" s="57"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="43"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="45"/>
     </row>
     <row r="5" spans="1:12" ht="45" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
@@ -5644,14 +5647,14 @@
       <c r="H5" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="I5" s="57"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="43"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="45"/>
     </row>
     <row r="6" spans="1:12" ht="45" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
@@ -5668,14 +5671,14 @@
       <c r="H6" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="I6" s="57"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="43"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="45"/>
     </row>
     <row r="7" spans="1:12" ht="45" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
@@ -5692,10 +5695,10 @@
       <c r="H7" s="31" t="s">
         <v>194</v>
       </c>
-      <c r="I7" s="57"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="43"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="45"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="10"/>

</xml_diff>

<commit_message>
Started re-running signeR for SBS_set1/Realistic, on HPC
</commit_message>
<xml_diff>
--- a/documents/CPU_timing/mSigHdp-paper-tracking.xlsx
+++ b/documents/CPU_timing/mSigHdp-paper-tracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\documents\CPU_timing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A2AB4A-D369-4022-B780-8352B2E8FE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4FABF1-2C25-4BDD-B545-AEC42A4A9C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11550" yWindow="1485" windowWidth="15615" windowHeight="13980" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8025" yWindow="225" windowWidth="15615" windowHeight="13980" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -177,7 +177,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="201">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -1257,6 +1257,11 @@
     <t>m2
 &lt;1811857&gt;
 (e0240162)</t>
+  </si>
+  <si>
+    <t>HPC
+(wuyang)
+&lt;137431&gt;</t>
   </si>
 </sst>
 </file>
@@ -1409,7 +1414,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1531,13 +1536,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1546,16 +1545,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1567,7 +1566,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -1579,7 +1587,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2118,40 +2126,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="50.1" customHeight="1">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="M1" s="42" t="s">
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="M1" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="F2" s="9">
         <v>5</v>
       </c>
@@ -2190,10 +2198,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="68.25" customHeight="1">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="42" t="s">
         <v>136</v>
       </c>
       <c r="C3" s="40" t="s">
@@ -2218,121 +2226,121 @@
       <c r="J3" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="M3" s="43" t="s">
+      <c r="M3" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="N3" s="43" t="s">
+      <c r="N3" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="O3" s="43" t="s">
+      <c r="O3" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="P3" s="43" t="s">
+      <c r="P3" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="Q3" s="43" t="s">
+      <c r="Q3" s="44" t="s">
         <v>127</v>
       </c>
-      <c r="R3" s="43" t="s">
+      <c r="R3" s="44" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="75" customHeight="1">
-      <c r="A4" s="45"/>
-      <c r="B4" s="52"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="50"/>
       <c r="C4" s="40"/>
       <c r="D4" s="10">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="J4" s="43" t="s">
+      <c r="J4" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="K4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="43"/>
+      <c r="K4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
     </row>
     <row r="5" spans="1:18" ht="36" customHeight="1">
-      <c r="A5" s="45"/>
-      <c r="B5" s="52"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="50"/>
       <c r="C5" s="40"/>
       <c r="D5" s="10">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="43"/>
-      <c r="R5" s="43"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="44"/>
     </row>
     <row r="6" spans="1:18" ht="36" customHeight="1">
-      <c r="A6" s="45"/>
-      <c r="B6" s="52"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="40"/>
       <c r="D6" s="10">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="43"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="44"/>
     </row>
     <row r="7" spans="1:18" ht="36" customHeight="1">
-      <c r="A7" s="45"/>
-      <c r="B7" s="52"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="40"/>
       <c r="D7" s="10">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="43"/>
-      <c r="R7" s="43"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="44"/>
+      <c r="R7" s="44"/>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="2"/>
@@ -2343,139 +2351,139 @@
       <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:18" ht="54" customHeight="1">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="51" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="10">
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="H9" s="43" t="s">
+      <c r="H9" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="I9" s="43" t="s">
+      <c r="I9" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="J9" s="43" t="s">
+      <c r="J9" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="43" t="s">
+      <c r="K9" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="M9" s="43" t="s">
+      <c r="M9" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="N9" s="43" t="s">
+      <c r="N9" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="O9" s="43" t="s">
+      <c r="O9" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="P9" s="43" t="s">
+      <c r="P9" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="Q9" s="43" t="s">
+      <c r="Q9" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="R9" s="43" t="s">
+      <c r="R9" s="44" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="54" customHeight="1">
-      <c r="A10" s="45"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="49"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
       <c r="D10" s="10">
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="43"/>
-      <c r="Q10" s="43"/>
-      <c r="R10" s="43"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="44"/>
     </row>
     <row r="11" spans="1:18" ht="54" customHeight="1">
-      <c r="A11" s="45"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="49"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
       <c r="D11" s="10">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="43"/>
-      <c r="Q11" s="43"/>
-      <c r="R11" s="43"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="44"/>
     </row>
     <row r="12" spans="1:18" ht="54" customHeight="1">
-      <c r="A12" s="45"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="49"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="10">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="43"/>
-      <c r="Q12" s="43"/>
-      <c r="R12" s="43"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+      <c r="M12" s="44"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="44"/>
+      <c r="Q12" s="44"/>
+      <c r="R12" s="44"/>
     </row>
     <row r="13" spans="1:18" ht="54" customHeight="1">
-      <c r="A13" s="45"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="49"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="10">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="43"/>
-      <c r="R13" s="43"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="44"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="44"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="5"/>
@@ -2509,6 +2517,28 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="M3:M7"/>
+    <mergeCell ref="N3:N7"/>
+    <mergeCell ref="O3:O7"/>
+    <mergeCell ref="P3:P7"/>
+    <mergeCell ref="M9:M13"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="N9:N13"/>
+    <mergeCell ref="O9:O13"/>
+    <mergeCell ref="P9:P13"/>
+    <mergeCell ref="Q9:Q13"/>
+    <mergeCell ref="R9:R13"/>
+    <mergeCell ref="Q3:Q7"/>
+    <mergeCell ref="R3:R7"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="K9:K13"/>
     <mergeCell ref="J9:J13"/>
@@ -2524,28 +2554,6 @@
     <mergeCell ref="K3:K7"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="H4:H7"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="P3:P7"/>
-    <mergeCell ref="M9:M13"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="N9:N13"/>
-    <mergeCell ref="O9:O13"/>
-    <mergeCell ref="P9:P13"/>
-    <mergeCell ref="Q9:Q13"/>
-    <mergeCell ref="R9:R13"/>
-    <mergeCell ref="Q3:Q7"/>
-    <mergeCell ref="R3:R7"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="M3:M7"/>
-    <mergeCell ref="N3:N7"/>
-    <mergeCell ref="O3:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2574,32 +2582,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:15" ht="45">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="F2" s="9" t="s">
         <v>38</v>
       </c>
@@ -2616,10 +2624,10 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="45" customHeight="1">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="42" t="s">
         <v>144</v>
       </c>
       <c r="C3" s="40" t="s">
@@ -2629,79 +2637,79 @@
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:15" ht="45" customHeight="1">
-      <c r="A4" s="45"/>
-      <c r="B4" s="44"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="45" customHeight="1">
-      <c r="A5" s="45"/>
-      <c r="B5" s="44"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="45" customHeight="1">
-      <c r="A6" s="45"/>
-      <c r="B6" s="44"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
       <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="43" t="s">
+      <c r="F6" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:15" ht="45" customHeight="1">
-      <c r="A7" s="45"/>
-      <c r="B7" s="44"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
       <c r="K7" s="2"/>
@@ -2733,11 +2741,11 @@
         <v>34</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
       <c r="J9" s="4"/>
       <c r="K9" s="5"/>
     </row>
@@ -2827,84 +2835,84 @@
       <c r="O14" s="34"/>
     </row>
     <row r="15" spans="1:15" ht="60" customHeight="1">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="45" t="s">
         <v>56</v>
       </c>
       <c r="D15" s="2">
         <v>145879</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="43" t="s">
+      <c r="F15" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
       <c r="O15" s="34"/>
     </row>
     <row r="16" spans="1:15" ht="60" customHeight="1">
-      <c r="A16" s="45"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="47"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="45"/>
       <c r="D16" s="2">
         <v>200437</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="43" t="s">
+      <c r="F16" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
       <c r="O16" s="34"/>
     </row>
     <row r="17" spans="1:15" ht="60" customHeight="1">
-      <c r="A17" s="45"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="47"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="45"/>
       <c r="D17" s="2">
         <v>310111</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="43" t="s">
+      <c r="F17" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
       <c r="O17" s="34"/>
     </row>
     <row r="18" spans="1:15" ht="60" customHeight="1">
-      <c r="A18" s="45"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="47"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="45"/>
       <c r="D18" s="2">
         <v>528401</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="43" t="s">
+      <c r="F18" s="44" t="s">
         <v>163</v>
       </c>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
       <c r="O18" s="34"/>
     </row>
     <row r="19" spans="1:15" ht="60" customHeight="1">
-      <c r="A19" s="45"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="47"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="45"/>
       <c r="D19" s="2">
         <v>1076753</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="43" t="s">
+      <c r="F19" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
       <c r="O19" s="34"/>
     </row>
     <row r="20" spans="1:15">
@@ -2924,7 +2932,7 @@
       <c r="A21" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="42" t="s">
         <v>176</v>
       </c>
       <c r="C21" s="18" t="s">
@@ -2945,7 +2953,7 @@
     </row>
     <row r="22" spans="1:15" ht="30" customHeight="1">
       <c r="A22" s="10"/>
-      <c r="B22" s="44"/>
+      <c r="B22" s="42"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -2955,11 +2963,11 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:15" ht="60" customHeight="1">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="46" t="s">
+      <c r="B23" s="42"/>
+      <c r="C23" s="41" t="s">
         <v>64</v>
       </c>
       <c r="D23" s="2">
@@ -2969,16 +2977,16 @@
       <c r="H23" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="I23" s="43" t="s">
+      <c r="I23" s="44" t="s">
         <v>181</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:15" ht="60" customHeight="1">
-      <c r="A24" s="45"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="46"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="41"/>
       <c r="D24" s="2">
         <v>200437</v>
       </c>
@@ -2986,14 +2994,14 @@
       <c r="H24" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="I24" s="43"/>
+      <c r="I24" s="44"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:15" ht="60" customHeight="1">
-      <c r="A25" s="45"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="46"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="41"/>
       <c r="D25" s="2">
         <v>310111</v>
       </c>
@@ -3001,14 +3009,14 @@
       <c r="H25" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="I25" s="43"/>
+      <c r="I25" s="44"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:15" ht="60" customHeight="1">
-      <c r="A26" s="45"/>
-      <c r="B26" s="44"/>
-      <c r="C26" s="46"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="41"/>
       <c r="D26" s="2">
         <v>528401</v>
       </c>
@@ -3016,14 +3024,14 @@
       <c r="H26" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="I26" s="43"/>
+      <c r="I26" s="44"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
     </row>
     <row r="27" spans="1:15" ht="60" customHeight="1">
-      <c r="A27" s="45"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="46"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="41"/>
       <c r="D27" s="2">
         <v>1076753</v>
       </c>
@@ -3031,7 +3039,7 @@
       <c r="H27" s="27" t="s">
         <v>188</v>
       </c>
-      <c r="I27" s="43"/>
+      <c r="I27" s="44"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
@@ -3075,17 +3083,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="B21:B27"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="I23:I27"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
     <mergeCell ref="A29:F29"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="A1:A2"/>
@@ -3102,6 +3099,17 @@
     <mergeCell ref="F18:H18"/>
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="B15:B19"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="B21:B27"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="I23:I27"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="C15:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3132,24 +3140,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="46.5" customHeight="1">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="47" t="s">
         <v>20</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -3158,10 +3166,10 @@
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14" ht="30.75" customHeight="1">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="1"/>
       <c r="F2" s="9" t="s">
         <v>39</v>
@@ -3363,7 +3371,7 @@
       <c r="A13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="42" t="s">
         <v>176</v>
       </c>
       <c r="C13" s="18" t="s">
@@ -3384,7 +3392,7 @@
     </row>
     <row r="14" spans="1:14" ht="45">
       <c r="A14" s="5"/>
-      <c r="B14" s="44"/>
+      <c r="B14" s="42"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -3403,18 +3411,18 @@
       <c r="N14" s="5"/>
     </row>
     <row r="15" spans="1:14" ht="54" customHeight="1">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="46" t="s">
+      <c r="B15" s="42"/>
+      <c r="C15" s="41" t="s">
         <v>65</v>
       </c>
       <c r="D15" s="5">
         <v>145879</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="43" t="s">
+      <c r="F15" s="44" t="s">
         <v>170</v>
       </c>
       <c r="H15" s="24" t="s">
@@ -3426,14 +3434,14 @@
       <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:14" ht="54" customHeight="1">
-      <c r="A16" s="45"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="46"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="41"/>
       <c r="D16" s="5">
         <v>200437</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="43"/>
+      <c r="F16" s="44"/>
       <c r="H16" s="24" t="s">
         <v>77</v>
       </c>
@@ -3443,14 +3451,14 @@
       <c r="N16" s="5"/>
     </row>
     <row r="17" spans="1:14" ht="54" customHeight="1">
-      <c r="A17" s="45"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="46"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="41"/>
       <c r="D17" s="5">
         <v>310111</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="43"/>
+      <c r="F17" s="44"/>
       <c r="H17" s="25" t="s">
         <v>82</v>
       </c>
@@ -3460,14 +3468,14 @@
       <c r="N17" s="5"/>
     </row>
     <row r="18" spans="1:14" ht="54" customHeight="1">
-      <c r="A18" s="45"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="46"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="41"/>
       <c r="D18" s="5">
         <v>528401</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="43"/>
+      <c r="F18" s="44"/>
       <c r="H18" s="25" t="s">
         <v>82</v>
       </c>
@@ -3477,14 +3485,14 @@
       <c r="N18" s="5"/>
     </row>
     <row r="19" spans="1:14" ht="54" customHeight="1">
-      <c r="A19" s="45"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="46"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="41"/>
       <c r="D19" s="5">
         <v>1076753</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="43"/>
+      <c r="F19" s="44"/>
       <c r="H19" s="25" t="s">
         <v>82</v>
       </c>
@@ -3549,16 +3557,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="F15:F19"/>
+    <mergeCell ref="B13:B19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="A15:A19"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="F15:F19"/>
-    <mergeCell ref="B13:B19"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="A15:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3571,10 +3579,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3586,29 +3594,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="F2" s="9" t="s">
         <v>38</v>
       </c>
@@ -3620,87 +3628,87 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="45">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="51" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="G3" s="48"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="39" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45">
-      <c r="A4" s="45"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="49"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="52" t="s">
         <v>155</v>
       </c>
-      <c r="G4" s="48"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="39" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45">
-      <c r="A5" s="45"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="49"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="51"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="52" t="s">
         <v>156</v>
       </c>
-      <c r="G5" s="48"/>
+      <c r="G5" s="52"/>
       <c r="H5" s="39" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45">
-      <c r="A6" s="45"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="49"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="G6" s="48"/>
+      <c r="G6" s="52"/>
       <c r="H6" s="39" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45">
-      <c r="A7" s="45"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="49"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="52" t="s">
         <v>158</v>
       </c>
-      <c r="G7" s="48"/>
+      <c r="G7" s="52"/>
       <c r="H7" s="39" t="s">
         <v>158</v>
       </c>
@@ -3713,10 +3721,10 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="45">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="42" t="s">
         <v>136</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -3726,10 +3734,10 @@
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="44" t="s">
         <v>86</v>
       </c>
       <c r="H9" s="27" t="s">
@@ -3737,57 +3745,57 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="36" customHeight="1">
-      <c r="A10" s="45"/>
-      <c r="B10" s="52"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="40"/>
       <c r="D10" s="2">
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
       <c r="H10" s="27" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="36" customHeight="1">
-      <c r="A11" s="45"/>
-      <c r="B11" s="52"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="40"/>
       <c r="D11" s="2">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
       <c r="H11" s="27" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="36" customHeight="1">
-      <c r="A12" s="45"/>
-      <c r="B12" s="52"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="40"/>
       <c r="D12" s="2">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
       <c r="H12" s="27" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="36" customHeight="1">
-      <c r="A13" s="45"/>
-      <c r="B13" s="52"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="40"/>
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
       <c r="H13" s="27" t="s">
         <v>79</v>
       </c>
@@ -3803,84 +3811,84 @@
       <c r="H14" s="29"/>
     </row>
     <row r="15" spans="1:8" ht="54" customHeight="1">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="51" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="2">
         <v>145879</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="43" t="s">
+      <c r="F15" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43" t="s">
+      <c r="G15" s="44"/>
+      <c r="H15" s="44" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="54" customHeight="1">
-      <c r="A16" s="45"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="49"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="51"/>
       <c r="D16" s="2">
         <v>200437</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="43" t="s">
+      <c r="F16" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
-    </row>
-    <row r="17" spans="1:8" ht="54" customHeight="1">
-      <c r="A17" s="45"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="49"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+    </row>
+    <row r="17" spans="1:9" ht="54" customHeight="1">
+      <c r="A17" s="43"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="51"/>
       <c r="D17" s="2">
         <v>310111</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="43" t="s">
+      <c r="F17" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-    </row>
-    <row r="18" spans="1:8" ht="54" customHeight="1">
-      <c r="A18" s="45"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="49"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+    </row>
+    <row r="18" spans="1:9" ht="54" customHeight="1">
+      <c r="A18" s="43"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="51"/>
       <c r="D18" s="2">
         <v>528401</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="43" t="s">
+      <c r="F18" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-    </row>
-    <row r="19" spans="1:8" ht="54" customHeight="1">
-      <c r="A19" s="45"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="49"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+    </row>
+    <row r="19" spans="1:9" ht="54" customHeight="1">
+      <c r="A19" s="43"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="51"/>
       <c r="D19" s="2">
         <v>1076753</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="43" t="s">
+      <c r="F19" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="2"/>
       <c r="B20" s="10"/>
       <c r="C20" s="2"/>
@@ -3889,14 +3897,14 @@
       <c r="F20" s="20"/>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:8" ht="60" customHeight="1">
-      <c r="A21" s="47" t="s">
+    <row r="21" spans="1:9" ht="60" customHeight="1">
+      <c r="A21" s="45" t="s">
         <v>195</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="C21" s="49"/>
+      <c r="C21" s="51"/>
       <c r="D21" s="2">
         <v>145879</v>
       </c>
@@ -3907,10 +3915,10 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="45">
-      <c r="A22" s="47"/>
-      <c r="B22" s="44"/>
-      <c r="C22" s="49"/>
+    <row r="22" spans="1:9" ht="45">
+      <c r="A22" s="45"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="51"/>
       <c r="D22" s="2">
         <v>200437</v>
       </c>
@@ -3921,10 +3929,10 @@
         <v>198</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="47"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="49"/>
+    <row r="23" spans="1:9">
+      <c r="A23" s="45"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="51"/>
       <c r="D23" s="2">
         <v>310111</v>
       </c>
@@ -3932,10 +3940,10 @@
       <c r="F23" s="20"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="47"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="49"/>
+    <row r="24" spans="1:9">
+      <c r="A24" s="45"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="51"/>
       <c r="D24" s="2">
         <v>528401</v>
       </c>
@@ -3943,10 +3951,10 @@
       <c r="F24" s="20"/>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="47"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="49"/>
+    <row r="25" spans="1:9">
+      <c r="A25" s="45"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="51"/>
       <c r="D25" s="2">
         <v>1076753</v>
       </c>
@@ -3954,16 +3962,26 @@
       <c r="F25" s="20"/>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:9" ht="45">
       <c r="A26" s="2"/>
       <c r="B26" s="10"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" spans="1:8" ht="30">
+      <c r="F26" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -3987,24 +4005,33 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9" ht="45">
       <c r="A28" s="2"/>
       <c r="B28" s="10"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-    </row>
-    <row r="29" spans="1:8" ht="45">
-      <c r="A29" s="47" t="s">
+      <c r="F28" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="60">
+      <c r="A29" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="C29" s="45" t="s">
+      <c r="C29" s="43" t="s">
         <v>54</v>
       </c>
       <c r="D29" s="5">
@@ -4013,63 +4040,70 @@
       <c r="E29" s="5"/>
       <c r="F29"/>
       <c r="G29"/>
-      <c r="H29" s="27" t="s">
+      <c r="H29" s="58" t="s">
+        <v>200</v>
+      </c>
+      <c r="I29" s="27" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="45">
-      <c r="A30" s="47"/>
-      <c r="B30" s="44"/>
-      <c r="C30" s="45"/>
+    <row r="30" spans="1:9" ht="60">
+      <c r="A30" s="45"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="43"/>
       <c r="D30" s="5">
         <v>200437</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30"/>
       <c r="G30"/>
-      <c r="H30" s="27" t="s">
+      <c r="H30" s="58"/>
+      <c r="I30" s="27" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="45" customHeight="1">
-      <c r="A31" s="47"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="45"/>
+    <row r="31" spans="1:9" ht="45" customHeight="1">
+      <c r="A31" s="45"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="43"/>
       <c r="D31" s="5">
         <v>310111</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31"/>
       <c r="G31"/>
-      <c r="H31" s="43" t="s">
+      <c r="H31" s="58"/>
+      <c r="I31" s="44" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="45" customHeight="1">
-      <c r="A32" s="47"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="45"/>
+    <row r="32" spans="1:9" ht="45" customHeight="1">
+      <c r="A32" s="45"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="43"/>
       <c r="D32" s="5">
         <v>528401</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32"/>
       <c r="G32"/>
-      <c r="H32" s="43"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="47"/>
-      <c r="B33" s="44"/>
-      <c r="C33" s="45"/>
+      <c r="H32"/>
+      <c r="I32" s="44"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="45"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="43"/>
       <c r="D33" s="5">
         <v>1076753</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33"/>
       <c r="G33"/>
-      <c r="H33" s="43"/>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="H33"/>
+      <c r="I33" s="44"/>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="5"/>
       <c r="B34" s="10"/>
       <c r="C34" s="5"/>
@@ -4079,14 +4113,14 @@
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
     </row>
-    <row r="35" spans="1:8" ht="54" customHeight="1">
-      <c r="A35" s="47" t="s">
+    <row r="35" spans="1:9" ht="54" customHeight="1">
+      <c r="A35" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="44" t="s">
+      <c r="B35" s="42" t="s">
         <v>176</v>
       </c>
-      <c r="C35" s="50" t="s">
+      <c r="C35" s="48" t="s">
         <v>63</v>
       </c>
       <c r="D35" s="5">
@@ -4099,10 +4133,10 @@
         <v>110</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="54" customHeight="1">
-      <c r="A36" s="47"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="51"/>
+    <row r="36" spans="1:9" ht="54" customHeight="1">
+      <c r="A36" s="45"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="49"/>
       <c r="D36" s="5">
         <v>200437</v>
       </c>
@@ -4113,10 +4147,10 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="54" customHeight="1">
-      <c r="A37" s="47"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="51"/>
+    <row r="37" spans="1:9" ht="54" customHeight="1">
+      <c r="A37" s="45"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="49"/>
       <c r="D37" s="5">
         <v>310111</v>
       </c>
@@ -4127,10 +4161,10 @@
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="54" customHeight="1">
-      <c r="A38" s="47"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="51"/>
+    <row r="38" spans="1:9" ht="54" customHeight="1">
+      <c r="A38" s="45"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="49"/>
       <c r="D38" s="5">
         <v>528401</v>
       </c>
@@ -4141,10 +4175,10 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="54" customHeight="1">
-      <c r="A39" s="47"/>
-      <c r="B39" s="44"/>
-      <c r="C39" s="51"/>
+    <row r="39" spans="1:9" ht="54" customHeight="1">
+      <c r="A39" s="45"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="49"/>
       <c r="D39" s="5">
         <v>1076753</v>
       </c>
@@ -4155,9 +4189,9 @@
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:9">
       <c r="A40" s="5"/>
-      <c r="B40" s="44"/>
+      <c r="B40" s="42"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -4165,11 +4199,11 @@
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
     </row>
-    <row r="41" spans="1:8" ht="270" customHeight="1">
+    <row r="41" spans="1:9" ht="270" customHeight="1">
       <c r="A41" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="44"/>
+      <c r="B41" s="42"/>
       <c r="C41" s="19" t="s">
         <v>70</v>
       </c>
@@ -4183,7 +4217,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:9">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -4193,7 +4227,7 @@
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:9">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -4203,7 +4237,7 @@
       <c r="G43" s="10"/>
       <c r="H43" s="10"/>
     </row>
-    <row r="44" spans="1:8" ht="94.5" customHeight="1">
+    <row r="44" spans="1:9" ht="94.5" customHeight="1">
       <c r="A44" s="40" t="s">
         <v>135</v>
       </c>
@@ -4213,23 +4247,46 @@
       <c r="E44" s="40"/>
       <c r="F44" s="40"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:9">
       <c r="A46" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>137</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="39">
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H15:H19"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="G9:G13"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="A44:F44"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="B35:B41"/>
@@ -4246,28 +4303,6 @@
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="F9:F13"/>
-    <mergeCell ref="G9:G13"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="H31:H33"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H15:H19"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4282,7 +4317,7 @@
   </sheetPr>
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -4296,29 +4331,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="49.5" customHeight="1">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="47" t="s">
         <v>20</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="42"/>
+      <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="41"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="1"/>
       <c r="F2" s="9" t="s">
         <v>39</v>
@@ -4328,10 +4363,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="36" customHeight="1">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="42" t="s">
         <v>136</v>
       </c>
       <c r="C3" s="40" t="s">
@@ -4346,8 +4381,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="36" customHeight="1">
-      <c r="A4" s="45"/>
-      <c r="B4" s="44"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
@@ -4358,8 +4393,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="36" customHeight="1">
-      <c r="A5" s="45"/>
-      <c r="B5" s="44"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
@@ -4370,8 +4405,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="36" customHeight="1">
-      <c r="A6" s="45"/>
-      <c r="B6" s="44"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
       <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
@@ -4382,8 +4417,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1">
-      <c r="A7" s="45"/>
-      <c r="B7" s="44"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
@@ -4400,13 +4435,13 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="45" customHeight="1">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="51" t="s">
         <v>46</v>
       </c>
       <c r="D9" s="2">
@@ -4420,9 +4455,9 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="45" customHeight="1">
-      <c r="A10" s="45"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="49"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="51"/>
       <c r="D10" s="2">
         <v>200437</v>
       </c>
@@ -4431,9 +4466,9 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="45" customHeight="1">
-      <c r="A11" s="45"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="49"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="51"/>
       <c r="D11" s="2">
         <v>310111</v>
       </c>
@@ -4443,28 +4478,28 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="45" customHeight="1">
-      <c r="A12" s="45"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="49"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="2">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="57" t="s">
+      <c r="F12" s="54" t="s">
         <v>189</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="45" customHeight="1">
-      <c r="A13" s="45"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="49"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="57"/>
+      <c r="F13" s="54"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:8">
@@ -4476,56 +4511,56 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="43" t="s">
         <v>195</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="C15" s="49"/>
+      <c r="C15" s="51"/>
       <c r="D15" s="2">
         <v>145879</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="57" t="s">
+      <c r="F15" s="54" t="s">
         <v>199</v>
       </c>
       <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1">
-      <c r="A16" s="45"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="49"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="51"/>
       <c r="D16" s="2">
         <v>200437</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="57"/>
+      <c r="F16" s="54"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="45"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="49"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="51"/>
       <c r="D17" s="2">
         <v>310111</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="57"/>
+      <c r="F17" s="54"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="45"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="49"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="51"/>
       <c r="D18" s="2">
         <v>528401</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="57"/>
+      <c r="F18" s="54"/>
     </row>
     <row r="19" spans="1:14" ht="45">
-      <c r="A19" s="45"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="49"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="51"/>
       <c r="D19" s="2">
         <v>1076753</v>
       </c>
@@ -4599,13 +4634,13 @@
       <c r="N24" s="12"/>
     </row>
     <row r="25" spans="1:14" ht="54" customHeight="1">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="42" t="s">
         <v>176</v>
       </c>
-      <c r="C25" s="50" t="s">
+      <c r="C25" s="48" t="s">
         <v>95</v>
       </c>
       <c r="D25" s="5">
@@ -4618,9 +4653,9 @@
       <c r="N25" s="12"/>
     </row>
     <row r="26" spans="1:14" ht="54" customHeight="1">
-      <c r="A26" s="45"/>
-      <c r="B26" s="44"/>
-      <c r="C26" s="51"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="5">
         <v>200437</v>
       </c>
@@ -4631,9 +4666,9 @@
       <c r="N26" s="12"/>
     </row>
     <row r="27" spans="1:14" ht="54" customHeight="1">
-      <c r="A27" s="45"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="51"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="49"/>
       <c r="D27" s="5">
         <v>310111</v>
       </c>
@@ -4644,9 +4679,9 @@
       <c r="N27" s="12"/>
     </row>
     <row r="28" spans="1:14" ht="54" customHeight="1">
-      <c r="A28" s="45"/>
-      <c r="B28" s="44"/>
-      <c r="C28" s="51"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="49"/>
       <c r="D28" s="5">
         <v>528401</v>
       </c>
@@ -4657,9 +4692,9 @@
       <c r="N28" s="12"/>
     </row>
     <row r="29" spans="1:14" ht="54" customHeight="1">
-      <c r="A29" s="45"/>
-      <c r="B29" s="44"/>
-      <c r="C29" s="51"/>
+      <c r="A29" s="43"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="49"/>
       <c r="D29" s="5">
         <v>1076753</v>
       </c>
@@ -4671,18 +4706,18 @@
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="5"/>
-      <c r="B30" s="44"/>
+      <c r="B30" s="42"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="N30" s="12"/>
     </row>
     <row r="31" spans="1:14" ht="54" customHeight="1">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="44"/>
-      <c r="C31" s="50" t="s">
+      <c r="B31" s="42"/>
+      <c r="C31" s="48" t="s">
         <v>69</v>
       </c>
       <c r="D31" s="5">
@@ -4695,9 +4730,9 @@
       <c r="N31" s="12"/>
     </row>
     <row r="32" spans="1:14" ht="54" customHeight="1">
-      <c r="A32" s="45"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="51"/>
+      <c r="A32" s="43"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="49"/>
       <c r="D32" s="5">
         <v>200437</v>
       </c>
@@ -4708,9 +4743,9 @@
       <c r="N32" s="12"/>
     </row>
     <row r="33" spans="1:7" ht="54" customHeight="1">
-      <c r="A33" s="45"/>
-      <c r="B33" s="44"/>
-      <c r="C33" s="51"/>
+      <c r="A33" s="43"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="49"/>
       <c r="D33" s="5">
         <v>310111</v>
       </c>
@@ -4720,9 +4755,9 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="54" customHeight="1">
-      <c r="A34" s="45"/>
-      <c r="B34" s="44"/>
-      <c r="C34" s="51"/>
+      <c r="A34" s="43"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="49"/>
       <c r="D34" s="5">
         <v>528401</v>
       </c>
@@ -4732,9 +4767,9 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="54" customHeight="1">
-      <c r="A35" s="45"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="51"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="49"/>
       <c r="D35" s="5">
         <v>1076753</v>
       </c>
@@ -4775,16 +4810,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="A3:A7"/>
@@ -4798,6 +4823,16 @@
     <mergeCell ref="C9:C13"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="A9:A13"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F15:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4833,12 +4868,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -5008,12 +5043,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -5055,10 +5090,10 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="42" t="s">
         <v>136</v>
       </c>
       <c r="C3" s="40" t="s">
@@ -5067,87 +5102,87 @@
       <c r="D3" s="2">
         <v>145879</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="44" t="s">
         <v>183</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="44" t="s">
         <v>183</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="44" t="s">
         <v>183</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="44" t="s">
         <v>183</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="I3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="45" t="s">
+      <c r="K3" s="43" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A4" s="45"/>
-      <c r="B4" s="44"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="45"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="43"/>
     </row>
     <row r="5" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A5" s="45"/>
-      <c r="B5" s="44"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="45"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="43"/>
     </row>
     <row r="6" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A6" s="45"/>
-      <c r="B6" s="44"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
       <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="45"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="43"/>
     </row>
     <row r="7" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A7" s="45"/>
-      <c r="B7" s="44"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="45"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="43"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="10"/>
@@ -5267,12 +5302,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -5314,13 +5349,13 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="45">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="49" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="10">
@@ -5349,11 +5384,11 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1">
-      <c r="A4" s="45"/>
-      <c r="B4" s="44" t="s">
+      <c r="A4" s="43"/>
+      <c r="B4" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="55"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="10">
         <v>200437</v>
       </c>
@@ -5374,9 +5409,9 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1">
-      <c r="A5" s="45"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="55"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="56"/>
       <c r="D5" s="10">
         <v>310111</v>
       </c>
@@ -5397,9 +5432,9 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
-      <c r="A6" s="45"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="55"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="10">
         <v>528401</v>
       </c>
@@ -5420,9 +5455,9 @@
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
-      <c r="A7" s="45"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="55"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="56"/>
       <c r="D7" s="10">
         <v>1076753</v>
       </c>
@@ -5517,13 +5552,13 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
       <c r="J1" s="10"/>
       <c r="K1" s="11"/>
       <c r="L1" s="10"/>
@@ -5567,10 +5602,10 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="45" customHeight="1">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="42" t="s">
         <v>136</v>
       </c>
       <c r="C3" s="40" t="s">
@@ -5591,22 +5626,22 @@
       <c r="H3" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="I3" s="56" t="s">
+      <c r="I3" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="54" t="s">
+      <c r="K3" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="45" t="s">
+      <c r="L3" s="43" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="45" customHeight="1">
-      <c r="A4" s="45"/>
-      <c r="B4" s="44"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
@@ -5623,14 +5658,14 @@
       <c r="H4" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="I4" s="56"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="45"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="43"/>
     </row>
     <row r="5" spans="1:12" ht="45" customHeight="1">
-      <c r="A5" s="45"/>
-      <c r="B5" s="44"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
@@ -5647,14 +5682,14 @@
       <c r="H5" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="I5" s="56"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="45"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="43"/>
     </row>
     <row r="6" spans="1:12" ht="45" customHeight="1">
-      <c r="A6" s="45"/>
-      <c r="B6" s="44"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
       <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
@@ -5671,14 +5706,14 @@
       <c r="H6" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="I6" s="56"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="45"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="43"/>
     </row>
     <row r="7" spans="1:12" ht="45" customHeight="1">
-      <c r="A7" s="45"/>
-      <c r="B7" s="44"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
@@ -5695,10 +5730,10 @@
       <c r="H7" s="31" t="s">
         <v>194</v>
       </c>
-      <c r="I7" s="56"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="45"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="43"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="10"/>

</xml_diff>

<commit_message>
Finished running SP_default on SBS_set2/Realistic
</commit_message>
<xml_diff>
--- a/documents/CPU_timing/mSigHdp-paper-tracking.xlsx
+++ b/documents/CPU_timing/mSigHdp-paper-tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\documents\CPU_timing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4FABF1-2C25-4BDD-B545-AEC42A4A9C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427FAD5C-D5AF-4C56-B7E2-A9A20BE791E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8025" yWindow="225" windowWidth="15615" windowHeight="13980" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -177,7 +177,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="201">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -644,9 +644,6 @@
     <t>mSigHdp_ds_3k</t>
   </si>
   <si>
-    <t>hpc (e0240162)</t>
-  </si>
-  <si>
     <t>10k-rerun</t>
   </si>
   <si>
@@ -1262,6 +1259,11 @@
     <t>HPC
 (wuyang)
 &lt;137431&gt;</t>
+  </si>
+  <si>
+    <t>m2
+&lt;2058488&gt;
+(e0240162)</t>
   </si>
 </sst>
 </file>
@@ -1414,7 +1416,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1536,7 +1538,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1545,16 +1553,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1566,16 +1577,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -1585,9 +1587,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2114,7 +2113,7 @@
   </sheetPr>
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N3" sqref="N3:N7"/>
     </sheetView>
   </sheetViews>
@@ -2126,40 +2125,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="50.1" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="M1" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="M1" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
       <c r="F2" s="9">
         <v>5</v>
       </c>
@@ -2198,11 +2197,11 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="68.25" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="42" t="s">
-        <v>136</v>
+      <c r="B3" s="44" t="s">
+        <v>135</v>
       </c>
       <c r="C3" s="40" t="s">
         <v>71</v>
@@ -2212,135 +2211,135 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="H3" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="I3" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="27" t="s">
-        <v>90</v>
-      </c>
       <c r="J3" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="K3" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="M3" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="K3" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="M3" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="N3" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="O3" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="P3" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="N3" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="O3" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="P3" s="44" t="s">
+      <c r="Q3" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="Q3" s="44" t="s">
+      <c r="R3" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="R3" s="44" t="s">
-        <v>128</v>
-      </c>
     </row>
     <row r="4" spans="1:18" ht="75" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="50"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="53"/>
       <c r="C4" s="40"/>
       <c r="D4" s="10">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="G4" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="H4" s="44" t="s">
+      <c r="F4" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="I4" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="I4" s="44" t="s">
+      <c r="J4" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="J4" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="K4" s="44"/>
-      <c r="M4" s="44"/>
-      <c r="N4" s="44"/>
-      <c r="O4" s="44"/>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="44"/>
-      <c r="R4" s="44"/>
+      <c r="K4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
     </row>
     <row r="5" spans="1:18" ht="36" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="50"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="53"/>
       <c r="C5" s="40"/>
       <c r="D5" s="10">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
     </row>
     <row r="6" spans="1:18" ht="36" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="50"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="40"/>
       <c r="D6" s="10">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="44"/>
-      <c r="P6" s="44"/>
-      <c r="Q6" s="44"/>
-      <c r="R6" s="44"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
     </row>
     <row r="7" spans="1:18" ht="36" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="50"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="53"/>
       <c r="C7" s="40"/>
       <c r="D7" s="10">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="M7" s="44"/>
-      <c r="N7" s="44"/>
-      <c r="O7" s="44"/>
-      <c r="P7" s="44"/>
-      <c r="Q7" s="44"/>
-      <c r="R7" s="44"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="43"/>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="2"/>
@@ -2351,139 +2350,139 @@
       <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:18" ht="54" customHeight="1">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="51" t="s">
+      <c r="B9" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="50" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="10">
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="G9" s="44" t="s">
+      <c r="H9" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="H9" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="I9" s="44" t="s">
+      <c r="I9" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="J9" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="J9" s="44" t="s">
-        <v>108</v>
-      </c>
-      <c r="K9" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="M9" s="44" t="s">
+      <c r="K9" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="M9" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="N9" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="N9" s="44" t="s">
+      <c r="O9" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="O9" s="44" t="s">
+      <c r="P9" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="P9" s="44" t="s">
+      <c r="Q9" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="Q9" s="44" t="s">
+      <c r="R9" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="R9" s="44" t="s">
-        <v>134</v>
-      </c>
     </row>
     <row r="10" spans="1:18" ht="54" customHeight="1">
-      <c r="A10" s="43"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="51"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="50"/>
       <c r="D10" s="10">
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="44"/>
-      <c r="Q10" s="44"/>
-      <c r="R10" s="44"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
     </row>
     <row r="11" spans="1:18" ht="54" customHeight="1">
-      <c r="A11" s="43"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="51"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="10">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="44"/>
-      <c r="O11" s="44"/>
-      <c r="P11" s="44"/>
-      <c r="Q11" s="44"/>
-      <c r="R11" s="44"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
     </row>
     <row r="12" spans="1:18" ht="54" customHeight="1">
-      <c r="A12" s="43"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="51"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="10">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="44"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="44"/>
-      <c r="R12" s="44"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
     </row>
     <row r="13" spans="1:18" ht="54" customHeight="1">
-      <c r="A13" s="43"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="10">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="44"/>
-      <c r="O13" s="44"/>
-      <c r="P13" s="44"/>
-      <c r="Q13" s="44"/>
-      <c r="R13" s="44"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="43"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="5"/>
@@ -2497,7 +2496,7 @@
     </row>
     <row r="15" spans="1:18" ht="94.5" customHeight="1">
       <c r="A15" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B15" s="40"/>
       <c r="C15" s="40"/>
@@ -2517,28 +2516,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="M3:M7"/>
-    <mergeCell ref="N3:N7"/>
-    <mergeCell ref="O3:O7"/>
-    <mergeCell ref="P3:P7"/>
-    <mergeCell ref="M9:M13"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="N9:N13"/>
-    <mergeCell ref="O9:O13"/>
-    <mergeCell ref="P9:P13"/>
-    <mergeCell ref="Q9:Q13"/>
-    <mergeCell ref="R9:R13"/>
-    <mergeCell ref="Q3:Q7"/>
-    <mergeCell ref="R3:R7"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="K9:K13"/>
     <mergeCell ref="J9:J13"/>
@@ -2554,6 +2531,28 @@
     <mergeCell ref="K3:K7"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="H4:H7"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="P3:P7"/>
+    <mergeCell ref="M9:M13"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="N9:N13"/>
+    <mergeCell ref="O9:O13"/>
+    <mergeCell ref="P9:P13"/>
+    <mergeCell ref="Q9:Q13"/>
+    <mergeCell ref="R9:R13"/>
+    <mergeCell ref="Q3:Q7"/>
+    <mergeCell ref="R3:R7"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="M3:M7"/>
+    <mergeCell ref="N3:N7"/>
+    <mergeCell ref="O3:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2566,10 +2565,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2582,32 +2581,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:15" ht="45">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
       <c r="F2" s="9" t="s">
         <v>38</v>
       </c>
@@ -2618,17 +2617,17 @@
         <v>39</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="45" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="42" t="s">
-        <v>144</v>
+      <c r="B3" s="44" t="s">
+        <v>143</v>
       </c>
       <c r="C3" s="40" t="s">
         <v>50</v>
@@ -2637,79 +2636,79 @@
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="44" t="s">
-        <v>147</v>
-      </c>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
+      <c r="F3" s="43" t="s">
+        <v>146</v>
+      </c>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:15" ht="45" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
+      <c r="F4" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="45" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="44" t="s">
-        <v>149</v>
-      </c>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
+      <c r="F5" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="45" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="44" t="s">
-        <v>150</v>
-      </c>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
+      <c r="F6" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:15" ht="45" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="44" t="s">
-        <v>151</v>
-      </c>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
+      <c r="F7" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
       <c r="K7" s="2"/>
@@ -2732,7 +2731,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>44</v>
@@ -2741,11 +2740,11 @@
         <v>34</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="44" t="s">
-        <v>145</v>
-      </c>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
+      <c r="F9" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
       <c r="J9" s="4"/>
       <c r="K9" s="5"/>
     </row>
@@ -2761,29 +2760,31 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:15" ht="90" customHeight="1">
-      <c r="A11" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>138</v>
-      </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="2" t="s">
-        <v>34</v>
+      <c r="A11" s="45" t="s">
+        <v>194</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="50"/>
+      <c r="D11" s="2">
+        <v>145879</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G11" s="5"/>
       <c r="J11" s="4"/>
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="2">
+        <v>200437</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="4"/>
       <c r="G12" s="5"/>
@@ -2792,298 +2793,370 @@
       <c r="K12" s="5"/>
       <c r="O12" s="34"/>
     </row>
-    <row r="13" spans="1:15" ht="45">
-      <c r="A13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>34</v>
+    <row r="13" spans="1:15">
+      <c r="A13" s="45"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="2">
+        <v>310111</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="G13" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="H13" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="I13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
+      <c r="I13" s="2"/>
       <c r="J13" s="4"/>
       <c r="K13" s="5"/>
       <c r="O13" s="34"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="A14" s="45"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="2">
+        <v>528401</v>
+      </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
       <c r="I14" s="2"/>
       <c r="J14" s="4"/>
       <c r="K14" s="5"/>
       <c r="O14" s="34"/>
     </row>
-    <row r="15" spans="1:15" ht="60" customHeight="1">
-      <c r="A15" s="43" t="s">
+    <row r="15" spans="1:15">
+      <c r="A15" s="45"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="2">
+        <v>1076753</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="5"/>
+      <c r="O15" s="34"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="5"/>
+      <c r="O16" s="34"/>
+    </row>
+    <row r="17" spans="1:15" ht="45">
+      <c r="A17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="5"/>
+      <c r="O17" s="34"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="5"/>
+      <c r="O18" s="34"/>
+    </row>
+    <row r="19" spans="1:15" ht="60" customHeight="1">
+      <c r="A19" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="42" t="s">
-        <v>165</v>
-      </c>
-      <c r="C15" s="45" t="s">
+      <c r="B19" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D19" s="2">
         <v>145879</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="44" t="s">
+      <c r="E19" s="5"/>
+      <c r="F19" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="O19" s="34"/>
+    </row>
+    <row r="20" spans="1:15" ht="60" customHeight="1">
+      <c r="A20" s="45"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="2">
+        <v>200437</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="43" t="s">
         <v>160</v>
       </c>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="O15" s="34"/>
-    </row>
-    <row r="16" spans="1:15" ht="60" customHeight="1">
-      <c r="A16" s="43"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="2">
-        <v>200437</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="44" t="s">
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="O20" s="34"/>
+    </row>
+    <row r="21" spans="1:15" ht="60" customHeight="1">
+      <c r="A21" s="45"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="2">
+        <v>310111</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="O16" s="34"/>
-    </row>
-    <row r="17" spans="1:15" ht="60" customHeight="1">
-      <c r="A17" s="43"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="2">
-        <v>310111</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="44" t="s">
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="O21" s="34"/>
+    </row>
+    <row r="22" spans="1:15" ht="60" customHeight="1">
+      <c r="A22" s="45"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="2">
+        <v>528401</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="O17" s="34"/>
-    </row>
-    <row r="18" spans="1:15" ht="60" customHeight="1">
-      <c r="A18" s="43"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="2">
-        <v>528401</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="44" t="s">
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="O22" s="34"/>
+    </row>
+    <row r="23" spans="1:15" ht="60" customHeight="1">
+      <c r="A23" s="45"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="2">
+        <v>1076753</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="43" t="s">
         <v>163</v>
       </c>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="O18" s="34"/>
-    </row>
-    <row r="19" spans="1:15" ht="60" customHeight="1">
-      <c r="A19" s="43"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="2">
-        <v>1076753</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="44" t="s">
-        <v>164</v>
-      </c>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="O19" s="34"/>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-    </row>
-    <row r="21" spans="1:15" ht="270" customHeight="1">
-      <c r="A21" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="42" t="s">
-        <v>176</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-    </row>
-    <row r="22" spans="1:15" ht="30" customHeight="1">
-      <c r="A22" s="10"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-    </row>
-    <row r="23" spans="1:15" ht="60" customHeight="1">
-      <c r="A23" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="42"/>
-      <c r="C23" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="2">
-        <v>145879</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="H23" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="I23" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-    </row>
-    <row r="24" spans="1:15" ht="60" customHeight="1">
-      <c r="A24" s="43"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="2">
-        <v>200437</v>
-      </c>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="O23" s="34"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-      <c r="H24" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="I24" s="44"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:15" ht="60" customHeight="1">
-      <c r="A25" s="43"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="2">
-        <v>310111</v>
+    <row r="25" spans="1:15" ht="270" customHeight="1">
+      <c r="A25" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
       <c r="H25" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="I25" s="44"/>
+        <v>180</v>
+      </c>
+      <c r="I25" s="2"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" spans="1:15" ht="60" customHeight="1">
-      <c r="A26" s="43"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="2">
-        <v>528401</v>
-      </c>
+    <row r="26" spans="1:15" ht="30" customHeight="1">
+      <c r="A26" s="10"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="5"/>
-      <c r="H26" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="I26" s="44"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
     </row>
     <row r="27" spans="1:15" ht="60" customHeight="1">
-      <c r="A27" s="43"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="41"/>
+      <c r="A27" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="44"/>
+      <c r="C27" s="46" t="s">
+        <v>64</v>
+      </c>
       <c r="D27" s="2">
-        <v>1076753</v>
+        <v>145879</v>
       </c>
       <c r="E27" s="5"/>
       <c r="H27" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="I27" s="44"/>
+        <v>183</v>
+      </c>
+      <c r="I27" s="43" t="s">
+        <v>180</v>
+      </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="5"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+    <row r="28" spans="1:15" ht="60" customHeight="1">
+      <c r="A28" s="45"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="2">
+        <v>200437</v>
+      </c>
       <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
+      <c r="H28" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="I28" s="43"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:15" ht="75" customHeight="1">
-      <c r="A29" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
+    <row r="29" spans="1:15" ht="60" customHeight="1">
+      <c r="A29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="2">
+        <v>310111</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="H29" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="I29" s="43"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
-    <row r="30" spans="1:15">
-      <c r="A30" t="s">
+    <row r="30" spans="1:15" ht="60" customHeight="1">
+      <c r="A30" s="45"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="2">
+        <v>528401</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="H30" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="I30" s="43"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+    </row>
+    <row r="31" spans="1:15" ht="60" customHeight="1">
+      <c r="A31" s="45"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="2">
+        <v>1076753</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="H31" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="I31" s="43"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="5"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+    </row>
+    <row r="33" spans="1:11" ht="75" customHeight="1">
+      <c r="A33" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
-      <c r="A31" s="5" t="s">
+    <row r="35" spans="1:11">
+      <c r="A35" s="5" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="A29:F29"/>
+  <mergeCells count="30">
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="A33:F33"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -3095,21 +3168,10 @@
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="B21:B27"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="I23:I27"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="B19:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3123,8 +3185,8 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3140,24 +3202,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="46.5" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="42" t="s">
         <v>20</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -3166,16 +3228,16 @@
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14" ht="30.75" customHeight="1">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="1"/>
       <c r="F2" s="9" t="s">
         <v>39</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>38</v>
@@ -3192,7 +3254,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>49</v>
@@ -3202,13 +3264,13 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I3" s="2"/>
       <c r="N3" s="2"/>
@@ -3230,7 +3292,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>45</v>
@@ -3240,7 +3302,7 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G5" s="26" t="s">
         <v>21</v>
@@ -3262,18 +3324,18 @@
     </row>
     <row r="7" spans="1:14" ht="75">
       <c r="A7" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="27" t="s">
-        <v>196</v>
+      <c r="F7" s="28" t="s">
+        <v>195</v>
       </c>
       <c r="I7" s="5"/>
       <c r="N7" s="5"/>
@@ -3301,10 +3363,10 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N9" s="5"/>
     </row>
@@ -3318,13 +3380,13 @@
         <v>39</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>38</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N10" s="5"/>
     </row>
@@ -3343,16 +3405,16 @@
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G11" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="H11" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="H11" s="31" t="s">
-        <v>173</v>
-      </c>
       <c r="I11" s="33" t="s">
-        <v>22</v>
+        <v>168</v>
       </c>
       <c r="N11" s="5"/>
     </row>
@@ -3371,8 +3433,8 @@
       <c r="A13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="42" t="s">
-        <v>176</v>
+      <c r="B13" s="44" t="s">
+        <v>175</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>66</v>
@@ -3382,17 +3444,17 @@
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H13" s="28" t="s">
-        <v>73</v>
+        <v>169</v>
       </c>
       <c r="I13" s="10"/>
       <c r="N13" s="5"/>
     </row>
     <row r="14" spans="1:14" ht="45">
       <c r="A14" s="5"/>
-      <c r="B14" s="42"/>
+      <c r="B14" s="44"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -3400,33 +3462,33 @@
         <v>39</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>38</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N14" s="5"/>
     </row>
     <row r="15" spans="1:14" ht="54" customHeight="1">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="41" t="s">
+      <c r="B15" s="44"/>
+      <c r="C15" s="46" t="s">
         <v>65</v>
       </c>
       <c r="D15" s="5">
         <v>145879</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="44" t="s">
-        <v>170</v>
+      <c r="F15" s="43" t="s">
+        <v>169</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I15" s="16" t="s">
         <v>22</v>
@@ -3434,16 +3496,16 @@
       <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:14" ht="54" customHeight="1">
-      <c r="A16" s="43"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="41"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="5">
         <v>200437</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="44"/>
+      <c r="F16" s="43"/>
       <c r="H16" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I16" s="16" t="s">
         <v>22</v>
@@ -3451,16 +3513,16 @@
       <c r="N16" s="5"/>
     </row>
     <row r="17" spans="1:14" ht="54" customHeight="1">
-      <c r="A17" s="43"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="41"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="46"/>
       <c r="D17" s="5">
         <v>310111</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="44"/>
+      <c r="F17" s="43"/>
       <c r="H17" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I17" s="21" t="s">
         <v>22</v>
@@ -3468,16 +3530,16 @@
       <c r="N17" s="5"/>
     </row>
     <row r="18" spans="1:14" ht="54" customHeight="1">
-      <c r="A18" s="43"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="41"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="46"/>
       <c r="D18" s="5">
         <v>528401</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="44"/>
+      <c r="F18" s="43"/>
       <c r="H18" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>22</v>
@@ -3485,16 +3547,16 @@
       <c r="N18" s="5"/>
     </row>
     <row r="19" spans="1:14" ht="54" customHeight="1">
-      <c r="A19" s="43"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="41"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="46"/>
       <c r="D19" s="5">
         <v>1076753</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="44"/>
+      <c r="F19" s="43"/>
       <c r="H19" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I19" s="21" t="s">
         <v>22</v>
@@ -3535,7 +3597,7 @@
     </row>
     <row r="22" spans="1:14" ht="105" customHeight="1">
       <c r="A22" s="40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="40"/>
       <c r="C22" s="40"/>
@@ -3557,16 +3619,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="F15:F19"/>
     <mergeCell ref="B13:B19"/>
     <mergeCell ref="C15:C19"/>
     <mergeCell ref="A15:A19"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3581,8 +3643,8 @@
   </sheetPr>
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3594,29 +3656,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
       <c r="F2" s="9" t="s">
         <v>38</v>
       </c>
@@ -3628,89 +3690,89 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="45">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" s="51" t="s">
+      <c r="B3" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="50" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="52" t="s">
-        <v>154</v>
-      </c>
-      <c r="G3" s="52"/>
+      <c r="F3" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" s="48"/>
       <c r="H3" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="51"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="52" t="s">
-        <v>155</v>
-      </c>
-      <c r="G4" s="52"/>
+      <c r="F4" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="G4" s="48"/>
       <c r="H4" s="39" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="51"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="52" t="s">
-        <v>156</v>
-      </c>
-      <c r="G5" s="52"/>
+      <c r="F5" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" s="48"/>
       <c r="H5" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="51"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="52" t="s">
-        <v>157</v>
-      </c>
-      <c r="G6" s="52"/>
+      <c r="F6" s="48" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6" s="48"/>
       <c r="H6" s="39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="51"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="52" t="s">
-        <v>158</v>
-      </c>
-      <c r="G7" s="52"/>
+      <c r="F7" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="G7" s="48"/>
       <c r="H7" s="39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -3721,11 +3783,11 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="45">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="42" t="s">
-        <v>136</v>
+      <c r="B9" s="44" t="s">
+        <v>135</v>
       </c>
       <c r="C9" s="40" t="s">
         <v>71</v>
@@ -3734,70 +3796,70 @@
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" s="44" t="s">
-        <v>86</v>
+      <c r="F9" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>85</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="36" customHeight="1">
-      <c r="A10" s="43"/>
-      <c r="B10" s="50"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="53"/>
       <c r="C10" s="40"/>
       <c r="D10" s="2">
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="36" customHeight="1">
-      <c r="A11" s="43"/>
-      <c r="B11" s="50"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="40"/>
       <c r="D11" s="2">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
       <c r="H11" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="36" customHeight="1">
-      <c r="A12" s="43"/>
-      <c r="B12" s="50"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="40"/>
       <c r="D12" s="2">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
       <c r="H12" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="36" customHeight="1">
-      <c r="A13" s="43"/>
-      <c r="B13" s="50"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="40"/>
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
       <c r="H13" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -3811,82 +3873,82 @@
       <c r="H14" s="29"/>
     </row>
     <row r="15" spans="1:8" ht="54" customHeight="1">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="42" t="s">
-        <v>179</v>
-      </c>
-      <c r="C15" s="51" t="s">
+      <c r="B15" s="44" t="s">
+        <v>178</v>
+      </c>
+      <c r="C15" s="50" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="2">
         <v>145879</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44" t="s">
-        <v>177</v>
+      <c r="F15" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="54" customHeight="1">
-      <c r="A16" s="43"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="51"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="2">
         <v>200437</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="44" t="s">
-        <v>140</v>
-      </c>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
+      <c r="F16" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
     </row>
     <row r="17" spans="1:9" ht="54" customHeight="1">
-      <c r="A17" s="43"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="51"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="2">
         <v>310111</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
+      <c r="F17" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
     </row>
     <row r="18" spans="1:9" ht="54" customHeight="1">
-      <c r="A18" s="43"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="51"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="50"/>
       <c r="D18" s="2">
         <v>528401</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="44" t="s">
-        <v>142</v>
-      </c>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
+      <c r="F18" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
     </row>
     <row r="19" spans="1:9" ht="54" customHeight="1">
-      <c r="A19" s="43"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="51"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="2">
         <v>1076753</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="44" t="s">
-        <v>143</v>
-      </c>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
+      <c r="F19" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2"/>
@@ -3898,13 +3960,13 @@
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:9" ht="60" customHeight="1">
-      <c r="A21" s="45" t="s">
-        <v>195</v>
-      </c>
-      <c r="B21" s="42" t="s">
-        <v>138</v>
-      </c>
-      <c r="C21" s="51"/>
+      <c r="A21" s="47" t="s">
+        <v>194</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" s="50"/>
       <c r="D21" s="2">
         <v>145879</v>
       </c>
@@ -3912,55 +3974,60 @@
       <c r="F21" s="20"/>
       <c r="G21" s="10"/>
       <c r="H21" s="35" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="45">
-      <c r="A22" s="45"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="51"/>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="45" customHeight="1">
+      <c r="A22" s="47"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="50"/>
       <c r="D22" s="2">
         <v>200437</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="20"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="38" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="45"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="51"/>
+      <c r="H22" s="35" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="45" customHeight="1">
+      <c r="A23" s="47"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="50"/>
       <c r="D23" s="2">
         <v>310111</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="20"/>
       <c r="G23" s="10"/>
+      <c r="H23" s="49" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="45"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="51"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="50"/>
       <c r="D24" s="2">
         <v>528401</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="20"/>
       <c r="G24" s="10"/>
+      <c r="H24" s="49"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="45"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="51"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="50"/>
       <c r="D25" s="2">
         <v>1076753</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="20"/>
       <c r="G25" s="10"/>
+      <c r="H25" s="49"/>
     </row>
     <row r="26" spans="1:9" ht="45">
       <c r="A26" s="2"/>
@@ -3978,7 +4045,7 @@
         <v>39</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30">
@@ -3996,13 +4063,13 @@
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G27" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H27" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="45">
@@ -4021,17 +4088,17 @@
         <v>39</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="60">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="42" t="s">
-        <v>165</v>
-      </c>
-      <c r="C29" s="43" t="s">
+      <c r="B29" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="C29" s="45" t="s">
         <v>54</v>
       </c>
       <c r="D29" s="5">
@@ -4040,47 +4107,47 @@
       <c r="E29" s="5"/>
       <c r="F29"/>
       <c r="G29"/>
-      <c r="H29" s="58" t="s">
-        <v>200</v>
+      <c r="H29" s="49" t="s">
+        <v>199</v>
       </c>
       <c r="I29" s="27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="60">
-      <c r="A30" s="45"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="43"/>
+      <c r="A30" s="47"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="45"/>
       <c r="D30" s="5">
         <v>200437</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30"/>
       <c r="G30"/>
-      <c r="H30" s="58"/>
+      <c r="H30" s="49"/>
       <c r="I30" s="27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="45" customHeight="1">
-      <c r="A31" s="45"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="43"/>
+      <c r="A31" s="47"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="45"/>
       <c r="D31" s="5">
         <v>310111</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31"/>
       <c r="G31"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="44" t="s">
-        <v>159</v>
+      <c r="H31" s="49"/>
+      <c r="I31" s="43" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="45" customHeight="1">
-      <c r="A32" s="45"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="43"/>
+      <c r="A32" s="47"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="45"/>
       <c r="D32" s="5">
         <v>528401</v>
       </c>
@@ -4088,12 +4155,12 @@
       <c r="F32"/>
       <c r="G32"/>
       <c r="H32"/>
-      <c r="I32" s="44"/>
+      <c r="I32" s="43"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="45"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="43"/>
+      <c r="A33" s="47"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="45"/>
       <c r="D33" s="5">
         <v>1076753</v>
       </c>
@@ -4101,7 +4168,7 @@
       <c r="F33"/>
       <c r="G33"/>
       <c r="H33"/>
-      <c r="I33" s="44"/>
+      <c r="I33" s="43"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="5"/>
@@ -4114,13 +4181,13 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:9" ht="54" customHeight="1">
-      <c r="A35" s="45" t="s">
+      <c r="A35" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="42" t="s">
-        <v>176</v>
-      </c>
-      <c r="C35" s="48" t="s">
+      <c r="B35" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="C35" s="51" t="s">
         <v>63</v>
       </c>
       <c r="D35" s="5">
@@ -4130,13 +4197,13 @@
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
       <c r="H35" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="54" customHeight="1">
-      <c r="A36" s="45"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="49"/>
+      <c r="A36" s="47"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="52"/>
       <c r="D36" s="5">
         <v>200437</v>
       </c>
@@ -4144,13 +4211,13 @@
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
       <c r="H36" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="54" customHeight="1">
-      <c r="A37" s="45"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="49"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="52"/>
       <c r="D37" s="5">
         <v>310111</v>
       </c>
@@ -4158,13 +4225,13 @@
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
       <c r="H37" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="54" customHeight="1">
-      <c r="A38" s="45"/>
-      <c r="B38" s="42"/>
-      <c r="C38" s="49"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="44"/>
+      <c r="C38" s="52"/>
       <c r="D38" s="5">
         <v>528401</v>
       </c>
@@ -4172,13 +4239,13 @@
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
       <c r="H38" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="54" customHeight="1">
-      <c r="A39" s="45"/>
-      <c r="B39" s="42"/>
-      <c r="C39" s="49"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="52"/>
       <c r="D39" s="5">
         <v>1076753</v>
       </c>
@@ -4186,12 +4253,12 @@
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
       <c r="H39" s="27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="5"/>
-      <c r="B40" s="42"/>
+      <c r="B40" s="44"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -4203,7 +4270,7 @@
       <c r="A41" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="42"/>
+      <c r="B41" s="44"/>
       <c r="C41" s="19" t="s">
         <v>70</v>
       </c>
@@ -4214,7 +4281,7 @@
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
       <c r="H41" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -4239,7 +4306,7 @@
     </row>
     <row r="44" spans="1:9" ht="94.5" customHeight="1">
       <c r="A44" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B44" s="40"/>
       <c r="C44" s="40"/>
@@ -4259,34 +4326,11 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H15:H19"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="G9:G13"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="C21:C25"/>
+  <mergeCells count="40">
     <mergeCell ref="A44:F44"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="B35:B41"/>
@@ -4303,6 +4347,30 @@
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="F9:F13"/>
+    <mergeCell ref="G9:G13"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H15:H19"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4317,8 +4385,8 @@
   </sheetPr>
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4331,29 +4399,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="49.5" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="42" t="s">
         <v>20</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="47"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="1"/>
       <c r="F2" s="9" t="s">
         <v>39</v>
@@ -4363,11 +4431,11 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="36" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="42" t="s">
-        <v>136</v>
+      <c r="B3" s="44" t="s">
+        <v>135</v>
       </c>
       <c r="C3" s="40" t="s">
         <v>51</v>
@@ -4377,55 +4445,55 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="36" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="36" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="36" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -4435,71 +4503,71 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="45" customHeight="1">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="42" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9" s="51" t="s">
+      <c r="B9" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="50" t="s">
         <v>46</v>
       </c>
       <c r="D9" s="2">
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="53" t="s">
-        <v>178</v>
+      <c r="F9" s="43" t="s">
+        <v>177</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="45" customHeight="1">
-      <c r="A10" s="43"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="51"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="50"/>
       <c r="D10" s="2">
         <v>200437</v>
       </c>
-      <c r="F10" s="53"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="45" customHeight="1">
-      <c r="A11" s="43"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="51"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="2">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="53"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="45" customHeight="1">
-      <c r="A12" s="43"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="51"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="2">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="54" t="s">
-        <v>189</v>
+      <c r="F12" s="43" t="s">
+        <v>188</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="45" customHeight="1">
-      <c r="A13" s="43"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="51"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="54"/>
+      <c r="F13" s="43"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:8">
@@ -4510,27 +4578,27 @@
       <c r="E14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="43" t="s">
-        <v>195</v>
-      </c>
-      <c r="B15" s="42" t="s">
-        <v>138</v>
-      </c>
-      <c r="C15" s="51"/>
+    <row r="15" spans="1:8" ht="15" customHeight="1">
+      <c r="A15" s="45" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="50"/>
       <c r="D15" s="2">
         <v>145879</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="54" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1">
-      <c r="A16" s="43"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="51"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="2">
         <v>200437</v>
       </c>
@@ -4538,9 +4606,9 @@
       <c r="F16" s="54"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="43"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="51"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="2">
         <v>310111</v>
       </c>
@@ -4548,26 +4616,24 @@
       <c r="F17" s="54"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="43"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="51"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="50"/>
       <c r="D18" s="2">
         <v>528401</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="54"/>
     </row>
-    <row r="19" spans="1:14" ht="45">
-      <c r="A19" s="43"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="51"/>
+    <row r="19" spans="1:14">
+      <c r="A19" s="45"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="2">
         <v>1076753</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="31" t="s">
-        <v>199</v>
-      </c>
+      <c r="F19" s="54"/>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2"/>
@@ -4591,10 +4657,10 @@
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -4619,10 +4685,10 @@
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -4634,90 +4700,90 @@
       <c r="N24" s="12"/>
     </row>
     <row r="25" spans="1:14" ht="54" customHeight="1">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="42" t="s">
-        <v>176</v>
-      </c>
-      <c r="C25" s="48" t="s">
-        <v>95</v>
+      <c r="B25" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="C25" s="51" t="s">
+        <v>94</v>
       </c>
       <c r="D25" s="5">
         <v>145879</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N25" s="12"/>
     </row>
     <row r="26" spans="1:14" ht="54" customHeight="1">
-      <c r="A26" s="43"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="49"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="52"/>
       <c r="D26" s="5">
         <v>200437</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N26" s="12"/>
     </row>
     <row r="27" spans="1:14" ht="54" customHeight="1">
-      <c r="A27" s="43"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="49"/>
+      <c r="A27" s="45"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="52"/>
       <c r="D27" s="5">
         <v>310111</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N27" s="12"/>
     </row>
     <row r="28" spans="1:14" ht="54" customHeight="1">
-      <c r="A28" s="43"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="49"/>
+      <c r="A28" s="45"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="52"/>
       <c r="D28" s="5">
         <v>528401</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N28" s="12"/>
     </row>
     <row r="29" spans="1:14" ht="54" customHeight="1">
-      <c r="A29" s="43"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="49"/>
+      <c r="A29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="52"/>
       <c r="D29" s="5">
         <v>1076753</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N29" s="12"/>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="5"/>
-      <c r="B30" s="42"/>
+      <c r="B30" s="44"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="N30" s="12"/>
     </row>
     <row r="31" spans="1:14" ht="54" customHeight="1">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="42"/>
-      <c r="C31" s="48" t="s">
+      <c r="B31" s="44"/>
+      <c r="C31" s="51" t="s">
         <v>69</v>
       </c>
       <c r="D31" s="5">
@@ -4725,57 +4791,57 @@
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N31" s="12"/>
     </row>
     <row r="32" spans="1:14" ht="54" customHeight="1">
-      <c r="A32" s="43"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="49"/>
+      <c r="A32" s="45"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="52"/>
       <c r="D32" s="5">
         <v>200437</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N32" s="12"/>
     </row>
     <row r="33" spans="1:7" ht="54" customHeight="1">
-      <c r="A33" s="43"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="49"/>
+      <c r="A33" s="45"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="52"/>
       <c r="D33" s="5">
         <v>310111</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="54" customHeight="1">
-      <c r="A34" s="43"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="49"/>
+      <c r="A34" s="45"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="52"/>
       <c r="D34" s="5">
         <v>528401</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="54" customHeight="1">
-      <c r="A35" s="43"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="49"/>
+      <c r="A35" s="45"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="52"/>
       <c r="D35" s="5">
         <v>1076753</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -4789,7 +4855,7 @@
     </row>
     <row r="37" spans="1:7" ht="99.95" customHeight="1">
       <c r="A37" s="40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B37" s="40"/>
       <c r="C37" s="40"/>
@@ -4810,6 +4876,16 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F15:F19"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="A3:A7"/>
@@ -4823,16 +4899,6 @@
     <mergeCell ref="C9:C13"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="A9:A13"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F15:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4868,12 +4934,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -4919,7 +4985,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>47</v>
@@ -4928,16 +4994,16 @@
         <v>34</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>2</v>
@@ -4978,7 +5044,7 @@
     </row>
     <row r="7" spans="1:12" ht="90" customHeight="1">
       <c r="A7" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B7" s="40"/>
       <c r="C7" s="40"/>
@@ -5043,12 +5109,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -5090,11 +5156,11 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="42" t="s">
-        <v>136</v>
+      <c r="B3" s="44" t="s">
+        <v>135</v>
       </c>
       <c r="C3" s="40" t="s">
         <v>49</v>
@@ -5102,87 +5168,87 @@
       <c r="D3" s="2">
         <v>145879</v>
       </c>
-      <c r="E3" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="G3" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="H3" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="I3" s="43" t="s">
+      <c r="E3" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="G3" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="H3" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="I3" s="45" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="45" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="45"/>
       <c r="J4" s="55"/>
-      <c r="K4" s="43"/>
+      <c r="K4" s="45"/>
     </row>
     <row r="5" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="55"/>
-      <c r="K5" s="43"/>
+      <c r="K5" s="45"/>
     </row>
     <row r="6" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="55"/>
-      <c r="K6" s="43"/>
+      <c r="K6" s="45"/>
     </row>
     <row r="7" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="55"/>
-      <c r="K7" s="43"/>
+      <c r="K7" s="45"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="10"/>
@@ -5226,7 +5292,7 @@
     </row>
     <row r="11" spans="1:12" ht="99.95" customHeight="1">
       <c r="A11" s="40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="40"/>
       <c r="C11" s="40"/>
@@ -5302,12 +5368,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -5349,29 +5415,29 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="45">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>166</v>
-      </c>
-      <c r="C3" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" s="52" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="10">
         <v>145879</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>2</v>
@@ -5384,94 +5450,94 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42" t="s">
-        <v>136</v>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44" t="s">
+        <v>135</v>
       </c>
       <c r="C4" s="56"/>
       <c r="D4" s="10">
         <v>200437</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H4" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="3"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="56"/>
       <c r="D5" s="10">
         <v>310111</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="56"/>
       <c r="D6" s="10">
         <v>528401</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="56"/>
       <c r="D7" s="10">
         <v>1076753</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
@@ -5483,7 +5549,7 @@
     </row>
     <row r="9" spans="1:12" ht="90" customHeight="1">
       <c r="A9" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9" s="40"/>
       <c r="C9" s="40"/>
@@ -5530,7 +5596,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5552,13 +5618,13 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
       <c r="J1" s="10"/>
       <c r="K1" s="11"/>
       <c r="L1" s="10"/>
@@ -5586,10 +5652,10 @@
         <v>7</v>
       </c>
       <c r="H2" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>0</v>
@@ -5602,11 +5668,11 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="45" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="42" t="s">
-        <v>136</v>
+      <c r="B3" s="44" t="s">
+        <v>135</v>
       </c>
       <c r="C3" s="40" t="s">
         <v>51</v>
@@ -5624,24 +5690,24 @@
         <v>68</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I3" s="57" t="s">
-        <v>76</v>
-      </c>
-      <c r="J3" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="45" t="s">
         <v>2</v>
       </c>
       <c r="K3" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="43" t="s">
+      <c r="L3" s="45" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="45" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
@@ -5656,16 +5722,16 @@
         <v>68</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I4" s="57"/>
-      <c r="J4" s="43"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="55"/>
-      <c r="L4" s="43"/>
+      <c r="L4" s="45"/>
     </row>
     <row r="5" spans="1:12" ht="45" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
@@ -5680,16 +5746,16 @@
         <v>68</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I5" s="57"/>
-      <c r="J5" s="43"/>
+      <c r="J5" s="45"/>
       <c r="K5" s="55"/>
-      <c r="L5" s="43"/>
+      <c r="L5" s="45"/>
     </row>
     <row r="6" spans="1:12" ht="45" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
@@ -5704,16 +5770,16 @@
         <v>68</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I6" s="57"/>
-      <c r="J6" s="43"/>
+      <c r="J6" s="45"/>
       <c r="K6" s="55"/>
-      <c r="L6" s="43"/>
+      <c r="L6" s="45"/>
     </row>
     <row r="7" spans="1:12" ht="45" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
@@ -5728,12 +5794,12 @@
         <v>68</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I7" s="57"/>
-      <c r="J7" s="43"/>
+      <c r="J7" s="45"/>
       <c r="K7" s="55"/>
-      <c r="L7" s="43"/>
+      <c r="L7" s="45"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="10"/>
@@ -5766,7 +5832,7 @@
     </row>
     <row r="11" spans="1:12" ht="75" customHeight="1">
       <c r="A11" s="40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="40"/>
       <c r="C11" s="40"/>

</xml_diff>

<commit_message>
1 more run (now 2 runs) of SP_default on SBS_set1/Realistic finished
</commit_message>
<xml_diff>
--- a/documents/CPU_timing/mSigHdp-paper-tracking.xlsx
+++ b/documents/CPU_timing/mSigHdp-paper-tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\documents\CPU_timing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427FAD5C-D5AF-4C56-B7E2-A9A20BE791E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD271EC-4442-49A6-8F0A-DA7CCCE74B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="135" yWindow="780" windowWidth="15615" windowHeight="12045" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -134,6 +134,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={02DCCEA3-3360-4EC2-8065-19C6EFB3B5C6}</author>
+    <author>tc={AD9619A6-8F7F-4EDC-AE64-3DA2BDAAF3BD}</author>
   </authors>
   <commentList>
     <comment ref="I3" authorId="0" shapeId="0" xr:uid="{02DCCEA3-3360-4EC2-8065-19C6EFB3B5C6}">
@@ -143,6 +144,14 @@
 注释:
     Failed probably because it reached memory limit of qsub system (100GB) in the previous run.
 In the new run, I set memory limit to 200GB.</t>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="1" shapeId="0" xr:uid="{AD9619A6-8F7F-4EDC-AE64-3DA2BDAAF3BD}">
+      <text>
+        <t>[线程批注]
+你的Excel版本可读取此线程批注; 但如果在更新版本的Excel中打开文件，则对批注所作的任何改动都将被删除。了解详细信息: https://go.microsoft.com/fwlink/?linkid=870924
+注释:
+    Memory overflow</t>
       </text>
     </comment>
   </commentList>
@@ -177,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="206">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -1265,12 +1274,37 @@
 &lt;2058488&gt;
 (e0240162)</t>
   </si>
+  <si>
+    <t>m2
+&lt;2076596&gt;
+(e0240162)</t>
+  </si>
+  <si>
+    <t>HPC-super
+(wuyang)
+&lt;137431&gt;</t>
+  </si>
+  <si>
+    <t>HPC-long
+(wuyang)
+&lt;137496&gt;</t>
+  </si>
+  <si>
+    <t>HPC-long
+(wuyang)
+&lt;137497&gt;</t>
+  </si>
+  <si>
+    <t>HPC-long
+(wuyang)
+&lt;137498&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1350,6 +1384,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1553,19 +1601,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1587,6 +1632,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1925,6 +1973,9 @@
     <text>Failed probably because it reached memory limit of qsub system (100GB) in the previous run.
 In the new run, I set memory limit to 200GB.</text>
   </threadedComment>
+  <threadedComment ref="H5" dT="2022-10-03T02:39:49.77" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{AD9619A6-8F7F-4EDC-AE64-3DA2BDAAF3BD}">
+    <text>Memory overflow</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2249,7 +2300,7 @@
     </row>
     <row r="4" spans="1:18" ht="75" customHeight="1">
       <c r="A4" s="45"/>
-      <c r="B4" s="53"/>
+      <c r="B4" s="52"/>
       <c r="C4" s="40"/>
       <c r="D4" s="10">
         <v>200437</v>
@@ -2280,7 +2331,7 @@
     </row>
     <row r="5" spans="1:18" ht="36" customHeight="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="53"/>
+      <c r="B5" s="52"/>
       <c r="C5" s="40"/>
       <c r="D5" s="10">
         <v>310111</v>
@@ -2301,7 +2352,7 @@
     </row>
     <row r="6" spans="1:18" ht="36" customHeight="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="53"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="40"/>
       <c r="D6" s="10">
         <v>528401</v>
@@ -2322,7 +2373,7 @@
     </row>
     <row r="7" spans="1:18" ht="36" customHeight="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="53"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="40"/>
       <c r="D7" s="10">
         <v>1076753</v>
@@ -2356,7 +2407,7 @@
       <c r="B9" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="47" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="10">
@@ -2402,8 +2453,8 @@
     </row>
     <row r="10" spans="1:18" ht="54" customHeight="1">
       <c r="A10" s="45"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="50"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="10">
         <v>200437</v>
       </c>
@@ -2423,8 +2474,8 @@
     </row>
     <row r="11" spans="1:18" ht="54" customHeight="1">
       <c r="A11" s="45"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="50"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="47"/>
       <c r="D11" s="10">
         <v>310111</v>
       </c>
@@ -2444,8 +2495,8 @@
     </row>
     <row r="12" spans="1:18" ht="54" customHeight="1">
       <c r="A12" s="45"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="50"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="10">
         <v>528401</v>
       </c>
@@ -2465,8 +2516,8 @@
     </row>
     <row r="13" spans="1:18" ht="54" customHeight="1">
       <c r="A13" s="45"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="50"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="47"/>
       <c r="D13" s="10">
         <v>1076753</v>
       </c>
@@ -2567,8 +2618,8 @@
   </sheetPr>
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2766,7 +2817,7 @@
       <c r="B11" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="C11" s="50"/>
+      <c r="C11" s="47"/>
       <c r="D11" s="2">
         <v>145879</v>
       </c>
@@ -2781,7 +2832,7 @@
     <row r="12" spans="1:15">
       <c r="A12" s="45"/>
       <c r="B12" s="44"/>
-      <c r="C12" s="50"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="2">
         <v>200437</v>
       </c>
@@ -2796,7 +2847,7 @@
     <row r="13" spans="1:15">
       <c r="A13" s="45"/>
       <c r="B13" s="44"/>
-      <c r="C13" s="50"/>
+      <c r="C13" s="47"/>
       <c r="D13" s="2">
         <v>310111</v>
       </c>
@@ -2811,7 +2862,7 @@
     <row r="14" spans="1:15">
       <c r="A14" s="45"/>
       <c r="B14" s="44"/>
-      <c r="C14" s="50"/>
+      <c r="C14" s="47"/>
       <c r="D14" s="2">
         <v>528401</v>
       </c>
@@ -2826,7 +2877,7 @@
     <row r="15" spans="1:15">
       <c r="A15" s="45"/>
       <c r="B15" s="44"/>
-      <c r="C15" s="50"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="2">
         <v>1076753</v>
       </c>
@@ -2900,7 +2951,7 @@
       <c r="B19" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="C19" s="47" t="s">
+      <c r="C19" s="46" t="s">
         <v>56</v>
       </c>
       <c r="D19" s="2">
@@ -2917,7 +2968,7 @@
     <row r="20" spans="1:15" ht="60" customHeight="1">
       <c r="A20" s="45"/>
       <c r="B20" s="44"/>
-      <c r="C20" s="47"/>
+      <c r="C20" s="46"/>
       <c r="D20" s="2">
         <v>200437</v>
       </c>
@@ -2932,7 +2983,7 @@
     <row r="21" spans="1:15" ht="60" customHeight="1">
       <c r="A21" s="45"/>
       <c r="B21" s="44"/>
-      <c r="C21" s="47"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="2">
         <v>310111</v>
       </c>
@@ -2947,7 +2998,7 @@
     <row r="22" spans="1:15" ht="60" customHeight="1">
       <c r="A22" s="45"/>
       <c r="B22" s="44"/>
-      <c r="C22" s="47"/>
+      <c r="C22" s="46"/>
       <c r="D22" s="2">
         <v>528401</v>
       </c>
@@ -2962,7 +3013,7 @@
     <row r="23" spans="1:15" ht="60" customHeight="1">
       <c r="A23" s="45"/>
       <c r="B23" s="44"/>
-      <c r="C23" s="47"/>
+      <c r="C23" s="46"/>
       <c r="D23" s="2">
         <v>1076753</v>
       </c>
@@ -3026,7 +3077,7 @@
         <v>31</v>
       </c>
       <c r="B27" s="44"/>
-      <c r="C27" s="46" t="s">
+      <c r="C27" s="48" t="s">
         <v>64</v>
       </c>
       <c r="D27" s="2">
@@ -3045,7 +3096,7 @@
     <row r="28" spans="1:15" ht="60" customHeight="1">
       <c r="A28" s="45"/>
       <c r="B28" s="44"/>
-      <c r="C28" s="46"/>
+      <c r="C28" s="48"/>
       <c r="D28" s="2">
         <v>200437</v>
       </c>
@@ -3060,7 +3111,7 @@
     <row r="29" spans="1:15" ht="60" customHeight="1">
       <c r="A29" s="45"/>
       <c r="B29" s="44"/>
-      <c r="C29" s="46"/>
+      <c r="C29" s="48"/>
       <c r="D29" s="2">
         <v>310111</v>
       </c>
@@ -3075,7 +3126,7 @@
     <row r="30" spans="1:15" ht="60" customHeight="1">
       <c r="A30" s="45"/>
       <c r="B30" s="44"/>
-      <c r="C30" s="46"/>
+      <c r="C30" s="48"/>
       <c r="D30" s="2">
         <v>528401</v>
       </c>
@@ -3090,7 +3141,7 @@
     <row r="31" spans="1:15" ht="60" customHeight="1">
       <c r="A31" s="45"/>
       <c r="B31" s="44"/>
-      <c r="C31" s="46"/>
+      <c r="C31" s="48"/>
       <c r="D31" s="2">
         <v>1076753</v>
       </c>
@@ -3185,8 +3236,8 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3269,7 +3320,7 @@
       <c r="G3" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="28" t="s">
         <v>84</v>
       </c>
       <c r="I3" s="2"/>
@@ -3477,7 +3528,7 @@
         <v>31</v>
       </c>
       <c r="B15" s="44"/>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="48" t="s">
         <v>65</v>
       </c>
       <c r="D15" s="5">
@@ -3498,7 +3549,7 @@
     <row r="16" spans="1:14" ht="54" customHeight="1">
       <c r="A16" s="45"/>
       <c r="B16" s="44"/>
-      <c r="C16" s="46"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="5">
         <v>200437</v>
       </c>
@@ -3515,7 +3566,7 @@
     <row r="17" spans="1:14" ht="54" customHeight="1">
       <c r="A17" s="45"/>
       <c r="B17" s="44"/>
-      <c r="C17" s="46"/>
+      <c r="C17" s="48"/>
       <c r="D17" s="5">
         <v>310111</v>
       </c>
@@ -3532,7 +3583,7 @@
     <row r="18" spans="1:14" ht="54" customHeight="1">
       <c r="A18" s="45"/>
       <c r="B18" s="44"/>
-      <c r="C18" s="46"/>
+      <c r="C18" s="48"/>
       <c r="D18" s="5">
         <v>528401</v>
       </c>
@@ -3549,7 +3600,7 @@
     <row r="19" spans="1:14" ht="54" customHeight="1">
       <c r="A19" s="45"/>
       <c r="B19" s="44"/>
-      <c r="C19" s="46"/>
+      <c r="C19" s="48"/>
       <c r="D19" s="5">
         <v>1076753</v>
       </c>
@@ -3643,8 +3694,8 @@
   </sheetPr>
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23:H25"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3696,17 +3747,17 @@
       <c r="B3" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="47" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="G3" s="48"/>
+      <c r="G3" s="49"/>
       <c r="H3" s="39" t="s">
         <v>153</v>
       </c>
@@ -3714,15 +3765,15 @@
     <row r="4" spans="1:8" ht="45">
       <c r="A4" s="45"/>
       <c r="B4" s="44"/>
-      <c r="C4" s="50"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="49" t="s">
         <v>154</v>
       </c>
-      <c r="G4" s="48"/>
+      <c r="G4" s="49"/>
       <c r="H4" s="39" t="s">
         <v>154</v>
       </c>
@@ -3730,15 +3781,15 @@
     <row r="5" spans="1:8" ht="45">
       <c r="A5" s="45"/>
       <c r="B5" s="44"/>
-      <c r="C5" s="50"/>
+      <c r="C5" s="47"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="49" t="s">
         <v>155</v>
       </c>
-      <c r="G5" s="48"/>
+      <c r="G5" s="49"/>
       <c r="H5" s="39" t="s">
         <v>155</v>
       </c>
@@ -3746,15 +3797,15 @@
     <row r="6" spans="1:8" ht="45">
       <c r="A6" s="45"/>
       <c r="B6" s="44"/>
-      <c r="C6" s="50"/>
+      <c r="C6" s="47"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="G6" s="48"/>
+      <c r="G6" s="49"/>
       <c r="H6" s="39" t="s">
         <v>156</v>
       </c>
@@ -3762,15 +3813,15 @@
     <row r="7" spans="1:8" ht="45">
       <c r="A7" s="45"/>
       <c r="B7" s="44"/>
-      <c r="C7" s="50"/>
+      <c r="C7" s="47"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="G7" s="48"/>
+      <c r="G7" s="49"/>
       <c r="H7" s="39" t="s">
         <v>157</v>
       </c>
@@ -3808,7 +3859,7 @@
     </row>
     <row r="10" spans="1:8" ht="36" customHeight="1">
       <c r="A10" s="45"/>
-      <c r="B10" s="53"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="40"/>
       <c r="D10" s="2">
         <v>200437</v>
@@ -3822,7 +3873,7 @@
     </row>
     <row r="11" spans="1:8" ht="36" customHeight="1">
       <c r="A11" s="45"/>
-      <c r="B11" s="53"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="40"/>
       <c r="D11" s="2">
         <v>310111</v>
@@ -3836,7 +3887,7 @@
     </row>
     <row r="12" spans="1:8" ht="36" customHeight="1">
       <c r="A12" s="45"/>
-      <c r="B12" s="53"/>
+      <c r="B12" s="52"/>
       <c r="C12" s="40"/>
       <c r="D12" s="2">
         <v>528401</v>
@@ -3850,7 +3901,7 @@
     </row>
     <row r="13" spans="1:8" ht="36" customHeight="1">
       <c r="A13" s="45"/>
-      <c r="B13" s="53"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="40"/>
       <c r="D13" s="2">
         <v>1076753</v>
@@ -3879,7 +3930,7 @@
       <c r="B15" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="C15" s="50" t="s">
+      <c r="C15" s="47" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="2">
@@ -3897,7 +3948,7 @@
     <row r="16" spans="1:8" ht="54" customHeight="1">
       <c r="A16" s="45"/>
       <c r="B16" s="44"/>
-      <c r="C16" s="50"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="2">
         <v>200437</v>
       </c>
@@ -3911,7 +3962,7 @@
     <row r="17" spans="1:9" ht="54" customHeight="1">
       <c r="A17" s="45"/>
       <c r="B17" s="44"/>
-      <c r="C17" s="50"/>
+      <c r="C17" s="47"/>
       <c r="D17" s="2">
         <v>310111</v>
       </c>
@@ -3925,7 +3976,7 @@
     <row r="18" spans="1:9" ht="54" customHeight="1">
       <c r="A18" s="45"/>
       <c r="B18" s="44"/>
-      <c r="C18" s="50"/>
+      <c r="C18" s="47"/>
       <c r="D18" s="2">
         <v>528401</v>
       </c>
@@ -3939,7 +3990,7 @@
     <row r="19" spans="1:9" ht="54" customHeight="1">
       <c r="A19" s="45"/>
       <c r="B19" s="44"/>
-      <c r="C19" s="50"/>
+      <c r="C19" s="47"/>
       <c r="D19" s="2">
         <v>1076753</v>
       </c>
@@ -3960,27 +4011,27 @@
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:9" ht="60" customHeight="1">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="46" t="s">
         <v>194</v>
       </c>
       <c r="B21" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="C21" s="50"/>
+      <c r="C21" s="47"/>
       <c r="D21" s="2">
         <v>145879</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="20"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="35" t="s">
+      <c r="H21" s="27" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="45" customHeight="1">
-      <c r="A22" s="47"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="44"/>
-      <c r="C22" s="50"/>
+      <c r="C22" s="47"/>
       <c r="D22" s="2">
         <v>200437</v>
       </c>
@@ -3992,42 +4043,42 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="45" customHeight="1">
-      <c r="A23" s="47"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="44"/>
-      <c r="C23" s="50"/>
+      <c r="C23" s="47"/>
       <c r="D23" s="2">
         <v>310111</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="20"/>
       <c r="G23" s="10"/>
-      <c r="H23" s="49" t="s">
-        <v>200</v>
+      <c r="H23" s="56" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="47"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="44"/>
-      <c r="C24" s="50"/>
+      <c r="C24" s="47"/>
       <c r="D24" s="2">
         <v>528401</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="20"/>
       <c r="G24" s="10"/>
-      <c r="H24" s="49"/>
+      <c r="H24" s="56"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="47"/>
+      <c r="A25" s="46"/>
       <c r="B25" s="44"/>
-      <c r="C25" s="50"/>
+      <c r="C25" s="47"/>
       <c r="D25" s="2">
         <v>1076753</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="20"/>
       <c r="G25" s="10"/>
-      <c r="H25" s="49"/>
+      <c r="H25" s="56"/>
     </row>
     <row r="26" spans="1:9" ht="45">
       <c r="A26" s="2"/>
@@ -4092,7 +4143,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="60">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="46" t="s">
         <v>25</v>
       </c>
       <c r="B29" s="44" t="s">
@@ -4107,7 +4158,7 @@
       <c r="E29" s="5"/>
       <c r="F29"/>
       <c r="G29"/>
-      <c r="H29" s="49" t="s">
+      <c r="H29" s="35" t="s">
         <v>199</v>
       </c>
       <c r="I29" s="27" t="s">
@@ -4115,7 +4166,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="60">
-      <c r="A30" s="47"/>
+      <c r="A30" s="46"/>
       <c r="B30" s="44"/>
       <c r="C30" s="45"/>
       <c r="D30" s="5">
@@ -4124,13 +4175,15 @@
       <c r="E30" s="5"/>
       <c r="F30"/>
       <c r="G30"/>
-      <c r="H30" s="49"/>
+      <c r="H30" s="31" t="s">
+        <v>202</v>
+      </c>
       <c r="I30" s="27" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="45" customHeight="1">
-      <c r="A31" s="47"/>
+      <c r="A31" s="46"/>
       <c r="B31" s="44"/>
       <c r="C31" s="45"/>
       <c r="D31" s="5">
@@ -4139,13 +4192,15 @@
       <c r="E31" s="5"/>
       <c r="F31"/>
       <c r="G31"/>
-      <c r="H31" s="49"/>
+      <c r="H31" s="31" t="s">
+        <v>205</v>
+      </c>
       <c r="I31" s="43" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="45" customHeight="1">
-      <c r="A32" s="47"/>
+      <c r="A32" s="46"/>
       <c r="B32" s="44"/>
       <c r="C32" s="45"/>
       <c r="D32" s="5">
@@ -4154,11 +4209,13 @@
       <c r="E32" s="5"/>
       <c r="F32"/>
       <c r="G32"/>
-      <c r="H32"/>
+      <c r="H32" s="31" t="s">
+        <v>203</v>
+      </c>
       <c r="I32" s="43"/>
     </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="47"/>
+    <row r="33" spans="1:9" ht="45">
+      <c r="A33" s="46"/>
       <c r="B33" s="44"/>
       <c r="C33" s="45"/>
       <c r="D33" s="5">
@@ -4167,7 +4224,9 @@
       <c r="E33" s="5"/>
       <c r="F33"/>
       <c r="G33"/>
-      <c r="H33"/>
+      <c r="H33" s="31" t="s">
+        <v>204</v>
+      </c>
       <c r="I33" s="43"/>
     </row>
     <row r="34" spans="1:9">
@@ -4181,13 +4240,13 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:9" ht="54" customHeight="1">
-      <c r="A35" s="47" t="s">
+      <c r="A35" s="46" t="s">
         <v>28</v>
       </c>
       <c r="B35" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="C35" s="51" t="s">
+      <c r="C35" s="50" t="s">
         <v>63</v>
       </c>
       <c r="D35" s="5">
@@ -4201,9 +4260,9 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="54" customHeight="1">
-      <c r="A36" s="47"/>
+      <c r="A36" s="46"/>
       <c r="B36" s="44"/>
-      <c r="C36" s="52"/>
+      <c r="C36" s="51"/>
       <c r="D36" s="5">
         <v>200437</v>
       </c>
@@ -4215,9 +4274,9 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="54" customHeight="1">
-      <c r="A37" s="47"/>
+      <c r="A37" s="46"/>
       <c r="B37" s="44"/>
-      <c r="C37" s="52"/>
+      <c r="C37" s="51"/>
       <c r="D37" s="5">
         <v>310111</v>
       </c>
@@ -4229,9 +4288,9 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="54" customHeight="1">
-      <c r="A38" s="47"/>
+      <c r="A38" s="46"/>
       <c r="B38" s="44"/>
-      <c r="C38" s="52"/>
+      <c r="C38" s="51"/>
       <c r="D38" s="5">
         <v>528401</v>
       </c>
@@ -4243,9 +4302,9 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="54" customHeight="1">
-      <c r="A39" s="47"/>
+      <c r="A39" s="46"/>
       <c r="B39" s="44"/>
-      <c r="C39" s="52"/>
+      <c r="C39" s="51"/>
       <c r="D39" s="5">
         <v>1076753</v>
       </c>
@@ -4330,7 +4389,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="39">
     <mergeCell ref="A44:F44"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="B35:B41"/>
@@ -4364,7 +4423,6 @@
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H15:H19"/>
-    <mergeCell ref="H29:H31"/>
     <mergeCell ref="H23:H25"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F4:G4"/>
@@ -4385,8 +4443,8 @@
   </sheetPr>
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4509,7 +4567,7 @@
       <c r="B9" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="47" t="s">
         <v>46</v>
       </c>
       <c r="D9" s="2">
@@ -4525,7 +4583,7 @@
     <row r="10" spans="1:8" ht="45" customHeight="1">
       <c r="A10" s="45"/>
       <c r="B10" s="44"/>
-      <c r="C10" s="50"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="2">
         <v>200437</v>
       </c>
@@ -4536,7 +4594,7 @@
     <row r="11" spans="1:8" ht="45" customHeight="1">
       <c r="A11" s="45"/>
       <c r="B11" s="44"/>
-      <c r="C11" s="50"/>
+      <c r="C11" s="47"/>
       <c r="D11" s="2">
         <v>310111</v>
       </c>
@@ -4548,7 +4606,7 @@
     <row r="12" spans="1:8" ht="45" customHeight="1">
       <c r="A12" s="45"/>
       <c r="B12" s="44"/>
-      <c r="C12" s="50"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="2">
         <v>528401</v>
       </c>
@@ -4562,7 +4620,7 @@
     <row r="13" spans="1:8" ht="45" customHeight="1">
       <c r="A13" s="45"/>
       <c r="B13" s="44"/>
-      <c r="C13" s="50"/>
+      <c r="C13" s="47"/>
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
@@ -4585,12 +4643,12 @@
       <c r="B15" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="C15" s="50"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="2">
         <v>145879</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="54" t="s">
+      <c r="F15" s="53" t="s">
         <v>198</v>
       </c>
       <c r="G15" s="10"/>
@@ -4598,42 +4656,42 @@
     <row r="16" spans="1:8" ht="15" customHeight="1">
       <c r="A16" s="45"/>
       <c r="B16" s="44"/>
-      <c r="C16" s="50"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="2">
         <v>200437</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="54"/>
+      <c r="F16" s="53"/>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="45"/>
       <c r="B17" s="44"/>
-      <c r="C17" s="50"/>
+      <c r="C17" s="47"/>
       <c r="D17" s="2">
         <v>310111</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="54"/>
+      <c r="F17" s="53"/>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="45"/>
       <c r="B18" s="44"/>
-      <c r="C18" s="50"/>
+      <c r="C18" s="47"/>
       <c r="D18" s="2">
         <v>528401</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="54"/>
+      <c r="F18" s="53"/>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="45"/>
       <c r="B19" s="44"/>
-      <c r="C19" s="50"/>
+      <c r="C19" s="47"/>
       <c r="D19" s="2">
         <v>1076753</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="54"/>
+      <c r="F19" s="53"/>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2"/>
@@ -4706,7 +4764,7 @@
       <c r="B25" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="C25" s="51" t="s">
+      <c r="C25" s="50" t="s">
         <v>94</v>
       </c>
       <c r="D25" s="5">
@@ -4721,7 +4779,7 @@
     <row r="26" spans="1:14" ht="54" customHeight="1">
       <c r="A26" s="45"/>
       <c r="B26" s="44"/>
-      <c r="C26" s="52"/>
+      <c r="C26" s="51"/>
       <c r="D26" s="5">
         <v>200437</v>
       </c>
@@ -4734,7 +4792,7 @@
     <row r="27" spans="1:14" ht="54" customHeight="1">
       <c r="A27" s="45"/>
       <c r="B27" s="44"/>
-      <c r="C27" s="52"/>
+      <c r="C27" s="51"/>
       <c r="D27" s="5">
         <v>310111</v>
       </c>
@@ -4747,7 +4805,7 @@
     <row r="28" spans="1:14" ht="54" customHeight="1">
       <c r="A28" s="45"/>
       <c r="B28" s="44"/>
-      <c r="C28" s="52"/>
+      <c r="C28" s="51"/>
       <c r="D28" s="5">
         <v>528401</v>
       </c>
@@ -4760,7 +4818,7 @@
     <row r="29" spans="1:14" ht="54" customHeight="1">
       <c r="A29" s="45"/>
       <c r="B29" s="44"/>
-      <c r="C29" s="52"/>
+      <c r="C29" s="51"/>
       <c r="D29" s="5">
         <v>1076753</v>
       </c>
@@ -4783,7 +4841,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="44"/>
-      <c r="C31" s="51" t="s">
+      <c r="C31" s="50" t="s">
         <v>69</v>
       </c>
       <c r="D31" s="5">
@@ -4798,7 +4856,7 @@
     <row r="32" spans="1:14" ht="54" customHeight="1">
       <c r="A32" s="45"/>
       <c r="B32" s="44"/>
-      <c r="C32" s="52"/>
+      <c r="C32" s="51"/>
       <c r="D32" s="5">
         <v>200437</v>
       </c>
@@ -4811,7 +4869,7 @@
     <row r="33" spans="1:7" ht="54" customHeight="1">
       <c r="A33" s="45"/>
       <c r="B33" s="44"/>
-      <c r="C33" s="52"/>
+      <c r="C33" s="51"/>
       <c r="D33" s="5">
         <v>310111</v>
       </c>
@@ -4823,7 +4881,7 @@
     <row r="34" spans="1:7" ht="54" customHeight="1">
       <c r="A34" s="45"/>
       <c r="B34" s="44"/>
-      <c r="C34" s="52"/>
+      <c r="C34" s="51"/>
       <c r="D34" s="5">
         <v>528401</v>
       </c>
@@ -4835,7 +4893,7 @@
     <row r="35" spans="1:7" ht="54" customHeight="1">
       <c r="A35" s="45"/>
       <c r="B35" s="44"/>
-      <c r="C35" s="52"/>
+      <c r="C35" s="51"/>
       <c r="D35" s="5">
         <v>1076753</v>
       </c>
@@ -5183,7 +5241,7 @@
       <c r="I3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="55" t="s">
+      <c r="J3" s="54" t="s">
         <v>13</v>
       </c>
       <c r="K3" s="45" t="s">
@@ -5202,7 +5260,7 @@
       <c r="G4" s="43"/>
       <c r="H4" s="43"/>
       <c r="I4" s="45"/>
-      <c r="J4" s="55"/>
+      <c r="J4" s="54"/>
       <c r="K4" s="45"/>
     </row>
     <row r="5" spans="1:12" ht="35.1" customHeight="1">
@@ -5217,7 +5275,7 @@
       <c r="G5" s="43"/>
       <c r="H5" s="43"/>
       <c r="I5" s="45"/>
-      <c r="J5" s="55"/>
+      <c r="J5" s="54"/>
       <c r="K5" s="45"/>
     </row>
     <row r="6" spans="1:12" ht="35.1" customHeight="1">
@@ -5232,7 +5290,7 @@
       <c r="G6" s="43"/>
       <c r="H6" s="43"/>
       <c r="I6" s="45"/>
-      <c r="J6" s="55"/>
+      <c r="J6" s="54"/>
       <c r="K6" s="45"/>
     </row>
     <row r="7" spans="1:12" ht="35.1" customHeight="1">
@@ -5247,7 +5305,7 @@
       <c r="G7" s="43"/>
       <c r="H7" s="43"/>
       <c r="I7" s="45"/>
-      <c r="J7" s="55"/>
+      <c r="J7" s="54"/>
       <c r="K7" s="45"/>
     </row>
     <row r="8" spans="1:12">
@@ -5346,7 +5404,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5421,7 +5479,7 @@
       <c r="B3" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="51" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="10">
@@ -5454,7 +5512,7 @@
       <c r="B4" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="56"/>
+      <c r="C4" s="55"/>
       <c r="D4" s="10">
         <v>200437</v>
       </c>
@@ -5477,7 +5535,7 @@
     <row r="5" spans="1:12" ht="30" customHeight="1">
       <c r="A5" s="45"/>
       <c r="B5" s="44"/>
-      <c r="C5" s="56"/>
+      <c r="C5" s="55"/>
       <c r="D5" s="10">
         <v>310111</v>
       </c>
@@ -5500,7 +5558,7 @@
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="45"/>
       <c r="B6" s="44"/>
-      <c r="C6" s="56"/>
+      <c r="C6" s="55"/>
       <c r="D6" s="10">
         <v>528401</v>
       </c>
@@ -5523,7 +5581,7 @@
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="45"/>
       <c r="B7" s="44"/>
-      <c r="C7" s="56"/>
+      <c r="C7" s="55"/>
       <c r="D7" s="10">
         <v>1076753</v>
       </c>
@@ -5595,9 +5653,7 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5692,13 +5748,13 @@
       <c r="H3" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="I3" s="57" t="s">
+      <c r="I3" s="56" t="s">
         <v>75</v>
       </c>
       <c r="J3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="55" t="s">
+      <c r="K3" s="54" t="s">
         <v>13</v>
       </c>
       <c r="L3" s="45" t="s">
@@ -5724,9 +5780,9 @@
       <c r="H4" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="I4" s="57"/>
+      <c r="I4" s="56"/>
       <c r="J4" s="45"/>
-      <c r="K4" s="55"/>
+      <c r="K4" s="54"/>
       <c r="L4" s="45"/>
     </row>
     <row r="5" spans="1:12" ht="45" customHeight="1">
@@ -5745,12 +5801,12 @@
       <c r="G5" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="57" t="s">
         <v>191</v>
       </c>
-      <c r="I5" s="57"/>
+      <c r="I5" s="56"/>
       <c r="J5" s="45"/>
-      <c r="K5" s="55"/>
+      <c r="K5" s="54"/>
       <c r="L5" s="45"/>
     </row>
     <row r="6" spans="1:12" ht="45" customHeight="1">
@@ -5769,12 +5825,12 @@
       <c r="G6" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="I6" s="57"/>
+      <c r="I6" s="56"/>
       <c r="J6" s="45"/>
-      <c r="K6" s="55"/>
+      <c r="K6" s="54"/>
       <c r="L6" s="45"/>
     </row>
     <row r="7" spans="1:12" ht="45" customHeight="1">
@@ -5796,9 +5852,9 @@
       <c r="H7" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="I7" s="57"/>
+      <c r="I7" s="56"/>
       <c r="J7" s="45"/>
-      <c r="K7" s="55"/>
+      <c r="K7" s="54"/>
       <c r="L7" s="45"/>
     </row>
     <row r="8" spans="1:12">

</xml_diff>

<commit_message>
Updated supplementary table S4:
Added mSigHdp_ds_10k on SBS_set2/Realistic
</commit_message>
<xml_diff>
--- a/documents/CPU_timing/mSigHdp-paper-tracking.xlsx
+++ b/documents/CPU_timing/mSigHdp-paper-tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\documents\CPU_timing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F12EE9-1CCC-4E68-A7CA-91E5D37D2D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909B9E99-E08C-4C26-8158-1FFA3761F686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11895" yWindow="1440" windowWidth="15615" windowHeight="12045" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13620" yWindow="630" windowWidth="14940" windowHeight="12045" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -88,11 +88,12 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={C7106C03-6689-4A25-9A74-769B478807DA}</author>
+    <author>tc={969B69DB-1798-468C-980F-E678BCC615AD}</author>
+    <author>tc={4DB6E460-A4FE-40A6-B672-BB0B18A4A4A8}</author>
     <author>tc={7879683C-1E68-4F58-975B-EB0BED2C30CE}</author>
   </authors>
   <commentList>
-    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{C7106C03-6689-4A25-9A74-769B478807DA}">
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{969B69DB-1798-468C-980F-E678BCC615AD}">
       <text>
         <t>[线程批注]
 你的Excel版本可读取此线程批注; 但如果在更新版本的Excel中打开文件，则对批注所作的任何改动都将被删除。了解详细信息: https://go.microsoft.com/fwlink/?linkid=870924
@@ -100,12 +101,22 @@
     Needs to re-run on HPC</t>
       </text>
     </comment>
-    <comment ref="J40" authorId="1" shapeId="0" xr:uid="{7879683C-1E68-4F58-975B-EB0BED2C30CE}">
+    <comment ref="H27" authorId="1" shapeId="0" xr:uid="{4DB6E460-A4FE-40A6-B672-BB0B18A4A4A8}">
       <text>
         <t>[线程批注]
 你的Excel版本可读取此线程批注; 但如果在更新版本的Excel中打开文件，则对批注所作的任何改动都将被删除。了解详细信息: https://go.microsoft.com/fwlink/?linkid=870924
 注释:
-    Have different results compared to Realistic_wrong_time, despite using the same signeR and NMF version.</t>
+    Needs re-download</t>
+      </text>
+    </comment>
+    <comment ref="J40" authorId="2" shapeId="0" xr:uid="{7879683C-1E68-4F58-975B-EB0BED2C30CE}">
+      <text>
+        <t>[线程批注]
+你的Excel版本可读取此线程批注; 但如果在更新版本的Excel中打开文件，则对批注所作的任何改动都将被删除。了解详细信息: https://go.microsoft.com/fwlink/?linkid=870924
+注释:
+    Have different results compared to Realistic_wrong_time, despite using the same signeR and NMF version.
+答复:
+    Needs to download signeR.Rdata file</t>
       </text>
     </comment>
   </commentList>
@@ -142,25 +153,6 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={02DCCEA3-3360-4EC2-8065-19C6EFB3B5C6}</author>
-  </authors>
-  <commentList>
-    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{02DCCEA3-3360-4EC2-8065-19C6EFB3B5C6}">
-      <text>
-        <t>[线程批注]
-你的Excel版本可读取此线程批注; 但如果在更新版本的Excel中打开文件，则对批注所作的任何改动都将被删除。了解详细信息: https://go.microsoft.com/fwlink/?linkid=870924
-注释:
-    Failed probably because it reached memory limit of qsub system (100GB) in the previous run.
-In the new run, I set memory limit to 200GB.</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
     <author>tc={A3DE0894-D222-4604-B6B6-2E7833CF63F7}</author>
     <author>tc={E7E8AB2C-34D0-42B0-AC25-1C61178C0DC6}</author>
   </authors>
@@ -186,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="223">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -654,12 +646,6 @@
   </si>
   <si>
     <t>10k-rerun</t>
-  </si>
-  <si>
-    <t>10k-failed</t>
-  </si>
-  <si>
-    <t>hpc-super(e0240162)</t>
   </si>
   <si>
     <t>hpc-long
@@ -1439,6 +1425,21 @@
   </si>
   <si>
     <t>Realistic-HPC-2nd-trial</t>
+  </si>
+  <si>
+    <t>m2
+&lt;2656047&gt;
+(e0240162)</t>
+  </si>
+  <si>
+    <t>HPC-super
+&lt;138725&gt;
+(wuyang)</t>
+  </si>
+  <si>
+    <t>HPC-super
+&lt;138726&gt;
+(wuyang)</t>
   </si>
 </sst>
 </file>
@@ -1535,7 +1536,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1584,6 +1585,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD26900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1599,7 +1606,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1718,23 +1725,11 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1743,18 +1738,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1774,12 +1778,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2094,11 +2092,17 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="H3" dT="2022-09-28T08:49:32.12" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{C7106C03-6689-4A25-9A74-769B478807DA}">
+  <threadedComment ref="I3" dT="2022-09-28T08:49:32.12" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{969B69DB-1798-468C-980F-E678BCC615AD}">
     <text>Needs to re-run on HPC</text>
+  </threadedComment>
+  <threadedComment ref="H27" dT="2022-10-05T08:49:51.16" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{4DB6E460-A4FE-40A6-B672-BB0B18A4A4A8}">
+    <text>Needs re-download</text>
   </threadedComment>
   <threadedComment ref="J40" dT="2022-10-04T01:45:33.47" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{7879683C-1E68-4F58-975B-EB0BED2C30CE}">
     <text>Have different results compared to Realistic_wrong_time, despite using the same signeR and NMF version.</text>
+  </threadedComment>
+  <threadedComment ref="J40" dT="2022-10-05T08:49:27.78" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{D645002E-BC3C-43B1-B316-C7F4E418B207}" parentId="{7879683C-1E68-4F58-975B-EB0BED2C30CE}">
+    <text>Needs to download signeR.Rdata file</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -2115,15 +2119,6 @@
 </file>
 
 <file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="I3" dT="2022-08-08T13:23:30.12" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{02DCCEA3-3360-4EC2-8065-19C6EFB3B5C6}">
-    <text>Failed probably because it reached memory limit of qsub system (100GB) in the previous run.
-In the new run, I set memory limit to 200GB.</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
-<file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="F3" dT="2022-09-23T03:40:15.25" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{A3DE0894-D222-4604-B6B6-2E7833CF63F7}">
     <text>Downloading</text>
@@ -2275,10 +2270,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="42"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
@@ -2309,7 +2304,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:N7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2320,40 +2315,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="50.1" customHeight="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="M1" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
+      <c r="F1" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="M1" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="50"/>
       <c r="F2" s="9">
         <v>5</v>
       </c>
@@ -2392,13 +2387,13 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="68.25" customHeight="1">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="C3" s="42" t="s">
+      <c r="B3" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="41" t="s">
         <v>71</v>
       </c>
       <c r="D3" s="10">
@@ -2406,135 +2401,135 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="I3" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="H3" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>89</v>
-      </c>
       <c r="J3" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="K3" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="M3" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="K3" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="M3" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="N3" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="O3" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="P3" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q3" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="N3" s="45" t="s">
-        <v>122</v>
-      </c>
-      <c r="O3" s="45" t="s">
-        <v>123</v>
-      </c>
-      <c r="P3" s="45" t="s">
+      <c r="R3" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="Q3" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="R3" s="45" t="s">
-        <v>127</v>
-      </c>
     </row>
     <row r="4" spans="1:18" ht="75" customHeight="1">
-      <c r="A4" s="47"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="42"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="41"/>
       <c r="D4" s="10">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="45" t="s">
-        <v>108</v>
-      </c>
-      <c r="G4" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="H4" s="45" t="s">
+      <c r="F4" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="I4" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="J4" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="I4" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="J4" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="K4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
+      <c r="K4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="46"/>
     </row>
     <row r="5" spans="1:18" ht="36" customHeight="1">
-      <c r="A5" s="47"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="42"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="10">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
     </row>
     <row r="6" spans="1:18" ht="36" customHeight="1">
-      <c r="A6" s="47"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="42"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="41"/>
       <c r="D6" s="10">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
     </row>
     <row r="7" spans="1:18" ht="36" customHeight="1">
-      <c r="A7" s="47"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="42"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="10">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="46"/>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="2"/>
@@ -2545,139 +2540,139 @@
       <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:18" ht="54" customHeight="1">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="49" t="s">
+      <c r="B9" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="44" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="10">
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="45" t="s">
+      <c r="F9" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="H9" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="I9" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="J9" s="45" t="s">
-        <v>107</v>
-      </c>
-      <c r="K9" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="M9" s="45" t="s">
+      <c r="I9" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="J9" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="K9" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="M9" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="N9" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="O9" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="N9" s="45" t="s">
+      <c r="P9" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="O9" s="45" t="s">
+      <c r="Q9" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="P9" s="45" t="s">
+      <c r="R9" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="Q9" s="45" t="s">
-        <v>132</v>
-      </c>
-      <c r="R9" s="45" t="s">
-        <v>133</v>
-      </c>
     </row>
     <row r="10" spans="1:18" ht="54" customHeight="1">
-      <c r="A10" s="47"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="49"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="44"/>
       <c r="D10" s="10">
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="45"/>
-      <c r="Q10" s="45"/>
-      <c r="R10" s="45"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="46"/>
     </row>
     <row r="11" spans="1:18" ht="54" customHeight="1">
-      <c r="A11" s="47"/>
-      <c r="B11" s="55"/>
-      <c r="C11" s="49"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="10">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="45"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="45"/>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="45"/>
-      <c r="R11" s="45"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="46"/>
+      <c r="Q11" s="46"/>
+      <c r="R11" s="46"/>
     </row>
     <row r="12" spans="1:18" ht="54" customHeight="1">
-      <c r="A12" s="47"/>
-      <c r="B12" s="55"/>
-      <c r="C12" s="49"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="10">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="45"/>
-      <c r="R12" s="45"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="46"/>
+      <c r="P12" s="46"/>
+      <c r="Q12" s="46"/>
+      <c r="R12" s="46"/>
     </row>
     <row r="13" spans="1:18" ht="54" customHeight="1">
-      <c r="A13" s="47"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="49"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="10">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="45"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="45"/>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="45"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="46"/>
+      <c r="O13" s="46"/>
+      <c r="P13" s="46"/>
+      <c r="Q13" s="46"/>
+      <c r="R13" s="46"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="5"/>
@@ -2690,14 +2685,14 @@
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:18" ht="94.5" customHeight="1">
-      <c r="A15" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
+      <c r="A15" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
@@ -2711,6 +2706,28 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="M3:M7"/>
+    <mergeCell ref="N3:N7"/>
+    <mergeCell ref="O3:O7"/>
+    <mergeCell ref="P3:P7"/>
+    <mergeCell ref="M9:M13"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="N9:N13"/>
+    <mergeCell ref="O9:O13"/>
+    <mergeCell ref="P9:P13"/>
+    <mergeCell ref="Q9:Q13"/>
+    <mergeCell ref="R9:R13"/>
+    <mergeCell ref="Q3:Q7"/>
+    <mergeCell ref="R3:R7"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="K9:K13"/>
     <mergeCell ref="J9:J13"/>
@@ -2726,28 +2743,6 @@
     <mergeCell ref="K3:K7"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="H4:H7"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="P3:P7"/>
-    <mergeCell ref="M9:M13"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="N9:N13"/>
-    <mergeCell ref="O9:O13"/>
-    <mergeCell ref="P9:P13"/>
-    <mergeCell ref="Q9:Q13"/>
-    <mergeCell ref="R9:R13"/>
-    <mergeCell ref="Q3:Q7"/>
-    <mergeCell ref="R3:R7"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="M3:M7"/>
-    <mergeCell ref="N3:N7"/>
-    <mergeCell ref="O3:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2762,8 +2757,8 @@
   </sheetPr>
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2776,32 +2771,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:15" ht="45">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="50"/>
       <c r="F2" s="9" t="s">
         <v>38</v>
       </c>
@@ -2812,98 +2807,98 @@
         <v>39</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="45" customHeight="1">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" s="42" t="s">
+      <c r="B3" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="41" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="45" t="s">
-        <v>146</v>
-      </c>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
+      <c r="F3" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:15" ht="45" customHeight="1">
-      <c r="A4" s="47"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="42"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="41"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="45" t="s">
-        <v>147</v>
-      </c>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
+      <c r="F4" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="45" customHeight="1">
-      <c r="A5" s="47"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="42"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="45" t="s">
-        <v>148</v>
-      </c>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
+      <c r="F5" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="45" customHeight="1">
-      <c r="A6" s="47"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="42"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="41"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="45" t="s">
-        <v>149</v>
-      </c>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
+      <c r="F6" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:15" ht="45" customHeight="1">
-      <c r="A7" s="47"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="42"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="45" t="s">
-        <v>150</v>
-      </c>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
+      <c r="F7" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
       <c r="K7" s="2"/>
@@ -2926,7 +2921,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>44</v>
@@ -2935,11 +2930,11 @@
         <v>34</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="45" t="s">
-        <v>144</v>
-      </c>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
+      <c r="F9" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
       <c r="J9" s="4"/>
       <c r="K9" s="5"/>
     </row>
@@ -2954,78 +2949,79 @@
       <c r="J10" s="4"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:15" ht="45">
-      <c r="A11" s="47" t="s">
-        <v>193</v>
-      </c>
-      <c r="B11" s="46" t="s">
-        <v>137</v>
-      </c>
-      <c r="C11" s="49"/>
+    <row r="11" spans="1:15" ht="30" customHeight="1">
+      <c r="A11" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" s="44"/>
       <c r="D11" s="2">
         <v>145879</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="37" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="47"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="49"/>
+    <row r="12" spans="1:15" ht="30" customHeight="1">
+      <c r="A12" s="43"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="2">
         <v>200437</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="F12" s="48" t="s">
+        <v>222</v>
+      </c>
       <c r="I12" s="2"/>
       <c r="J12" s="4"/>
       <c r="K12" s="5"/>
       <c r="O12" s="33"/>
     </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="47"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="49"/>
+    <row r="13" spans="1:15" ht="30" customHeight="1">
+      <c r="A13" s="43"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="2">
         <v>310111</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="48"/>
       <c r="G13" s="5"/>
       <c r="I13" s="2"/>
       <c r="J13" s="4"/>
       <c r="K13" s="5"/>
       <c r="O13" s="33"/>
     </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="47"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="49"/>
+    <row r="14" spans="1:15" ht="30" customHeight="1">
+      <c r="A14" s="43"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="2">
         <v>528401</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="5"/>
+      <c r="F14" s="48"/>
       <c r="G14" s="5"/>
       <c r="I14" s="2"/>
       <c r="J14" s="4"/>
       <c r="K14" s="5"/>
       <c r="O14" s="33"/>
     </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="47"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="49"/>
+    <row r="15" spans="1:15" ht="30" customHeight="1">
+      <c r="A15" s="43"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="2">
         <v>1076753</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="5"/>
+      <c r="F15" s="48"/>
       <c r="G15" s="5"/>
       <c r="I15" s="2"/>
       <c r="J15" s="4"/>
@@ -3060,13 +3056,13 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H17" s="27" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -3088,84 +3084,84 @@
       <c r="O18" s="33"/>
     </row>
     <row r="19" spans="1:15" ht="60" customHeight="1">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="46" t="s">
-        <v>164</v>
-      </c>
-      <c r="C19" s="48" t="s">
+      <c r="B19" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="C19" s="47" t="s">
         <v>56</v>
       </c>
       <c r="D19" s="2">
         <v>145879</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="45" t="s">
-        <v>159</v>
-      </c>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
+      <c r="F19" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
       <c r="O19" s="33"/>
     </row>
     <row r="20" spans="1:15" ht="60" customHeight="1">
-      <c r="A20" s="47"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="48"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="47"/>
       <c r="D20" s="2">
         <v>200437</v>
       </c>
       <c r="E20" s="5"/>
-      <c r="F20" s="45" t="s">
-        <v>160</v>
-      </c>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
+      <c r="F20" s="46" t="s">
+        <v>158</v>
+      </c>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
       <c r="O20" s="33"/>
     </row>
     <row r="21" spans="1:15" ht="60" customHeight="1">
-      <c r="A21" s="47"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="48"/>
+      <c r="A21" s="43"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="47"/>
       <c r="D21" s="2">
         <v>310111</v>
       </c>
       <c r="E21" s="5"/>
-      <c r="F21" s="45" t="s">
-        <v>161</v>
-      </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
+      <c r="F21" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
       <c r="O21" s="33"/>
     </row>
     <row r="22" spans="1:15" ht="60" customHeight="1">
-      <c r="A22" s="47"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="48"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="47"/>
       <c r="D22" s="2">
         <v>528401</v>
       </c>
       <c r="E22" s="5"/>
-      <c r="F22" s="45" t="s">
-        <v>162</v>
-      </c>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
+      <c r="F22" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
       <c r="O22" s="33"/>
     </row>
     <row r="23" spans="1:15" ht="60" customHeight="1">
-      <c r="A23" s="47"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="48"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="47"/>
       <c r="D23" s="2">
         <v>1076753</v>
       </c>
       <c r="E23" s="5"/>
-      <c r="F23" s="45" t="s">
-        <v>163</v>
-      </c>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
+      <c r="F23" s="46" t="s">
+        <v>161</v>
+      </c>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
       <c r="O23" s="33"/>
     </row>
     <row r="24" spans="1:15">
@@ -3185,8 +3181,8 @@
       <c r="A25" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="46" t="s">
-        <v>175</v>
+      <c r="B25" s="42" t="s">
+        <v>173</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>67</v>
@@ -3198,7 +3194,7 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="27" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="5"/>
@@ -3206,7 +3202,7 @@
     </row>
     <row r="26" spans="1:15" ht="30" customHeight="1">
       <c r="A26" s="10"/>
-      <c r="B26" s="46"/>
+      <c r="B26" s="42"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -3216,11 +3212,11 @@
       <c r="K26" s="5"/>
     </row>
     <row r="27" spans="1:15" ht="60" customHeight="1">
-      <c r="A27" s="47" t="s">
+      <c r="A27" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="46"/>
-      <c r="C27" s="50" t="s">
+      <c r="B27" s="42"/>
+      <c r="C27" s="45" t="s">
         <v>64</v>
       </c>
       <c r="D27" s="2">
@@ -3228,71 +3224,71 @@
       </c>
       <c r="E27" s="5"/>
       <c r="H27" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="I27" s="45" t="s">
-        <v>180</v>
+        <v>181</v>
+      </c>
+      <c r="I27" s="46" t="s">
+        <v>178</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:15" ht="60" customHeight="1">
-      <c r="A28" s="47"/>
-      <c r="B28" s="46"/>
-      <c r="C28" s="50"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="45"/>
       <c r="D28" s="2">
         <v>200437</v>
       </c>
       <c r="E28" s="5"/>
       <c r="H28" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="I28" s="45"/>
+        <v>182</v>
+      </c>
+      <c r="I28" s="46"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:15" ht="60" customHeight="1">
-      <c r="A29" s="47"/>
-      <c r="B29" s="46"/>
-      <c r="C29" s="50"/>
+      <c r="A29" s="43"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="45"/>
       <c r="D29" s="2">
         <v>310111</v>
       </c>
       <c r="E29" s="5"/>
       <c r="H29" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="I29" s="45"/>
+        <v>183</v>
+      </c>
+      <c r="I29" s="46"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:15" ht="60" customHeight="1">
-      <c r="A30" s="47"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="50"/>
+      <c r="A30" s="43"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="45"/>
       <c r="D30" s="2">
         <v>528401</v>
       </c>
       <c r="E30" s="5"/>
       <c r="H30" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="I30" s="45"/>
+        <v>184</v>
+      </c>
+      <c r="I30" s="46"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:15" ht="60" customHeight="1">
-      <c r="A31" s="47"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="50"/>
+      <c r="A31" s="43"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="45"/>
       <c r="D31" s="2">
         <v>1076753</v>
       </c>
       <c r="E31" s="5"/>
       <c r="H31" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="I31" s="45"/>
+        <v>185</v>
+      </c>
+      <c r="I31" s="46"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
@@ -3310,14 +3306,14 @@
       <c r="K32" s="5"/>
     </row>
     <row r="33" spans="1:11" ht="75" customHeight="1">
-      <c r="A33" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="B33" s="42"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="42"/>
+      <c r="A33" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -3335,21 +3331,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="B25:B31"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="I27:I31"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
+  <mergeCells count="31">
     <mergeCell ref="A33:F33"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="A1:A2"/>
@@ -3366,6 +3348,21 @@
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="A19:A23"/>
     <mergeCell ref="B19:B23"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="A27:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3379,8 +3376,8 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3396,24 +3393,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="46.5" customHeight="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="50" t="s">
         <v>20</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -3422,16 +3419,16 @@
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14" ht="30.75" customHeight="1">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
       <c r="E2" s="1"/>
       <c r="F2" s="9" t="s">
         <v>39</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>38</v>
@@ -3448,7 +3445,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>49</v>
@@ -3458,13 +3455,13 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="27" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I3" s="2"/>
       <c r="N3" s="2"/>
@@ -3486,7 +3483,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>45</v>
@@ -3496,7 +3493,7 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="27" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G5" s="26" t="s">
         <v>21</v>
@@ -3518,18 +3515,18 @@
     </row>
     <row r="7" spans="1:14" ht="75">
       <c r="A7" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="28" t="s">
-        <v>194</v>
+      <c r="F7" s="27" t="s">
+        <v>192</v>
       </c>
       <c r="I7" s="5"/>
       <c r="N7" s="5"/>
@@ -3557,10 +3554,10 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="26" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="N9" s="5"/>
     </row>
@@ -3574,13 +3571,13 @@
         <v>39</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>38</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="N10" s="5"/>
     </row>
@@ -3599,16 +3596,16 @@
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="27" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I11" s="32" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="N11" s="5"/>
     </row>
@@ -3627,8 +3624,8 @@
       <c r="A13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="46" t="s">
-        <v>175</v>
+      <c r="B13" s="42" t="s">
+        <v>173</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>66</v>
@@ -3638,17 +3635,17 @@
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="27" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H13" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I13" s="10"/>
       <c r="N13" s="5"/>
     </row>
     <row r="14" spans="1:14" ht="45">
       <c r="A14" s="5"/>
-      <c r="B14" s="46"/>
+      <c r="B14" s="42"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -3656,33 +3653,33 @@
         <v>39</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>38</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N14" s="5"/>
     </row>
     <row r="15" spans="1:14" ht="54" customHeight="1">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="46"/>
-      <c r="C15" s="50" t="s">
+      <c r="B15" s="42"/>
+      <c r="C15" s="45" t="s">
         <v>65</v>
       </c>
       <c r="D15" s="5">
         <v>145879</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="45" t="s">
-        <v>169</v>
+      <c r="F15" s="46" t="s">
+        <v>167</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I15" s="16" t="s">
         <v>22</v>
@@ -3690,16 +3687,16 @@
       <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:14" ht="54" customHeight="1">
-      <c r="A16" s="47"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="50"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="45"/>
       <c r="D16" s="5">
         <v>200437</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="45"/>
+      <c r="F16" s="46"/>
       <c r="H16" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I16" s="16" t="s">
         <v>22</v>
@@ -3707,16 +3704,16 @@
       <c r="N16" s="5"/>
     </row>
     <row r="17" spans="1:14" ht="54" customHeight="1">
-      <c r="A17" s="47"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="50"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="45"/>
       <c r="D17" s="5">
         <v>310111</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="45"/>
+      <c r="F17" s="46"/>
       <c r="H17" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I17" s="21" t="s">
         <v>22</v>
@@ -3724,16 +3721,16 @@
       <c r="N17" s="5"/>
     </row>
     <row r="18" spans="1:14" ht="54" customHeight="1">
-      <c r="A18" s="47"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="50"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="45"/>
       <c r="D18" s="5">
         <v>528401</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="45"/>
+      <c r="F18" s="46"/>
       <c r="H18" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>22</v>
@@ -3741,16 +3738,16 @@
       <c r="N18" s="5"/>
     </row>
     <row r="19" spans="1:14" ht="54" customHeight="1">
-      <c r="A19" s="47"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="50"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="45"/>
       <c r="D19" s="5">
         <v>1076753</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="45"/>
+      <c r="F19" s="46"/>
       <c r="H19" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I19" s="21" t="s">
         <v>22</v>
@@ -3790,16 +3787,16 @@
       <c r="N21" s="5"/>
     </row>
     <row r="22" spans="1:14" ht="105" customHeight="1">
-      <c r="A22" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
+      <c r="A22" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" t="s">
@@ -3813,16 +3810,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="F15:F19"/>
+    <mergeCell ref="B13:B19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="A15:A19"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="F15:F19"/>
-    <mergeCell ref="B13:B19"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="A15:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3837,8 +3834,8 @@
   </sheetPr>
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42:I44"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33:H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3851,29 +3848,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+    </row>
+    <row r="2" spans="1:9" ht="30">
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="50"/>
       <c r="F2" s="9" t="s">
         <v>38</v>
       </c>
@@ -3883,15 +3880,18 @@
       <c r="H2" s="9" t="s">
         <v>39</v>
       </c>
+      <c r="I2" s="8" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="45">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="44" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="2">
@@ -3899,75 +3899,80 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="51" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G3" s="51"/>
-      <c r="H3" s="38" t="s">
-        <v>153</v>
+      <c r="H3"/>
+      <c r="I3" s="38" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45">
-      <c r="A4" s="47"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="49"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="51" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G4" s="51"/>
-      <c r="H4" s="38" t="s">
-        <v>154</v>
+      <c r="H4"/>
+      <c r="I4" s="38" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45">
-      <c r="A5" s="47"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="49"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="51" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G5" s="51"/>
-      <c r="H5" s="38" t="s">
-        <v>155</v>
+      <c r="H5"/>
+      <c r="I5" s="38" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="45">
-      <c r="A6" s="47"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="49"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="51" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G6" s="51"/>
-      <c r="H6" s="38" t="s">
-        <v>156</v>
+      <c r="H6"/>
+      <c r="I6" s="38" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45">
-      <c r="A7" s="47"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="49"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="51" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G7" s="51"/>
-      <c r="H7" s="38" t="s">
-        <v>157</v>
+      <c r="H7"/>
+      <c r="I7" s="38" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30">
@@ -3986,99 +3991,99 @@
         <v>39</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="45">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="C9" s="42" t="s">
+      <c r="B9" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="41" t="s">
         <v>71</v>
       </c>
       <c r="D9" s="2">
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="G9" s="45" t="s">
-        <v>85</v>
+      <c r="F9" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>83</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="45">
-      <c r="A10" s="47"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="42"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="41"/>
       <c r="D10" s="2">
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="34" t="s">
-        <v>207</v>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="28" t="s">
+        <v>205</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="45">
-      <c r="A11" s="47"/>
-      <c r="B11" s="55"/>
-      <c r="C11" s="42"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="2">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="34" t="s">
-        <v>208</v>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="28" t="s">
+        <v>206</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="45">
-      <c r="A12" s="47"/>
-      <c r="B12" s="55"/>
-      <c r="C12" s="42"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="2">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="34" t="s">
-        <v>209</v>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="28" t="s">
+        <v>207</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45">
-      <c r="A13" s="47"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="42"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="41"/>
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="34" t="s">
-        <v>210</v>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="28" t="s">
+        <v>208</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -4098,82 +4103,82 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="54" customHeight="1">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="C15" s="49" t="s">
+      <c r="B15" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="C15" s="44" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="2">
         <v>145879</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="45" t="s">
-        <v>138</v>
-      </c>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45" t="s">
-        <v>176</v>
+      <c r="F15" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="54" customHeight="1">
-      <c r="A16" s="47"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="49"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="44"/>
       <c r="D16" s="2">
         <v>200437</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="45" t="s">
-        <v>139</v>
-      </c>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
+      <c r="F16" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
     </row>
     <row r="17" spans="1:9" ht="54" customHeight="1">
-      <c r="A17" s="47"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="49"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="44"/>
       <c r="D17" s="2">
         <v>310111</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="45" t="s">
-        <v>140</v>
-      </c>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
+      <c r="F17" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
     </row>
     <row r="18" spans="1:9" ht="54" customHeight="1">
-      <c r="A18" s="47"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="49"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="2">
         <v>528401</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="45" t="s">
-        <v>141</v>
-      </c>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
+      <c r="F18" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
     </row>
     <row r="19" spans="1:9" ht="54" customHeight="1">
-      <c r="A19" s="47"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="49"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="2">
         <v>1076753</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
+      <c r="F19" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
     </row>
     <row r="20" spans="1:9" ht="54" customHeight="1">
       <c r="A20" s="10"/>
@@ -4191,63 +4196,69 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" customHeight="1">
-      <c r="A21" s="47" t="s">
-        <v>216</v>
-      </c>
-      <c r="B21" s="46" t="s">
+    <row r="21" spans="1:9" ht="45" customHeight="1">
+      <c r="A21" s="43" t="s">
+        <v>214</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>211</v>
+      </c>
+      <c r="C21" s="44" t="s">
         <v>213</v>
-      </c>
-      <c r="C21" s="49" t="s">
-        <v>215</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="52" t="s">
-        <v>217</v>
+      <c r="F21" s="28" t="s">
+        <v>215</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="9"/>
     </row>
-    <row r="22" spans="1:9" ht="30" customHeight="1">
-      <c r="A22" s="47"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="49"/>
+    <row r="22" spans="1:9" ht="45" customHeight="1">
+      <c r="A22" s="43"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="52"/>
+      <c r="F22" s="28" t="s">
+        <v>215</v>
+      </c>
       <c r="G22" s="10"/>
       <c r="H22" s="9"/>
     </row>
-    <row r="23" spans="1:9" ht="30" customHeight="1">
-      <c r="A23" s="47"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="49"/>
+    <row r="23" spans="1:9" ht="45" customHeight="1">
+      <c r="A23" s="43"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="44"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="52"/>
+      <c r="F23" s="28" t="s">
+        <v>221</v>
+      </c>
       <c r="G23" s="10"/>
       <c r="H23" s="9"/>
     </row>
-    <row r="24" spans="1:9" ht="30" customHeight="1">
-      <c r="A24" s="47"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="49"/>
+    <row r="24" spans="1:9" ht="45" customHeight="1">
+      <c r="A24" s="43"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="44"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="52" t="s">
-        <v>218</v>
+      <c r="F24" s="28" t="s">
+        <v>216</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="9"/>
     </row>
-    <row r="25" spans="1:9" ht="30" customHeight="1">
-      <c r="A25" s="47"/>
-      <c r="B25" s="46"/>
-      <c r="C25" s="49"/>
+    <row r="25" spans="1:9" ht="45" customHeight="1">
+      <c r="A25" s="43"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="44"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="52"/>
+      <c r="F25" s="28" t="s">
+        <v>216</v>
+      </c>
       <c r="G25" s="10"/>
       <c r="H25" s="9"/>
     </row>
@@ -4262,42 +4273,42 @@
       <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:9" ht="60" customHeight="1">
-      <c r="A27" s="48" t="s">
-        <v>193</v>
-      </c>
-      <c r="B27" s="46" t="s">
-        <v>137</v>
-      </c>
-      <c r="C27" s="49" t="s">
-        <v>220</v>
+      <c r="A27" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="B27" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="44" t="s">
+        <v>218</v>
       </c>
       <c r="D27" s="2">
         <v>145879</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="20"/>
-      <c r="H27" s="27" t="s">
-        <v>195</v>
+      <c r="H27" s="28" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="60" customHeight="1">
-      <c r="A28" s="48"/>
-      <c r="B28" s="46"/>
-      <c r="C28" s="49"/>
+      <c r="A28" s="47"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="44"/>
       <c r="D28" s="2">
         <v>200437</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="20"/>
       <c r="G28" s="10"/>
-      <c r="H28" s="34" t="s">
-        <v>198</v>
+      <c r="H28" s="28" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="60" customHeight="1">
-      <c r="A29" s="48"/>
-      <c r="B29" s="46"/>
-      <c r="C29" s="49"/>
+      <c r="A29" s="47"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="44"/>
       <c r="D29" s="2">
         <v>310111</v>
       </c>
@@ -4305,34 +4316,36 @@
       <c r="F29" s="20"/>
       <c r="G29" s="10"/>
       <c r="H29" s="39" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="60" customHeight="1">
-      <c r="A30" s="48"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="49"/>
+      <c r="A30" s="47"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="44"/>
       <c r="D30" s="2">
         <v>528401</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="20"/>
       <c r="G30" s="10"/>
-      <c r="H30" s="30" t="s">
-        <v>219</v>
+      <c r="H30" s="28" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="60" customHeight="1">
-      <c r="A31" s="48"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="49"/>
+      <c r="A31" s="47"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="44"/>
       <c r="D31" s="2">
         <v>1076753</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="20"/>
       <c r="G31" s="10"/>
-      <c r="H31" s="40"/>
+      <c r="H31" s="28" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="32" spans="1:9" ht="30">
       <c r="A32" s="2"/>
@@ -4350,89 +4363,87 @@
         <v>39</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="49" t="s">
+      <c r="C33" s="44" t="s">
         <v>61</v>
       </c>
       <c r="D33" s="5">
         <v>145879</v>
       </c>
       <c r="E33" s="2"/>
-      <c r="F33" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="G33" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="H33" s="60" t="s">
-        <v>214</v>
-      </c>
-      <c r="I33" s="45" t="s">
-        <v>78</v>
+      <c r="F33" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="G33" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="H33" s="55" t="s">
+        <v>212</v>
+      </c>
+      <c r="I33" s="46" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30" customHeight="1">
-      <c r="A34" s="47"/>
-      <c r="B34" s="49"/>
-      <c r="C34" s="49"/>
+      <c r="A34" s="43"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
       <c r="D34" s="5">
         <v>200437</v>
       </c>
       <c r="E34" s="2"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
-      <c r="H34" s="60"/>
-      <c r="I34" s="45"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="46"/>
     </row>
     <row r="35" spans="1:10" ht="30" customHeight="1">
-      <c r="A35" s="47"/>
-      <c r="B35" s="49"/>
-      <c r="C35" s="49"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
       <c r="D35" s="5">
         <v>310111</v>
       </c>
       <c r="E35" s="2"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="45"/>
-      <c r="H35" s="60"/>
-      <c r="I35" s="45"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="46"/>
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1">
-      <c r="A36" s="47"/>
-      <c r="B36" s="49"/>
-      <c r="C36" s="49"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
       <c r="D36" s="5">
         <v>528401</v>
       </c>
       <c r="E36" s="2"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="52" t="s">
-        <v>214</v>
-      </c>
-      <c r="I36" s="45"/>
-    </row>
-    <row r="37" spans="1:10" ht="30" customHeight="1">
-      <c r="A37" s="47"/>
-      <c r="B37" s="49"/>
-      <c r="C37" s="49"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="46"/>
+    </row>
+    <row r="37" spans="1:10" ht="45" customHeight="1">
+      <c r="A37" s="43"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="44"/>
       <c r="D37" s="5">
         <v>1076753</v>
       </c>
       <c r="E37" s="2"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="45"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="46"/>
       <c r="J37" s="8"/>
     </row>
     <row r="38" spans="1:10">
@@ -4460,23 +4471,23 @@
         <v>43</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="60">
-      <c r="A40" s="48" t="s">
+      <c r="A40" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="46" t="s">
-        <v>164</v>
-      </c>
-      <c r="C40" s="47" t="s">
+      <c r="B40" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="C40" s="43" t="s">
         <v>54</v>
       </c>
       <c r="D40" s="5">
@@ -4486,16 +4497,16 @@
       <c r="F40"/>
       <c r="G40"/>
       <c r="I40" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="J40" s="41" t="s">
-        <v>197</v>
+        <v>149</v>
+      </c>
+      <c r="J40" s="40" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="75">
-      <c r="A41" s="48"/>
-      <c r="B41" s="46"/>
-      <c r="C41" s="47"/>
+      <c r="A41" s="47"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="43"/>
       <c r="D41" s="5">
         <v>200437</v>
       </c>
@@ -4503,60 +4514,60 @@
       <c r="F41"/>
       <c r="G41"/>
       <c r="I41" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="J41" s="41" t="s">
-        <v>199</v>
+        <v>150</v>
+      </c>
+      <c r="J41" s="40" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="45" customHeight="1">
-      <c r="A42" s="48"/>
-      <c r="B42" s="46"/>
-      <c r="C42" s="47"/>
+      <c r="A42" s="47"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="43"/>
       <c r="D42" s="5">
         <v>310111</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42"/>
       <c r="G42"/>
-      <c r="I42" s="45" t="s">
-        <v>158</v>
-      </c>
-      <c r="J42" s="41" t="s">
-        <v>202</v>
+      <c r="I42" s="46" t="s">
+        <v>156</v>
+      </c>
+      <c r="J42" s="40" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="45" customHeight="1">
-      <c r="A43" s="48"/>
-      <c r="B43" s="46"/>
-      <c r="C43" s="47"/>
+      <c r="A43" s="47"/>
+      <c r="B43" s="42"/>
+      <c r="C43" s="43"/>
       <c r="D43" s="5">
         <v>528401</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43"/>
       <c r="G43"/>
-      <c r="I43" s="45"/>
-      <c r="J43" s="41" t="s">
-        <v>200</v>
+      <c r="I43" s="46"/>
+      <c r="J43" s="40" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="60">
-      <c r="A44" s="48"/>
-      <c r="B44" s="46"/>
-      <c r="C44" s="47"/>
+      <c r="A44" s="47"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="43"/>
       <c r="D44" s="5">
         <v>1076753</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44"/>
       <c r="G44"/>
-      <c r="H44" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="I44" s="45"/>
-      <c r="J44" s="41" t="s">
-        <v>201</v>
+      <c r="H44" s="34" t="s">
+        <v>199</v>
+      </c>
+      <c r="I44" s="46"/>
+      <c r="J44" s="40" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -4570,13 +4581,13 @@
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:10" ht="54" customHeight="1">
-      <c r="A46" s="48" t="s">
+      <c r="A46" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B46" s="46" t="s">
-        <v>175</v>
-      </c>
-      <c r="C46" s="53" t="s">
+      <c r="B46" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="C46" s="52" t="s">
         <v>63</v>
       </c>
       <c r="D46" s="5">
@@ -4586,13 +4597,13 @@
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
       <c r="H46" s="27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="54" customHeight="1">
-      <c r="A47" s="48"/>
-      <c r="B47" s="46"/>
-      <c r="C47" s="54"/>
+      <c r="A47" s="47"/>
+      <c r="B47" s="42"/>
+      <c r="C47" s="53"/>
       <c r="D47" s="5">
         <v>200437</v>
       </c>
@@ -4600,13 +4611,13 @@
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
       <c r="H47" s="27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="54" customHeight="1">
-      <c r="A48" s="48"/>
-      <c r="B48" s="46"/>
-      <c r="C48" s="54"/>
+      <c r="A48" s="47"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="53"/>
       <c r="D48" s="5">
         <v>310111</v>
       </c>
@@ -4614,13 +4625,13 @@
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
       <c r="H48" s="27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="54" customHeight="1">
-      <c r="A49" s="48"/>
-      <c r="B49" s="46"/>
-      <c r="C49" s="54"/>
+      <c r="A49" s="47"/>
+      <c r="B49" s="42"/>
+      <c r="C49" s="53"/>
       <c r="D49" s="5">
         <v>528401</v>
       </c>
@@ -4628,13 +4639,13 @@
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
       <c r="H49" s="27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="54" customHeight="1">
-      <c r="A50" s="48"/>
-      <c r="B50" s="46"/>
-      <c r="C50" s="54"/>
+      <c r="A50" s="47"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="53"/>
       <c r="D50" s="5">
         <v>1076753</v>
       </c>
@@ -4642,12 +4653,12 @@
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
       <c r="H50" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="5"/>
-      <c r="B51" s="46"/>
+      <c r="B51" s="42"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
@@ -4659,7 +4670,7 @@
       <c r="A52" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B52" s="46"/>
+      <c r="B52" s="42"/>
       <c r="C52" s="19" t="s">
         <v>70</v>
       </c>
@@ -4670,7 +4681,7 @@
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
       <c r="H52" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -4694,14 +4705,14 @@
       <c r="H54" s="10"/>
     </row>
     <row r="55" spans="1:8" ht="94.5" customHeight="1">
-      <c r="A55" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="B55" s="42"/>
-      <c r="C55" s="42"/>
-      <c r="D55" s="42"/>
-      <c r="E55" s="42"/>
-      <c r="F55" s="42"/>
+      <c r="A55" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="B55" s="41"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="41"/>
+      <c r="E55" s="41"/>
+      <c r="F55" s="41"/>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
@@ -4715,18 +4726,24 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="51">
-    <mergeCell ref="B33:B37"/>
+  <mergeCells count="48">
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="I42:I44"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H15:H19"/>
+    <mergeCell ref="I33:I37"/>
+    <mergeCell ref="H33:H37"/>
+    <mergeCell ref="G33:G37"/>
+    <mergeCell ref="C33:C37"/>
     <mergeCell ref="A33:A37"/>
-    <mergeCell ref="H33:H35"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B46:B52"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -4739,38 +4756,29 @@
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="A3:A7"/>
-    <mergeCell ref="F9:F13"/>
-    <mergeCell ref="G9:G13"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="B40:B44"/>
-    <mergeCell ref="C40:C44"/>
     <mergeCell ref="B15:B19"/>
     <mergeCell ref="C15:C19"/>
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="A27:A31"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="F9:F13"/>
+    <mergeCell ref="G9:G13"/>
     <mergeCell ref="B27:B31"/>
     <mergeCell ref="C27:C31"/>
     <mergeCell ref="C21:C25"/>
     <mergeCell ref="B21:B25"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="F33:F37"/>
-    <mergeCell ref="G33:G37"/>
-    <mergeCell ref="C33:C37"/>
-    <mergeCell ref="I42:I44"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H15:H19"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="I33:I37"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B33:B37"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="B40:B44"/>
+    <mergeCell ref="C40:C44"/>
+    <mergeCell ref="F33:F37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4785,8 +4793,8 @@
   </sheetPr>
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4799,29 +4807,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="49.5" customHeight="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="50" t="s">
         <v>20</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="44"/>
+      <c r="G1" s="50"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="43"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="50"/>
       <c r="E2" s="1"/>
       <c r="F2" s="9" t="s">
         <v>39</v>
@@ -4831,13 +4839,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="36" customHeight="1">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="C3" s="42" t="s">
+      <c r="B3" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="41" t="s">
         <v>51</v>
       </c>
       <c r="D3" s="2">
@@ -4845,55 +4853,55 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="36" customHeight="1">
-      <c r="A4" s="47"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="42"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="41"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="36" customHeight="1">
-      <c r="A5" s="47"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="42"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="36" customHeight="1">
-      <c r="A6" s="47"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="42"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="41"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1">
-      <c r="A7" s="47"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="42"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -4903,71 +4911,73 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="45" customHeight="1">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="46" t="s">
-        <v>145</v>
-      </c>
-      <c r="C9" s="49" t="s">
+      <c r="B9" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="44" t="s">
         <v>46</v>
       </c>
       <c r="D9" s="2">
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="45" t="s">
-        <v>177</v>
+      <c r="F9" s="46" t="s">
+        <v>175</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="45" customHeight="1">
-      <c r="A10" s="47"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="49"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="44"/>
       <c r="D10" s="2">
         <v>200437</v>
       </c>
-      <c r="F10" s="45"/>
+      <c r="F10" s="46"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="45" customHeight="1">
-      <c r="A11" s="47"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="49"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="2">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="45"/>
+      <c r="F11" s="27" t="s">
+        <v>175</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="45" customHeight="1">
-      <c r="A12" s="47"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="49"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="2">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="45" t="s">
-        <v>188</v>
+      <c r="F12" s="46" t="s">
+        <v>186</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="45" customHeight="1">
-      <c r="A13" s="47"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="49"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="45"/>
+      <c r="F13" s="46"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:8">
@@ -4979,61 +4989,61 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1">
-      <c r="A15" s="47" t="s">
-        <v>193</v>
-      </c>
-      <c r="B15" s="46" t="s">
-        <v>137</v>
-      </c>
-      <c r="C15" s="49"/>
+      <c r="A15" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="44"/>
       <c r="D15" s="2">
         <v>145879</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="56" t="s">
-        <v>196</v>
+      <c r="F15" s="55" t="s">
+        <v>194</v>
       </c>
       <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1">
-      <c r="A16" s="47"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="49"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="44"/>
       <c r="D16" s="2">
         <v>200437</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="56"/>
+      <c r="F16" s="55"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="47"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="49"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="44"/>
       <c r="D17" s="2">
         <v>310111</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="56"/>
+      <c r="F17" s="55"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="47"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="49"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="2">
         <v>528401</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="56"/>
+      <c r="F18" s="55"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="47"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="49"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="2">
         <v>1076753</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="56"/>
+      <c r="F19" s="55"/>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2"/>
@@ -5057,10 +5067,10 @@
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="26" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -5085,10 +5095,10 @@
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="26" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -5100,90 +5110,90 @@
       <c r="N24" s="12"/>
     </row>
     <row r="25" spans="1:14" ht="54" customHeight="1">
-      <c r="A25" s="47" t="s">
+      <c r="A25" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="46" t="s">
-        <v>175</v>
-      </c>
-      <c r="C25" s="53" t="s">
-        <v>94</v>
+      <c r="B25" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="C25" s="52" t="s">
+        <v>92</v>
       </c>
       <c r="D25" s="5">
         <v>145879</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N25" s="12"/>
     </row>
     <row r="26" spans="1:14" ht="54" customHeight="1">
-      <c r="A26" s="47"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="54"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="53"/>
       <c r="D26" s="5">
         <v>200437</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N26" s="12"/>
     </row>
     <row r="27" spans="1:14" ht="54" customHeight="1">
-      <c r="A27" s="47"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="54"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="53"/>
       <c r="D27" s="5">
         <v>310111</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="N27" s="12"/>
     </row>
     <row r="28" spans="1:14" ht="54" customHeight="1">
-      <c r="A28" s="47"/>
-      <c r="B28" s="46"/>
-      <c r="C28" s="54"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="53"/>
       <c r="D28" s="5">
         <v>528401</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="N28" s="12"/>
     </row>
     <row r="29" spans="1:14" ht="54" customHeight="1">
-      <c r="A29" s="47"/>
-      <c r="B29" s="46"/>
-      <c r="C29" s="54"/>
+      <c r="A29" s="43"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="53"/>
       <c r="D29" s="5">
         <v>1076753</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="N29" s="12"/>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="5"/>
-      <c r="B30" s="46"/>
+      <c r="B30" s="42"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="N30" s="12"/>
     </row>
     <row r="31" spans="1:14" ht="54" customHeight="1">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="53" t="s">
+      <c r="B31" s="42"/>
+      <c r="C31" s="52" t="s">
         <v>69</v>
       </c>
       <c r="D31" s="5">
@@ -5191,57 +5201,57 @@
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N31" s="12"/>
     </row>
     <row r="32" spans="1:14" ht="54" customHeight="1">
-      <c r="A32" s="47"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="54"/>
+      <c r="A32" s="43"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="53"/>
       <c r="D32" s="5">
         <v>200437</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="N32" s="12"/>
     </row>
     <row r="33" spans="1:7" ht="54" customHeight="1">
-      <c r="A33" s="47"/>
-      <c r="B33" s="46"/>
-      <c r="C33" s="54"/>
+      <c r="A33" s="43"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="53"/>
       <c r="D33" s="5">
         <v>310111</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="54" customHeight="1">
-      <c r="A34" s="47"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="54"/>
+      <c r="A34" s="43"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="53"/>
       <c r="D34" s="5">
         <v>528401</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="54" customHeight="1">
-      <c r="A35" s="47"/>
-      <c r="B35" s="46"/>
-      <c r="C35" s="54"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="53"/>
       <c r="D35" s="5">
         <v>1076753</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -5254,15 +5264,15 @@
       <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:7" ht="99.95" customHeight="1">
-      <c r="A37" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="42"/>
+      <c r="A37" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
@@ -5276,16 +5286,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F15:F19"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="A3:A7"/>
@@ -5299,6 +5299,16 @@
     <mergeCell ref="C9:C13"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="A9:A13"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F15:F19"/>
+    <mergeCell ref="F9:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5312,7 +5322,7 @@
   </sheetPr>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -5334,12 +5344,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -5385,7 +5395,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>47</v>
@@ -5394,16 +5404,16 @@
         <v>34</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>2</v>
@@ -5429,27 +5439,27 @@
       <c r="K4" s="2"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
     </row>
     <row r="7" spans="1:12" ht="90" customHeight="1">
-      <c r="A7" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
+      <c r="A7" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -5509,12 +5519,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -5556,99 +5566,99 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="C3" s="42" t="s">
+      <c r="B3" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="41" t="s">
         <v>49</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
-      <c r="E3" s="45" t="s">
-        <v>182</v>
-      </c>
-      <c r="F3" s="45" t="s">
-        <v>182</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>182</v>
-      </c>
-      <c r="H3" s="45" t="s">
-        <v>182</v>
-      </c>
-      <c r="I3" s="47" t="s">
+      <c r="E3" s="46" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>180</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>180</v>
+      </c>
+      <c r="H3" s="46" t="s">
+        <v>180</v>
+      </c>
+      <c r="I3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="57" t="s">
+      <c r="J3" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="43" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A4" s="47"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="42"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="41"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="47"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="43"/>
     </row>
     <row r="5" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A5" s="47"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="42"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="47"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="43"/>
     </row>
     <row r="6" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A6" s="47"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="42"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="41"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="47"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="43"/>
     </row>
     <row r="7" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A7" s="47"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="42"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="47"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="43"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="10"/>
@@ -5677,29 +5687,29 @@
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
     </row>
     <row r="11" spans="1:12" ht="99.95" customHeight="1">
-      <c r="A11" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
+      <c r="A11" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -5746,7 +5756,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5768,13 +5778,13 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
@@ -5799,7 +5809,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>7</v>
@@ -5819,29 +5829,29 @@
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="45">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>165</v>
-      </c>
-      <c r="C3" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="53" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="10">
         <v>145879</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>2</v>
@@ -5854,106 +5864,106 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="45">
-      <c r="A4" s="47"/>
-      <c r="B4" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" s="58"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="57"/>
       <c r="D4" s="10">
         <v>200437</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H4" s="34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I4" s="34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="3"/>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="45">
-      <c r="A5" s="47"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="58"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="10">
         <v>310111</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G5" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H5" s="34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I5" s="34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="3"/>
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:13" ht="45">
-      <c r="A6" s="47"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="58"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="10">
         <v>528401</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G6" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I6" s="34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="3"/>
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:13" ht="45">
-      <c r="A7" s="47"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="58"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="10">
         <v>1076753</v>
       </c>
       <c r="E7" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="F7" s="34" t="s">
-        <v>210</v>
-      </c>
-      <c r="G7" s="36" t="s">
+      <c r="I7" s="34" t="s">
         <v>78</v>
-      </c>
-      <c r="H7" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="I7" s="34" t="s">
-        <v>80</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="3"/>
@@ -5964,15 +5974,15 @@
       <c r="L8" s="5"/>
     </row>
     <row r="9" spans="1:13" ht="90" customHeight="1">
-      <c r="A9" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
+      <c r="A9" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -6006,14 +6016,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF7C9A9-BAE7-4BED-BECB-93E5F2CC9436}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF7C9A9-BAE7-4BED-BECB-93E5F2CC9436}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6025,28 +6035,26 @@
     <col min="5" max="6" width="9.7109375" customWidth="1"/>
     <col min="7" max="7" width="9.140625" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" style="17" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="17" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:11">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="10"/>
-    </row>
-    <row r="2" spans="1:12" ht="45">
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="10"/>
+    </row>
+    <row r="2" spans="1:11" ht="45">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
@@ -6071,27 +6079,24 @@
       <c r="H2" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>74</v>
+      <c r="I2" s="8" t="s">
+        <v>0</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="45" customHeight="1">
-      <c r="A3" s="47" t="s">
+    <row r="3" spans="1:11" ht="45" customHeight="1">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="C3" s="42" t="s">
+      <c r="B3" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="41" t="s">
         <v>51</v>
       </c>
       <c r="D3" s="2">
@@ -6106,26 +6111,23 @@
       <c r="G3" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="H3" s="34" t="s">
-        <v>189</v>
-      </c>
-      <c r="I3" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="J3" s="47" t="s">
+      <c r="H3" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="I3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="57" t="s">
+      <c r="J3" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="47" t="s">
+      <c r="K3" s="43" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="45" customHeight="1">
-      <c r="A4" s="47"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="42"/>
+    <row r="4" spans="1:11" ht="45" customHeight="1">
+      <c r="A4" s="43"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="41"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
@@ -6138,18 +6140,17 @@
       <c r="G4" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="34" t="s">
-        <v>190</v>
-      </c>
-      <c r="I4" s="59"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="47"/>
-    </row>
-    <row r="5" spans="1:12" ht="45" customHeight="1">
-      <c r="A5" s="47"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="42"/>
+      <c r="H4" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="I4" s="43"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="43"/>
+    </row>
+    <row r="5" spans="1:11" ht="45" customHeight="1">
+      <c r="A5" s="43"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
@@ -6162,18 +6163,17 @@
       <c r="G5" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="30" t="s">
-        <v>205</v>
-      </c>
-      <c r="I5" s="59"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="57"/>
-      <c r="L5" s="47"/>
-    </row>
-    <row r="6" spans="1:12" ht="45" customHeight="1">
-      <c r="A6" s="47"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="42"/>
+      <c r="H5" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="I5" s="43"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="43"/>
+    </row>
+    <row r="6" spans="1:11" ht="45" customHeight="1">
+      <c r="A6" s="43"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="41"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
@@ -6186,18 +6186,17 @@
       <c r="G6" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="34" t="s">
-        <v>191</v>
-      </c>
-      <c r="I6" s="59"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="47"/>
-    </row>
-    <row r="7" spans="1:12" ht="45" customHeight="1">
-      <c r="A7" s="47"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="42"/>
+      <c r="H6" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="I6" s="43"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="43"/>
+    </row>
+    <row r="7" spans="1:11" ht="45" customHeight="1">
+      <c r="A7" s="43"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
@@ -6210,15 +6209,14 @@
       <c r="G7" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="H7" s="34" t="s">
-        <v>192</v>
-      </c>
-      <c r="I7" s="59"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="47"/>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="H7" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="I7" s="43"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="43"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="10"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -6228,57 +6226,54 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="42" t="s">
+      <c r="J8" s="22"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-    </row>
-    <row r="11" spans="1:12" ht="75" customHeight="1">
-      <c r="A11" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+    </row>
+    <row r="11" spans="1:11" ht="75" customHeight="1">
+      <c r="A11" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="12"/>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:11">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:11">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -6299,12 +6294,12 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="42"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="5"/>
@@ -6315,24 +6310,22 @@
       <c r="F20" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="10">
     <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="L3:L7"/>
-    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="E1:H1"/>
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="A3:A7"/>
+    <mergeCell ref="I3:I7"/>
     <mergeCell ref="J3:J7"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="I3:I7"/>
     <mergeCell ref="A11:G11"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1" xr:uid="{BB77AC9D-0D8E-4A54-B106-A21D8FD578EE}"/>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{BB77AC9D-0D8E-4A54-B106-A21D8FD578EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added signeR on SBS_set1/Noiseless and SBS_set1/Moderate to Supp Tables and Supp Figures.
</commit_message>
<xml_diff>
--- a/documents/CPU_timing/mSigHdp-paper-tracking.xlsx
+++ b/documents/CPU_timing/mSigHdp-paper-tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\documents\CPU_timing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909B9E99-E08C-4C26-8158-1FFA3761F686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C539D5EB-80D9-44FB-AFFE-2F15EEC36215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13620" yWindow="630" windowWidth="14940" windowHeight="12045" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -109,7 +109,7 @@
     Needs re-download</t>
       </text>
     </comment>
-    <comment ref="J40" authorId="2" shapeId="0" xr:uid="{7879683C-1E68-4F58-975B-EB0BED2C30CE}">
+    <comment ref="H40" authorId="2" shapeId="0" xr:uid="{7879683C-1E68-4F58-975B-EB0BED2C30CE}">
       <text>
         <t>[线程批注]
 你的Excel版本可读取此线程批注; 但如果在更新版本的Excel中打开文件，则对批注所作的任何改动都将被删除。了解详细信息: https://go.microsoft.com/fwlink/?linkid=870924
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="222">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -1422,9 +1422,6 @@
 nmf_test_conv=1000,
 nmf_tolerance=1e-08</t>
     </r>
-  </si>
-  <si>
-    <t>Realistic-HPC-2nd-trial</t>
   </si>
   <si>
     <t>m2
@@ -1606,7 +1603,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1725,11 +1722,17 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1738,27 +1741,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1770,7 +1764,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -2098,10 +2092,10 @@
   <threadedComment ref="H27" dT="2022-10-05T08:49:51.16" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{4DB6E460-A4FE-40A6-B672-BB0B18A4A4A8}">
     <text>Needs re-download</text>
   </threadedComment>
-  <threadedComment ref="J40" dT="2022-10-04T01:45:33.47" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{7879683C-1E68-4F58-975B-EB0BED2C30CE}">
+  <threadedComment ref="H40" dT="2022-10-04T01:45:33.47" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{7879683C-1E68-4F58-975B-EB0BED2C30CE}">
     <text>Have different results compared to Realistic_wrong_time, despite using the same signeR and NMF version.</text>
   </threadedComment>
-  <threadedComment ref="J40" dT="2022-10-05T08:49:27.78" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{D645002E-BC3C-43B1-B316-C7F4E418B207}" parentId="{7879683C-1E68-4F58-975B-EB0BED2C30CE}">
+  <threadedComment ref="H40" dT="2022-10-05T08:49:27.78" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{D645002E-BC3C-43B1-B316-C7F4E418B207}" parentId="{7879683C-1E68-4F58-975B-EB0BED2C30CE}">
     <text>Needs to download signeR.Rdata file</text>
   </threadedComment>
 </ThreadedComments>
@@ -2270,10 +2264,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
@@ -2315,40 +2309,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="50.1" customHeight="1">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="M1" s="50" t="s">
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="M1" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
       <c r="F2" s="9">
         <v>5</v>
       </c>
@@ -2387,13 +2381,13 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="68.25" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="40" t="s">
         <v>71</v>
       </c>
       <c r="D3" s="10">
@@ -2415,121 +2409,121 @@
       <c r="J3" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="K3" s="46" t="s">
+      <c r="K3" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="M3" s="46" t="s">
+      <c r="M3" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="N3" s="46" t="s">
+      <c r="N3" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="O3" s="46" t="s">
+      <c r="O3" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="P3" s="46" t="s">
+      <c r="P3" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="Q3" s="46" t="s">
+      <c r="Q3" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="R3" s="46" t="s">
+      <c r="R3" s="43" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="75" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="41"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="10">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="H4" s="46" t="s">
+      <c r="H4" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="I4" s="46" t="s">
+      <c r="I4" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="J4" s="46" t="s">
+      <c r="J4" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="K4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="46"/>
+      <c r="K4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
     </row>
     <row r="5" spans="1:18" ht="36" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="41"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="10">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
     </row>
     <row r="6" spans="1:18" ht="36" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="41"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="10">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
     </row>
     <row r="7" spans="1:18" ht="36" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="54"/>
-      <c r="C7" s="41"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="10">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="M7" s="46"/>
-      <c r="N7" s="46"/>
-      <c r="O7" s="46"/>
-      <c r="P7" s="46"/>
-      <c r="Q7" s="46"/>
-      <c r="R7" s="46"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="43"/>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="2"/>
@@ -2540,139 +2534,139 @@
       <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:18" ht="54" customHeight="1">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="48" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="10">
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="46" t="s">
+      <c r="F9" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="G9" s="46" t="s">
+      <c r="G9" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="H9" s="46" t="s">
+      <c r="H9" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="I9" s="46" t="s">
+      <c r="I9" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="J9" s="46" t="s">
+      <c r="J9" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="K9" s="46" t="s">
+      <c r="K9" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="M9" s="46" t="s">
+      <c r="M9" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="N9" s="46" t="s">
+      <c r="N9" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="O9" s="46" t="s">
+      <c r="O9" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="P9" s="46" t="s">
+      <c r="P9" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="Q9" s="46" t="s">
+      <c r="Q9" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="R9" s="46" t="s">
+      <c r="R9" s="43" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="54" customHeight="1">
-      <c r="A10" s="43"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="44"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="48"/>
       <c r="D10" s="10">
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="46"/>
-      <c r="Q10" s="46"/>
-      <c r="R10" s="46"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
     </row>
     <row r="11" spans="1:18" ht="54" customHeight="1">
-      <c r="A11" s="43"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="44"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="48"/>
       <c r="D11" s="10">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
     </row>
     <row r="12" spans="1:18" ht="54" customHeight="1">
-      <c r="A12" s="43"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="44"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="10">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="M12" s="46"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="46"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
     </row>
     <row r="13" spans="1:18" ht="54" customHeight="1">
-      <c r="A13" s="43"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="44"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="10">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="M13" s="46"/>
-      <c r="N13" s="46"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="46"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="43"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="5"/>
@@ -2685,14 +2679,14 @@
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:18" ht="94.5" customHeight="1">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
@@ -2706,28 +2700,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="M3:M7"/>
-    <mergeCell ref="N3:N7"/>
-    <mergeCell ref="O3:O7"/>
-    <mergeCell ref="P3:P7"/>
-    <mergeCell ref="M9:M13"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="N9:N13"/>
-    <mergeCell ref="O9:O13"/>
-    <mergeCell ref="P9:P13"/>
-    <mergeCell ref="Q9:Q13"/>
-    <mergeCell ref="R9:R13"/>
-    <mergeCell ref="Q3:Q7"/>
-    <mergeCell ref="R3:R7"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="K9:K13"/>
     <mergeCell ref="J9:J13"/>
@@ -2743,6 +2715,28 @@
     <mergeCell ref="K3:K7"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="H4:H7"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="P3:P7"/>
+    <mergeCell ref="M9:M13"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="N9:N13"/>
+    <mergeCell ref="O9:O13"/>
+    <mergeCell ref="P9:P13"/>
+    <mergeCell ref="Q9:Q13"/>
+    <mergeCell ref="R9:R13"/>
+    <mergeCell ref="Q3:Q7"/>
+    <mergeCell ref="R3:R7"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="M3:M7"/>
+    <mergeCell ref="N3:N7"/>
+    <mergeCell ref="O3:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2771,32 +2765,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:15" ht="45">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
       <c r="F2" s="9" t="s">
         <v>38</v>
       </c>
@@ -2813,92 +2807,92 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="45" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="40" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:15" ht="45" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="41"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="45" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="41"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="45" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="41"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="46" t="s">
+      <c r="F6" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:15" ht="45" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="41"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="46" t="s">
+      <c r="F7" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
       <c r="K7" s="2"/>
@@ -2930,11 +2924,11 @@
         <v>34</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="46" t="s">
+      <c r="F9" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
       <c r="J9" s="4"/>
       <c r="K9" s="5"/>
     </row>
@@ -2950,13 +2944,13 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:15" ht="30" customHeight="1">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="45" t="s">
         <v>191</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="C11" s="44"/>
+      <c r="C11" s="48"/>
       <c r="D11" s="2">
         <v>145879</v>
       </c>
@@ -2968,15 +2962,15 @@
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:15" ht="30" customHeight="1">
-      <c r="A12" s="43"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="44"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="2">
         <v>200437</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="48" t="s">
-        <v>222</v>
+      <c r="F12" s="47" t="s">
+        <v>221</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="4"/>
@@ -2984,14 +2978,14 @@
       <c r="O12" s="33"/>
     </row>
     <row r="13" spans="1:15" ht="30" customHeight="1">
-      <c r="A13" s="43"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="44"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="2">
         <v>310111</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="48"/>
+      <c r="F13" s="47"/>
       <c r="G13" s="5"/>
       <c r="I13" s="2"/>
       <c r="J13" s="4"/>
@@ -2999,14 +2993,14 @@
       <c r="O13" s="33"/>
     </row>
     <row r="14" spans="1:15" ht="30" customHeight="1">
-      <c r="A14" s="43"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="44"/>
+      <c r="A14" s="45"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="48"/>
       <c r="D14" s="2">
         <v>528401</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="48"/>
+      <c r="F14" s="47"/>
       <c r="G14" s="5"/>
       <c r="I14" s="2"/>
       <c r="J14" s="4"/>
@@ -3014,14 +3008,14 @@
       <c r="O14" s="33"/>
     </row>
     <row r="15" spans="1:15" ht="30" customHeight="1">
-      <c r="A15" s="43"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="44"/>
+      <c r="A15" s="45"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="2">
         <v>1076753</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="48"/>
+      <c r="F15" s="47"/>
       <c r="G15" s="5"/>
       <c r="I15" s="2"/>
       <c r="J15" s="4"/>
@@ -3084,84 +3078,84 @@
       <c r="O18" s="33"/>
     </row>
     <row r="19" spans="1:15" ht="60" customHeight="1">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="C19" s="47" t="s">
+      <c r="C19" s="46" t="s">
         <v>56</v>
       </c>
       <c r="D19" s="2">
         <v>145879</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="46" t="s">
+      <c r="F19" s="43" t="s">
         <v>157</v>
       </c>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
       <c r="O19" s="33"/>
     </row>
     <row r="20" spans="1:15" ht="60" customHeight="1">
-      <c r="A20" s="43"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="47"/>
+      <c r="A20" s="45"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="46"/>
       <c r="D20" s="2">
         <v>200437</v>
       </c>
       <c r="E20" s="5"/>
-      <c r="F20" s="46" t="s">
+      <c r="F20" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
       <c r="O20" s="33"/>
     </row>
     <row r="21" spans="1:15" ht="60" customHeight="1">
-      <c r="A21" s="43"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="47"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="2">
         <v>310111</v>
       </c>
       <c r="E21" s="5"/>
-      <c r="F21" s="46" t="s">
+      <c r="F21" s="43" t="s">
         <v>159</v>
       </c>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
       <c r="O21" s="33"/>
     </row>
     <row r="22" spans="1:15" ht="60" customHeight="1">
-      <c r="A22" s="43"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="47"/>
+      <c r="A22" s="45"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="46"/>
       <c r="D22" s="2">
         <v>528401</v>
       </c>
       <c r="E22" s="5"/>
-      <c r="F22" s="46" t="s">
+      <c r="F22" s="43" t="s">
         <v>160</v>
       </c>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
       <c r="O22" s="33"/>
     </row>
     <row r="23" spans="1:15" ht="60" customHeight="1">
-      <c r="A23" s="43"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="47"/>
+      <c r="A23" s="45"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="46"/>
       <c r="D23" s="2">
         <v>1076753</v>
       </c>
       <c r="E23" s="5"/>
-      <c r="F23" s="46" t="s">
+      <c r="F23" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
       <c r="O23" s="33"/>
     </row>
     <row r="24" spans="1:15">
@@ -3181,7 +3175,7 @@
       <c r="A25" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="44" t="s">
         <v>173</v>
       </c>
       <c r="C25" s="18" t="s">
@@ -3202,7 +3196,7 @@
     </row>
     <row r="26" spans="1:15" ht="30" customHeight="1">
       <c r="A26" s="10"/>
-      <c r="B26" s="42"/>
+      <c r="B26" s="44"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -3212,11 +3206,11 @@
       <c r="K26" s="5"/>
     </row>
     <row r="27" spans="1:15" ht="60" customHeight="1">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="45" t="s">
+      <c r="B27" s="44"/>
+      <c r="C27" s="49" t="s">
         <v>64</v>
       </c>
       <c r="D27" s="2">
@@ -3226,16 +3220,16 @@
       <c r="H27" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="I27" s="46" t="s">
+      <c r="I27" s="43" t="s">
         <v>178</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:15" ht="60" customHeight="1">
-      <c r="A28" s="43"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="45"/>
+      <c r="A28" s="45"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="49"/>
       <c r="D28" s="2">
         <v>200437</v>
       </c>
@@ -3243,14 +3237,14 @@
       <c r="H28" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="I28" s="46"/>
+      <c r="I28" s="43"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:15" ht="60" customHeight="1">
-      <c r="A29" s="43"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="45"/>
+      <c r="A29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="49"/>
       <c r="D29" s="2">
         <v>310111</v>
       </c>
@@ -3258,14 +3252,14 @@
       <c r="H29" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="I29" s="46"/>
+      <c r="I29" s="43"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:15" ht="60" customHeight="1">
-      <c r="A30" s="43"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="45"/>
+      <c r="A30" s="45"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="49"/>
       <c r="D30" s="2">
         <v>528401</v>
       </c>
@@ -3273,14 +3267,14 @@
       <c r="H30" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="I30" s="46"/>
+      <c r="I30" s="43"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:15" ht="60" customHeight="1">
-      <c r="A31" s="43"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="45"/>
+      <c r="A31" s="45"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="49"/>
       <c r="D31" s="2">
         <v>1076753</v>
       </c>
@@ -3288,7 +3282,7 @@
       <c r="H31" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="I31" s="46"/>
+      <c r="I31" s="43"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
@@ -3306,14 +3300,14 @@
       <c r="K32" s="5"/>
     </row>
     <row r="33" spans="1:11" ht="75" customHeight="1">
-      <c r="A33" s="41" t="s">
+      <c r="A33" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -3332,6 +3326,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F12:F15"/>
     <mergeCell ref="A33:F33"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="A1:A2"/>
@@ -3348,21 +3357,6 @@
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="A19:A23"/>
     <mergeCell ref="B19:B23"/>
-    <mergeCell ref="I27:I31"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="B25:B31"/>
-    <mergeCell ref="A27:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3393,24 +3387,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="46.5" customHeight="1">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="42" t="s">
         <v>20</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -3419,10 +3413,10 @@
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14" ht="30.75" customHeight="1">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="1"/>
       <c r="F2" s="9" t="s">
         <v>39</v>
@@ -3624,7 +3618,7 @@
       <c r="A13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="44" t="s">
         <v>173</v>
       </c>
       <c r="C13" s="18" t="s">
@@ -3645,7 +3639,7 @@
     </row>
     <row r="14" spans="1:14" ht="45">
       <c r="A14" s="5"/>
-      <c r="B14" s="42"/>
+      <c r="B14" s="44"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -3664,18 +3658,18 @@
       <c r="N14" s="5"/>
     </row>
     <row r="15" spans="1:14" ht="54" customHeight="1">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="45" t="s">
+      <c r="B15" s="44"/>
+      <c r="C15" s="49" t="s">
         <v>65</v>
       </c>
       <c r="D15" s="5">
         <v>145879</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="46" t="s">
+      <c r="F15" s="43" t="s">
         <v>167</v>
       </c>
       <c r="H15" s="24" t="s">
@@ -3687,14 +3681,14 @@
       <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:14" ht="54" customHeight="1">
-      <c r="A16" s="43"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="45"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="49"/>
       <c r="D16" s="5">
         <v>200437</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="46"/>
+      <c r="F16" s="43"/>
       <c r="H16" s="24" t="s">
         <v>74</v>
       </c>
@@ -3704,14 +3698,14 @@
       <c r="N16" s="5"/>
     </row>
     <row r="17" spans="1:14" ht="54" customHeight="1">
-      <c r="A17" s="43"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="45"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="49"/>
       <c r="D17" s="5">
         <v>310111</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="46"/>
+      <c r="F17" s="43"/>
       <c r="H17" s="25" t="s">
         <v>79</v>
       </c>
@@ -3721,14 +3715,14 @@
       <c r="N17" s="5"/>
     </row>
     <row r="18" spans="1:14" ht="54" customHeight="1">
-      <c r="A18" s="43"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="45"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="49"/>
       <c r="D18" s="5">
         <v>528401</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="46"/>
+      <c r="F18" s="43"/>
       <c r="H18" s="25" t="s">
         <v>79</v>
       </c>
@@ -3738,14 +3732,14 @@
       <c r="N18" s="5"/>
     </row>
     <row r="19" spans="1:14" ht="54" customHeight="1">
-      <c r="A19" s="43"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="45"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="5">
         <v>1076753</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="46"/>
+      <c r="F19" s="43"/>
       <c r="H19" s="25" t="s">
         <v>79</v>
       </c>
@@ -3787,16 +3781,16 @@
       <c r="N21" s="5"/>
     </row>
     <row r="22" spans="1:14" ht="105" customHeight="1">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" t="s">
@@ -3810,16 +3804,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="F15:F19"/>
     <mergeCell ref="B13:B19"/>
     <mergeCell ref="C15:C19"/>
     <mergeCell ref="A15:A19"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3834,8 +3828,8 @@
   </sheetPr>
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33:H37"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3848,29 +3842,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:9" ht="30">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
       <c r="F2" s="9" t="s">
         <v>38</v>
       </c>
@@ -3885,91 +3879,91 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="45">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="48" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="54" t="s">
         <v>151</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="54"/>
       <c r="H3"/>
       <c r="I3" s="38" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="44"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="48"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="G4" s="51"/>
+      <c r="G4" s="54"/>
       <c r="H4"/>
       <c r="I4" s="38" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="44"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="54" t="s">
         <v>153</v>
       </c>
-      <c r="G5" s="51"/>
+      <c r="G5" s="54"/>
       <c r="H5"/>
       <c r="I5" s="38" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="45">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="44"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="51" t="s">
+      <c r="F6" s="54" t="s">
         <v>154</v>
       </c>
-      <c r="G6" s="51"/>
+      <c r="G6" s="54"/>
       <c r="H6"/>
       <c r="I6" s="38" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="44"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="51" t="s">
+      <c r="F7" s="54" t="s">
         <v>155</v>
       </c>
-      <c r="G7" s="51"/>
+      <c r="G7" s="54"/>
       <c r="H7"/>
       <c r="I7" s="38" t="s">
         <v>155</v>
@@ -3995,23 +3989,23 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="45">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="40" t="s">
         <v>71</v>
       </c>
       <c r="D9" s="2">
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="46" t="s">
+      <c r="F9" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="G9" s="46" t="s">
+      <c r="G9" s="43" t="s">
         <v>83</v>
       </c>
       <c r="H9" s="27" t="s">
@@ -4019,15 +4013,15 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="45">
-      <c r="A10" s="43"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="41"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="40"/>
       <c r="D10" s="2">
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="28" t="s">
         <v>205</v>
       </c>
@@ -4036,15 +4030,15 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="45">
-      <c r="A11" s="43"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="41"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="2">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
       <c r="H11" s="28" t="s">
         <v>206</v>
       </c>
@@ -4053,15 +4047,15 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="45">
-      <c r="A12" s="43"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="41"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="2">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
       <c r="H12" s="28" t="s">
         <v>207</v>
       </c>
@@ -4070,15 +4064,15 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="45">
-      <c r="A13" s="43"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="41"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
       <c r="H13" s="28" t="s">
         <v>208</v>
       </c>
@@ -4103,82 +4097,82 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="54" customHeight="1">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="48" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="2">
         <v>145879</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="46" t="s">
+      <c r="F15" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46" t="s">
+      <c r="G15" s="43"/>
+      <c r="H15" s="43" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="54" customHeight="1">
-      <c r="A16" s="43"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="44"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="2">
         <v>200437</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
     </row>
     <row r="17" spans="1:9" ht="54" customHeight="1">
-      <c r="A17" s="43"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="44"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="48"/>
       <c r="D17" s="2">
         <v>310111</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="46" t="s">
+      <c r="F17" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
     </row>
     <row r="18" spans="1:9" ht="54" customHeight="1">
-      <c r="A18" s="43"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="44"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="48"/>
       <c r="D18" s="2">
         <v>528401</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="46" t="s">
+      <c r="F18" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
     </row>
     <row r="19" spans="1:9" ht="54" customHeight="1">
-      <c r="A19" s="43"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="44"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="48"/>
       <c r="D19" s="2">
         <v>1076753</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="46" t="s">
+      <c r="F19" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
     </row>
     <row r="20" spans="1:9" ht="54" customHeight="1">
       <c r="A20" s="10"/>
@@ -4197,13 +4191,13 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="45" customHeight="1">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="44" t="s">
         <v>211</v>
       </c>
-      <c r="C21" s="44" t="s">
+      <c r="C21" s="48" t="s">
         <v>213</v>
       </c>
       <c r="D21" s="2"/>
@@ -4215,9 +4209,9 @@
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:9" ht="45" customHeight="1">
-      <c r="A22" s="43"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="44"/>
+      <c r="A22" s="45"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="48"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="28" t="s">
@@ -4227,21 +4221,21 @@
       <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:9" ht="45" customHeight="1">
-      <c r="A23" s="43"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="44"/>
+      <c r="A23" s="45"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="48"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:9" ht="45" customHeight="1">
-      <c r="A24" s="43"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="44"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="48"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="28" t="s">
@@ -4251,9 +4245,9 @@
       <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:9" ht="45" customHeight="1">
-      <c r="A25" s="43"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="44"/>
+      <c r="A25" s="45"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="48"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="28" t="s">
@@ -4273,13 +4267,13 @@
       <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:9" ht="60" customHeight="1">
-      <c r="A27" s="47" t="s">
+      <c r="A27" s="46" t="s">
         <v>191</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="C27" s="44" t="s">
+      <c r="C27" s="48" t="s">
         <v>218</v>
       </c>
       <c r="D27" s="2">
@@ -4292,9 +4286,9 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="60" customHeight="1">
-      <c r="A28" s="47"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="44"/>
+      <c r="A28" s="46"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="48"/>
       <c r="D28" s="2">
         <v>200437</v>
       </c>
@@ -4306,9 +4300,9 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="60" customHeight="1">
-      <c r="A29" s="47"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="44"/>
+      <c r="A29" s="46"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="48"/>
       <c r="D29" s="2">
         <v>310111</v>
       </c>
@@ -4320,9 +4314,9 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="60" customHeight="1">
-      <c r="A30" s="47"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="44"/>
+      <c r="A30" s="46"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="48"/>
       <c r="D30" s="2">
         <v>528401</v>
       </c>
@@ -4334,9 +4328,9 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="60" customHeight="1">
-      <c r="A31" s="47"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="44"/>
+      <c r="A31" s="46"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="48"/>
       <c r="D31" s="2">
         <v>1076753</v>
       </c>
@@ -4344,7 +4338,7 @@
       <c r="F31" s="20"/>
       <c r="G31" s="10"/>
       <c r="H31" s="28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="30">
@@ -4367,83 +4361,83 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="44" t="s">
+      <c r="B33" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="44" t="s">
+      <c r="C33" s="48" t="s">
         <v>61</v>
       </c>
       <c r="D33" s="5">
         <v>145879</v>
       </c>
       <c r="E33" s="2"/>
-      <c r="F33" s="46" t="s">
+      <c r="F33" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="G33" s="46" t="s">
+      <c r="G33" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="H33" s="55" t="s">
+      <c r="H33" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="I33" s="46" t="s">
+      <c r="I33" s="43" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30" customHeight="1">
-      <c r="A34" s="43"/>
-      <c r="B34" s="44"/>
-      <c r="C34" s="44"/>
+      <c r="A34" s="45"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
       <c r="D34" s="5">
         <v>200437</v>
       </c>
       <c r="E34" s="2"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="55"/>
-      <c r="I34" s="46"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="50"/>
+      <c r="I34" s="43"/>
     </row>
     <row r="35" spans="1:10" ht="30" customHeight="1">
-      <c r="A35" s="43"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
+      <c r="A35" s="45"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="48"/>
       <c r="D35" s="5">
         <v>310111</v>
       </c>
       <c r="E35" s="2"/>
-      <c r="F35" s="46"/>
-      <c r="G35" s="46"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="46"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="43"/>
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1">
-      <c r="A36" s="43"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
+      <c r="A36" s="45"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="48"/>
       <c r="D36" s="5">
         <v>528401</v>
       </c>
       <c r="E36" s="2"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="46"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="43"/>
     </row>
     <row r="37" spans="1:10" ht="45" customHeight="1">
-      <c r="A37" s="43"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
+      <c r="A37" s="45"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
       <c r="D37" s="5">
         <v>1076753</v>
       </c>
       <c r="E37" s="2"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="46"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="43"/>
       <c r="J37" s="8"/>
     </row>
     <row r="38" spans="1:10">
@@ -4471,23 +4465,20 @@
         <v>43</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="J39" s="8" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="60">
-      <c r="A40" s="47" t="s">
+    </row>
+    <row r="40" spans="1:10" ht="45">
+      <c r="A40" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="B40" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="C40" s="43" t="s">
+      <c r="C40" s="45" t="s">
         <v>54</v>
       </c>
       <c r="D40" s="5">
@@ -4496,66 +4487,66 @@
       <c r="E40" s="5"/>
       <c r="F40"/>
       <c r="G40"/>
+      <c r="H40" s="34" t="s">
+        <v>195</v>
+      </c>
       <c r="I40" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="J40" s="40" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="75">
-      <c r="A41" s="47"/>
-      <c r="B41" s="42"/>
-      <c r="C41" s="43"/>
+    </row>
+    <row r="41" spans="1:10" ht="45">
+      <c r="A41" s="46"/>
+      <c r="B41" s="44"/>
+      <c r="C41" s="45"/>
       <c r="D41" s="5">
         <v>200437</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41"/>
       <c r="G41"/>
+      <c r="H41" s="34" t="s">
+        <v>197</v>
+      </c>
       <c r="I41" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="J41" s="40" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="42" spans="1:10" ht="45" customHeight="1">
-      <c r="A42" s="47"/>
-      <c r="B42" s="42"/>
-      <c r="C42" s="43"/>
+      <c r="A42" s="46"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="45"/>
       <c r="D42" s="5">
         <v>310111</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42"/>
       <c r="G42"/>
-      <c r="I42" s="46" t="s">
+      <c r="H42" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="I42" s="43" t="s">
         <v>156</v>
       </c>
-      <c r="J42" s="40" t="s">
-        <v>200</v>
-      </c>
     </row>
     <row r="43" spans="1:10" ht="45" customHeight="1">
-      <c r="A43" s="47"/>
-      <c r="B43" s="42"/>
-      <c r="C43" s="43"/>
+      <c r="A43" s="46"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="45"/>
       <c r="D43" s="5">
         <v>528401</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43"/>
       <c r="G43"/>
-      <c r="I43" s="46"/>
-      <c r="J43" s="40" t="s">
+      <c r="H43" s="34" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="60">
-      <c r="A44" s="47"/>
-      <c r="B44" s="42"/>
-      <c r="C44" s="43"/>
+      <c r="I43" s="43"/>
+    </row>
+    <row r="44" spans="1:10" ht="45">
+      <c r="A44" s="46"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="45"/>
       <c r="D44" s="5">
         <v>1076753</v>
       </c>
@@ -4565,10 +4556,7 @@
       <c r="H44" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="I44" s="46"/>
-      <c r="J44" s="40" t="s">
-        <v>199</v>
-      </c>
+      <c r="I44" s="43"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="5"/>
@@ -4581,13 +4569,13 @@
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:10" ht="54" customHeight="1">
-      <c r="A46" s="47" t="s">
+      <c r="A46" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="B46" s="42" t="s">
+      <c r="B46" s="44" t="s">
         <v>173</v>
       </c>
-      <c r="C46" s="52" t="s">
+      <c r="C46" s="51" t="s">
         <v>63</v>
       </c>
       <c r="D46" s="5">
@@ -4601,9 +4589,9 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="54" customHeight="1">
-      <c r="A47" s="47"/>
-      <c r="B47" s="42"/>
-      <c r="C47" s="53"/>
+      <c r="A47" s="46"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="52"/>
       <c r="D47" s="5">
         <v>200437</v>
       </c>
@@ -4615,9 +4603,9 @@
       </c>
     </row>
     <row r="48" spans="1:10" ht="54" customHeight="1">
-      <c r="A48" s="47"/>
-      <c r="B48" s="42"/>
-      <c r="C48" s="53"/>
+      <c r="A48" s="46"/>
+      <c r="B48" s="44"/>
+      <c r="C48" s="52"/>
       <c r="D48" s="5">
         <v>310111</v>
       </c>
@@ -4629,9 +4617,9 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="54" customHeight="1">
-      <c r="A49" s="47"/>
-      <c r="B49" s="42"/>
-      <c r="C49" s="53"/>
+      <c r="A49" s="46"/>
+      <c r="B49" s="44"/>
+      <c r="C49" s="52"/>
       <c r="D49" s="5">
         <v>528401</v>
       </c>
@@ -4643,9 +4631,9 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="54" customHeight="1">
-      <c r="A50" s="47"/>
-      <c r="B50" s="42"/>
-      <c r="C50" s="53"/>
+      <c r="A50" s="46"/>
+      <c r="B50" s="44"/>
+      <c r="C50" s="52"/>
       <c r="D50" s="5">
         <v>1076753</v>
       </c>
@@ -4658,7 +4646,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="5"/>
-      <c r="B51" s="42"/>
+      <c r="B51" s="44"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
@@ -4670,7 +4658,7 @@
       <c r="A52" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B52" s="42"/>
+      <c r="B52" s="44"/>
       <c r="C52" s="19" t="s">
         <v>70</v>
       </c>
@@ -4705,14 +4693,14 @@
       <c r="H54" s="10"/>
     </row>
     <row r="55" spans="1:8" ht="94.5" customHeight="1">
-      <c r="A55" s="41" t="s">
+      <c r="A55" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B55" s="41"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="41"/>
-      <c r="E55" s="41"/>
-      <c r="F55" s="41"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
@@ -4731,19 +4719,25 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="I42:I44"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H15:H19"/>
-    <mergeCell ref="I33:I37"/>
-    <mergeCell ref="H33:H37"/>
-    <mergeCell ref="G33:G37"/>
-    <mergeCell ref="C33:C37"/>
-    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="B40:B44"/>
+    <mergeCell ref="C40:C44"/>
+    <mergeCell ref="F33:F37"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="F9:F13"/>
+    <mergeCell ref="G9:G13"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B33:B37"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -4760,25 +4754,19 @@
     <mergeCell ref="C15:C19"/>
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="A27:A31"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="F9:F13"/>
-    <mergeCell ref="G9:G13"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B33:B37"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="B40:B44"/>
-    <mergeCell ref="C40:C44"/>
-    <mergeCell ref="F33:F37"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="I42:I44"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H15:H19"/>
+    <mergeCell ref="I33:I37"/>
+    <mergeCell ref="H33:H37"/>
+    <mergeCell ref="G33:G37"/>
+    <mergeCell ref="C33:C37"/>
+    <mergeCell ref="A33:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4807,29 +4795,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="49.5" customHeight="1">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="42" t="s">
         <v>20</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="50"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="49"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="1"/>
       <c r="F2" s="9" t="s">
         <v>39</v>
@@ -4839,13 +4827,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="36" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="40" t="s">
         <v>51</v>
       </c>
       <c r="D3" s="2">
@@ -4857,9 +4845,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="36" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="41"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
@@ -4869,9 +4857,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="36" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="41"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
@@ -4881,9 +4869,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="36" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="41"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
@@ -4893,9 +4881,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="41"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
@@ -4911,40 +4899,40 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="45" customHeight="1">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="48" t="s">
         <v>46</v>
       </c>
       <c r="D9" s="2">
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="46" t="s">
+      <c r="F9" s="43" t="s">
         <v>175</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="45" customHeight="1">
-      <c r="A10" s="43"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="44"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="48"/>
       <c r="D10" s="2">
         <v>200437</v>
       </c>
-      <c r="F10" s="46"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="45" customHeight="1">
-      <c r="A11" s="43"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="44"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="48"/>
       <c r="D11" s="2">
         <v>310111</v>
       </c>
@@ -4956,28 +4944,28 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="45" customHeight="1">
-      <c r="A12" s="43"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="44"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="2">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="46" t="s">
+      <c r="F12" s="43" t="s">
         <v>186</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="45" customHeight="1">
-      <c r="A13" s="43"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="44"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="46"/>
+      <c r="F13" s="43"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:8">
@@ -4989,61 +4977,61 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="45" t="s">
         <v>191</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="C15" s="44"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="2">
         <v>145879</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="55" t="s">
+      <c r="F15" s="50" t="s">
         <v>194</v>
       </c>
       <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1">
-      <c r="A16" s="43"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="44"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="2">
         <v>200437</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="55"/>
+      <c r="F16" s="50"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="43"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="44"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="48"/>
       <c r="D17" s="2">
         <v>310111</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="55"/>
+      <c r="F17" s="50"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="43"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="44"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="48"/>
       <c r="D18" s="2">
         <v>528401</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="55"/>
+      <c r="F18" s="50"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="43"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="44"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="48"/>
       <c r="D19" s="2">
         <v>1076753</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="55"/>
+      <c r="F19" s="50"/>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2"/>
@@ -5110,13 +5098,13 @@
       <c r="N24" s="12"/>
     </row>
     <row r="25" spans="1:14" ht="54" customHeight="1">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="44" t="s">
         <v>173</v>
       </c>
-      <c r="C25" s="52" t="s">
+      <c r="C25" s="51" t="s">
         <v>92</v>
       </c>
       <c r="D25" s="5">
@@ -5129,9 +5117,9 @@
       <c r="N25" s="12"/>
     </row>
     <row r="26" spans="1:14" ht="54" customHeight="1">
-      <c r="A26" s="43"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="53"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="52"/>
       <c r="D26" s="5">
         <v>200437</v>
       </c>
@@ -5142,9 +5130,9 @@
       <c r="N26" s="12"/>
     </row>
     <row r="27" spans="1:14" ht="54" customHeight="1">
-      <c r="A27" s="43"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="53"/>
+      <c r="A27" s="45"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="52"/>
       <c r="D27" s="5">
         <v>310111</v>
       </c>
@@ -5155,9 +5143,9 @@
       <c r="N27" s="12"/>
     </row>
     <row r="28" spans="1:14" ht="54" customHeight="1">
-      <c r="A28" s="43"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="53"/>
+      <c r="A28" s="45"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="52"/>
       <c r="D28" s="5">
         <v>528401</v>
       </c>
@@ -5168,9 +5156,9 @@
       <c r="N28" s="12"/>
     </row>
     <row r="29" spans="1:14" ht="54" customHeight="1">
-      <c r="A29" s="43"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="53"/>
+      <c r="A29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="52"/>
       <c r="D29" s="5">
         <v>1076753</v>
       </c>
@@ -5182,18 +5170,18 @@
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="5"/>
-      <c r="B30" s="42"/>
+      <c r="B30" s="44"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="N30" s="12"/>
     </row>
     <row r="31" spans="1:14" ht="54" customHeight="1">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="42"/>
-      <c r="C31" s="52" t="s">
+      <c r="B31" s="44"/>
+      <c r="C31" s="51" t="s">
         <v>69</v>
       </c>
       <c r="D31" s="5">
@@ -5206,9 +5194,9 @@
       <c r="N31" s="12"/>
     </row>
     <row r="32" spans="1:14" ht="54" customHeight="1">
-      <c r="A32" s="43"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="53"/>
+      <c r="A32" s="45"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="52"/>
       <c r="D32" s="5">
         <v>200437</v>
       </c>
@@ -5219,9 +5207,9 @@
       <c r="N32" s="12"/>
     </row>
     <row r="33" spans="1:7" ht="54" customHeight="1">
-      <c r="A33" s="43"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="53"/>
+      <c r="A33" s="45"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="52"/>
       <c r="D33" s="5">
         <v>310111</v>
       </c>
@@ -5231,9 +5219,9 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="54" customHeight="1">
-      <c r="A34" s="43"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="53"/>
+      <c r="A34" s="45"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="52"/>
       <c r="D34" s="5">
         <v>528401</v>
       </c>
@@ -5243,9 +5231,9 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="54" customHeight="1">
-      <c r="A35" s="43"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="53"/>
+      <c r="A35" s="45"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="52"/>
       <c r="D35" s="5">
         <v>1076753</v>
       </c>
@@ -5264,15 +5252,15 @@
       <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:7" ht="99.95" customHeight="1">
-      <c r="A37" s="41" t="s">
+      <c r="A37" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
@@ -5286,6 +5274,16 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F15:F19"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="A3:A7"/>
@@ -5299,16 +5297,6 @@
     <mergeCell ref="C9:C13"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="A9:A13"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F15:F19"/>
-    <mergeCell ref="F9:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5344,12 +5332,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -5439,27 +5427,27 @@
       <c r="K4" s="2"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
     </row>
     <row r="7" spans="1:12" ht="90" customHeight="1">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -5519,12 +5507,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -5566,99 +5554,99 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="40" t="s">
         <v>49</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="43" t="s">
         <v>180</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="43" t="s">
         <v>180</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="43" t="s">
         <v>180</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="43" t="s">
         <v>180</v>
       </c>
-      <c r="I3" s="43" t="s">
+      <c r="I3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="56" t="s">
+      <c r="J3" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="45" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="41"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="45"/>
     </row>
     <row r="5" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="41"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="45"/>
     </row>
     <row r="6" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="41"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="45"/>
     </row>
     <row r="7" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="41"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="45"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="10"/>
@@ -5687,29 +5675,29 @@
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
     </row>
     <row r="11" spans="1:12" ht="99.95" customHeight="1">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -5778,13 +5766,13 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
@@ -5829,13 +5817,13 @@
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="45">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="52" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="10">
@@ -5864,11 +5852,11 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="45">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="C4" s="57"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="10">
         <v>200437</v>
       </c>
@@ -5892,9 +5880,9 @@
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="45">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="57"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="56"/>
       <c r="D5" s="10">
         <v>310111</v>
       </c>
@@ -5918,9 +5906,9 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:13" ht="45">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="57"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="10">
         <v>528401</v>
       </c>
@@ -5944,9 +5932,9 @@
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:13" ht="45">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="57"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="56"/>
       <c r="D7" s="10">
         <v>1076753</v>
       </c>
@@ -5974,15 +5962,15 @@
       <c r="L8" s="5"/>
     </row>
     <row r="9" spans="1:13" ht="90" customHeight="1">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -6022,7 +6010,7 @@
   </sheetPr>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -6044,12 +6032,12 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="10"/>
       <c r="J1" s="11"/>
       <c r="K1" s="10"/>
@@ -6090,13 +6078,13 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="45" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="40" t="s">
         <v>51</v>
       </c>
       <c r="D3" s="2">
@@ -6114,20 +6102,20 @@
       <c r="H3" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="I3" s="43" t="s">
+      <c r="I3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="56" t="s">
+      <c r="J3" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="45" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="45" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="41"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
@@ -6143,14 +6131,14 @@
       <c r="H4" s="27" t="s">
         <v>188</v>
       </c>
-      <c r="I4" s="43"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="43"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="45"/>
     </row>
     <row r="5" spans="1:11" ht="45" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="41"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
@@ -6166,14 +6154,14 @@
       <c r="H5" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="I5" s="43"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="43"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="45"/>
     </row>
     <row r="6" spans="1:11" ht="45" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="41"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
@@ -6189,14 +6177,14 @@
       <c r="H6" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="I6" s="43"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="43"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="45"/>
     </row>
     <row r="7" spans="1:11" ht="45" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="41"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
@@ -6212,9 +6200,9 @@
       <c r="H7" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="I7" s="43"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="43"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="45"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="10"/>
@@ -6230,29 +6218,29 @@
       <c r="K8" s="2"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
     </row>
     <row r="11" spans="1:11" ht="75" customHeight="1">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="12"/>
@@ -6294,12 +6282,12 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="5"/>

</xml_diff>